<commit_message>
Task 2 - Dodano "Multimedia"
</commit_message>
<xml_diff>
--- a/dane_aplikacji-zygol.xlsx
+++ b/dane_aplikacji-zygol.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="7575"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="7575" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Wykres1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="558">
   <si>
     <t>Id</t>
   </si>
@@ -1709,6 +1710,12 @@
   </si>
   <si>
     <t>3.2</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>50kk-100kk</t>
   </si>
 </sst>
 </file>
@@ -1859,7 +1866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1927,6 +1934,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1942,6 +1952,848 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AH$70:$AH$71</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AG$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AH$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="238939616"/>
+        <c:axId val="238940160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="238939616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="238940160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="238940160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="238939616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9302238" cy="6083710"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2233,8 +3085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3315,9 +4167,7 @@
       <c r="AB10" s="19">
         <v>1</v>
       </c>
-      <c r="AC10" s="19">
-        <v>1</v>
-      </c>
+      <c r="AC10" s="19"/>
       <c r="AD10" s="19"/>
       <c r="AE10" s="19"/>
       <c r="AF10" s="11"/>
@@ -3657,9 +4507,7 @@
       <c r="AB13" s="19">
         <v>1</v>
       </c>
-      <c r="AC13" s="19">
-        <v>1</v>
-      </c>
+      <c r="AC13" s="19"/>
       <c r="AD13" s="19"/>
       <c r="AE13" s="19">
         <v>1</v>
@@ -4751,9 +5599,7 @@
       <c r="AB23" s="19">
         <v>1</v>
       </c>
-      <c r="AC23" s="19">
-        <v>1</v>
-      </c>
+      <c r="AC23" s="19"/>
       <c r="AD23" s="19"/>
       <c r="AE23" s="19"/>
       <c r="AF23" s="11"/>
@@ -6659,9 +7505,7 @@
       <c r="AB47" s="9">
         <v>1</v>
       </c>
-      <c r="AC47" s="9">
-        <v>1</v>
-      </c>
+      <c r="AC47" s="9"/>
       <c r="AD47" s="9"/>
       <c r="AE47" s="9"/>
       <c r="AF47" s="11"/>
@@ -8521,9 +9365,7 @@
       <c r="AB64" s="9">
         <v>1</v>
       </c>
-      <c r="AC64" s="9">
-        <v>1</v>
-      </c>
+      <c r="AC64" s="9"/>
       <c r="AD64" s="9"/>
       <c r="AE64" s="9"/>
       <c r="AF64" s="11"/>
@@ -8639,9 +9481,7 @@
       <c r="AB65" s="9">
         <v>1</v>
       </c>
-      <c r="AC65" s="9">
-        <v>1</v>
-      </c>
+      <c r="AC65" s="9"/>
       <c r="AD65" s="9">
         <v>1</v>
       </c>
@@ -8838,16 +9678,30 @@
       <c r="D67" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="I67" s="9"/>
+      <c r="E67" s="4">
+        <v>983980</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I67" s="9">
+        <v>1</v>
+      </c>
       <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
+      <c r="K67" s="9">
+        <v>1</v>
+      </c>
+      <c r="L67" s="9">
+        <v>1</v>
+      </c>
       <c r="M67" s="11"/>
       <c r="N67" s="9"/>
-      <c r="O67" s="9"/>
+      <c r="O67" s="9">
+        <v>1</v>
+      </c>
       <c r="P67" s="9"/>
       <c r="Q67" s="9"/>
       <c r="R67" s="9"/>
@@ -8856,19 +9710,31 @@
       <c r="U67" s="9"/>
       <c r="V67" s="9"/>
       <c r="W67" s="9"/>
-      <c r="X67" s="9"/>
+      <c r="X67" s="9">
+        <v>1</v>
+      </c>
       <c r="Y67" s="11"/>
-      <c r="Z67" s="9"/>
+      <c r="Z67" s="9">
+        <v>1</v>
+      </c>
       <c r="AA67" s="9"/>
       <c r="AB67" s="9"/>
       <c r="AC67" s="9"/>
-      <c r="AD67" s="9"/>
-      <c r="AE67" s="9"/>
+      <c r="AD67" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE67" s="9">
+        <v>1</v>
+      </c>
       <c r="AF67" s="11"/>
-      <c r="AG67" s="9"/>
+      <c r="AG67" s="9">
+        <v>1</v>
+      </c>
       <c r="AH67" s="9"/>
       <c r="AI67" s="11"/>
-      <c r="AJ67" s="9"/>
+      <c r="AJ67" s="9">
+        <v>1</v>
+      </c>
       <c r="AK67" s="9"/>
       <c r="AL67" s="9"/>
       <c r="AM67" s="9"/>
@@ -8881,21 +9747,33 @@
       <c r="AT67" s="9"/>
       <c r="AU67" s="9"/>
       <c r="AV67" s="9"/>
-      <c r="AW67" s="9"/>
+      <c r="AW67" s="9">
+        <v>1</v>
+      </c>
       <c r="AX67" s="11"/>
       <c r="AY67" s="9"/>
-      <c r="AZ67" s="9"/>
+      <c r="AZ67" s="9">
+        <v>1</v>
+      </c>
       <c r="BA67" s="11"/>
       <c r="BB67" s="9"/>
-      <c r="BC67" s="9"/>
+      <c r="BC67" s="9">
+        <v>1</v>
+      </c>
       <c r="BD67" s="11"/>
-      <c r="BE67" s="9"/>
+      <c r="BE67" s="9">
+        <v>1</v>
+      </c>
       <c r="BF67" s="9"/>
       <c r="BG67" s="11"/>
-      <c r="BH67" s="9"/>
+      <c r="BH67" s="9">
+        <v>1</v>
+      </c>
       <c r="BI67" s="9"/>
       <c r="BJ67" s="11"/>
-      <c r="BK67" s="9"/>
+      <c r="BK67" s="9">
+        <v>1</v>
+      </c>
       <c r="BL67" s="9"/>
       <c r="BM67" s="11"/>
       <c r="BN67" s="9"/>
@@ -8914,27 +9792,43 @@
       <c r="D68" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="I68" s="9"/>
+      <c r="E68" s="4">
+        <v>65801</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="I68" s="9">
+        <v>1</v>
+      </c>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
-      <c r="L68" s="9"/>
+      <c r="L68" s="9">
+        <v>1</v>
+      </c>
       <c r="M68" s="11"/>
-      <c r="N68" s="9"/>
+      <c r="N68" s="9">
+        <v>1</v>
+      </c>
       <c r="O68" s="9"/>
       <c r="P68" s="9"/>
       <c r="Q68" s="9"/>
       <c r="R68" s="9"/>
       <c r="S68" s="9"/>
       <c r="T68" s="11"/>
-      <c r="U68" s="9"/>
+      <c r="U68" s="9">
+        <v>1</v>
+      </c>
       <c r="V68" s="9"/>
       <c r="W68" s="9"/>
       <c r="X68" s="9"/>
       <c r="Y68" s="11"/>
-      <c r="Z68" s="9"/>
+      <c r="Z68" s="9">
+        <v>1</v>
+      </c>
       <c r="AA68" s="9"/>
       <c r="AB68" s="9"/>
       <c r="AC68" s="9"/>
@@ -8956,22 +9850,34 @@
       <c r="AS68" s="9"/>
       <c r="AT68" s="9"/>
       <c r="AU68" s="9"/>
-      <c r="AV68" s="9"/>
+      <c r="AV68" s="9">
+        <v>1</v>
+      </c>
       <c r="AW68" s="9"/>
       <c r="AX68" s="11"/>
-      <c r="AY68" s="9"/>
+      <c r="AY68" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ68" s="9"/>
       <c r="BA68" s="11"/>
-      <c r="BB68" s="9"/>
+      <c r="BB68" s="9">
+        <v>1</v>
+      </c>
       <c r="BC68" s="9"/>
       <c r="BD68" s="11"/>
-      <c r="BE68" s="9"/>
+      <c r="BE68" s="9">
+        <v>1</v>
+      </c>
       <c r="BF68" s="9"/>
       <c r="BG68" s="11"/>
-      <c r="BH68" s="9"/>
+      <c r="BH68" s="9">
+        <v>1</v>
+      </c>
       <c r="BI68" s="9"/>
       <c r="BJ68" s="11"/>
-      <c r="BK68" s="9"/>
+      <c r="BK68" s="9">
+        <v>1</v>
+      </c>
       <c r="BL68" s="9"/>
       <c r="BM68" s="11"/>
       <c r="BN68" s="9"/>
@@ -8980,19 +9886,19 @@
       <c r="BQ68" s="9"/>
     </row>
     <row r="69" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4" t="s">
+      <c r="C69" s="26"/>
+      <c r="D69" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -9066,16 +9972,26 @@
       <c r="D70" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
+      <c r="E70" s="4">
+        <v>2530</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>543</v>
+      </c>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
-      <c r="L70" s="9"/>
+      <c r="L70" s="9">
+        <v>1</v>
+      </c>
       <c r="M70" s="11"/>
       <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
+      <c r="O70" s="9">
+        <v>1</v>
+      </c>
       <c r="P70" s="9"/>
       <c r="Q70" s="9"/>
       <c r="R70" s="9"/>
@@ -9084,24 +10000,34 @@
       <c r="U70" s="9"/>
       <c r="V70" s="9"/>
       <c r="W70" s="9"/>
-      <c r="X70" s="9"/>
+      <c r="X70" s="9">
+        <v>1</v>
+      </c>
       <c r="Y70" s="11"/>
       <c r="Z70" s="9"/>
-      <c r="AA70" s="9"/>
+      <c r="AA70" s="9">
+        <v>1</v>
+      </c>
       <c r="AB70" s="9"/>
       <c r="AC70" s="9"/>
       <c r="AD70" s="9"/>
       <c r="AE70" s="9"/>
       <c r="AF70" s="11"/>
       <c r="AG70" s="9"/>
-      <c r="AH70" s="9"/>
+      <c r="AH70" s="9">
+        <v>1</v>
+      </c>
       <c r="AI70" s="11"/>
       <c r="AJ70" s="9"/>
       <c r="AK70" s="9"/>
-      <c r="AL70" s="9"/>
+      <c r="AL70" s="9">
+        <v>1</v>
+      </c>
       <c r="AM70" s="9"/>
       <c r="AN70" s="11"/>
-      <c r="AO70" s="9"/>
+      <c r="AO70" s="9">
+        <v>1</v>
+      </c>
       <c r="AP70" s="9"/>
       <c r="AQ70" s="9"/>
       <c r="AR70" s="11"/>
@@ -9109,19 +10035,29 @@
       <c r="AT70" s="9"/>
       <c r="AU70" s="9"/>
       <c r="AV70" s="9"/>
-      <c r="AW70" s="9"/>
+      <c r="AW70" s="9">
+        <v>1</v>
+      </c>
       <c r="AX70" s="11"/>
       <c r="AY70" s="9"/>
-      <c r="AZ70" s="9"/>
+      <c r="AZ70" s="9">
+        <v>1</v>
+      </c>
       <c r="BA70" s="11"/>
-      <c r="BB70" s="9"/>
+      <c r="BB70" s="9">
+        <v>1</v>
+      </c>
       <c r="BC70" s="9"/>
       <c r="BD70" s="11"/>
       <c r="BE70" s="9"/>
-      <c r="BF70" s="9"/>
+      <c r="BF70" s="9">
+        <v>1</v>
+      </c>
       <c r="BG70" s="11"/>
       <c r="BH70" s="9"/>
-      <c r="BI70" s="9"/>
+      <c r="BI70" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ70" s="11"/>
       <c r="BK70" s="9"/>
       <c r="BL70" s="9"/>
@@ -9142,62 +10078,96 @@
       <c r="D71" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
+      <c r="E71" s="27">
+        <v>9029</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>543</v>
+      </c>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
-      <c r="L71" s="9"/>
+      <c r="L71" s="9">
+        <v>1</v>
+      </c>
       <c r="M71" s="11"/>
       <c r="N71" s="9"/>
-      <c r="O71" s="9"/>
+      <c r="O71" s="9">
+        <v>1</v>
+      </c>
       <c r="P71" s="9"/>
       <c r="Q71" s="9"/>
       <c r="R71" s="9"/>
       <c r="S71" s="9"/>
       <c r="T71" s="11"/>
-      <c r="U71" s="9"/>
+      <c r="U71" s="9">
+        <v>1</v>
+      </c>
       <c r="V71" s="9"/>
       <c r="W71" s="9"/>
       <c r="X71" s="9"/>
       <c r="Y71" s="11"/>
-      <c r="Z71" s="9"/>
-      <c r="AA71" s="9"/>
+      <c r="Z71" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA71" s="9">
+        <v>1</v>
+      </c>
       <c r="AB71" s="9"/>
       <c r="AC71" s="9"/>
       <c r="AD71" s="9"/>
       <c r="AE71" s="9"/>
       <c r="AF71" s="11"/>
       <c r="AG71" s="9"/>
-      <c r="AH71" s="9"/>
+      <c r="AH71" s="9">
+        <v>1</v>
+      </c>
       <c r="AI71" s="11"/>
       <c r="AJ71" s="9"/>
       <c r="AK71" s="9"/>
-      <c r="AL71" s="9"/>
-      <c r="AM71" s="9"/>
+      <c r="AL71" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM71" s="9">
+        <v>1</v>
+      </c>
       <c r="AN71" s="11"/>
       <c r="AO71" s="9"/>
       <c r="AP71" s="9"/>
-      <c r="AQ71" s="9"/>
+      <c r="AQ71" s="9">
+        <v>1</v>
+      </c>
       <c r="AR71" s="11"/>
       <c r="AS71" s="9"/>
       <c r="AT71" s="9"/>
       <c r="AU71" s="9"/>
       <c r="AV71" s="9"/>
-      <c r="AW71" s="9"/>
+      <c r="AW71" s="9">
+        <v>1</v>
+      </c>
       <c r="AX71" s="11"/>
-      <c r="AY71" s="9"/>
+      <c r="AY71" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ71" s="9"/>
       <c r="BA71" s="11"/>
-      <c r="BB71" s="9"/>
+      <c r="BB71" s="9">
+        <v>1</v>
+      </c>
       <c r="BC71" s="9"/>
       <c r="BD71" s="11"/>
       <c r="BE71" s="9"/>
-      <c r="BF71" s="9"/>
+      <c r="BF71" s="9">
+        <v>1</v>
+      </c>
       <c r="BG71" s="11"/>
       <c r="BH71" s="9"/>
-      <c r="BI71" s="9"/>
+      <c r="BI71" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ71" s="11"/>
       <c r="BK71" s="9"/>
       <c r="BL71" s="9"/>
@@ -9218,42 +10188,62 @@
       <c r="D72" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="I72" s="9"/>
+      <c r="E72" s="4">
+        <v>506</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="I72" s="9">
+        <v>1</v>
+      </c>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="11"/>
       <c r="N72" s="9"/>
-      <c r="O72" s="9"/>
+      <c r="O72" s="9">
+        <v>1</v>
+      </c>
       <c r="P72" s="9"/>
       <c r="Q72" s="9"/>
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
       <c r="T72" s="11"/>
-      <c r="U72" s="9"/>
+      <c r="U72" s="9">
+        <v>1</v>
+      </c>
       <c r="V72" s="9"/>
       <c r="W72" s="9"/>
       <c r="X72" s="9"/>
       <c r="Y72" s="11"/>
       <c r="Z72" s="9"/>
-      <c r="AA72" s="9"/>
+      <c r="AA72" s="9">
+        <v>1</v>
+      </c>
       <c r="AB72" s="9"/>
       <c r="AC72" s="9"/>
       <c r="AD72" s="9"/>
       <c r="AE72" s="9"/>
       <c r="AF72" s="11"/>
-      <c r="AG72" s="9"/>
+      <c r="AG72" s="9">
+        <v>1</v>
+      </c>
       <c r="AH72" s="9"/>
       <c r="AI72" s="11"/>
       <c r="AJ72" s="9"/>
-      <c r="AK72" s="9"/>
+      <c r="AK72" s="9">
+        <v>1</v>
+      </c>
       <c r="AL72" s="9"/>
       <c r="AM72" s="9"/>
       <c r="AN72" s="11"/>
-      <c r="AO72" s="9"/>
+      <c r="AO72" s="9">
+        <v>1</v>
+      </c>
       <c r="AP72" s="9"/>
       <c r="AQ72" s="9"/>
       <c r="AR72" s="11"/>
@@ -9261,18 +10251,28 @@
       <c r="AT72" s="9"/>
       <c r="AU72" s="9"/>
       <c r="AV72" s="9"/>
-      <c r="AW72" s="9"/>
+      <c r="AW72" s="9">
+        <v>1</v>
+      </c>
       <c r="AX72" s="11"/>
       <c r="AY72" s="9"/>
-      <c r="AZ72" s="9"/>
+      <c r="AZ72" s="9">
+        <v>1</v>
+      </c>
       <c r="BA72" s="11"/>
-      <c r="BB72" s="9"/>
+      <c r="BB72" s="9">
+        <v>1</v>
+      </c>
       <c r="BC72" s="9"/>
       <c r="BD72" s="11"/>
       <c r="BE72" s="9"/>
-      <c r="BF72" s="9"/>
+      <c r="BF72" s="9">
+        <v>1</v>
+      </c>
       <c r="BG72" s="11"/>
-      <c r="BH72" s="9"/>
+      <c r="BH72" s="9">
+        <v>1</v>
+      </c>
       <c r="BI72" s="9"/>
       <c r="BJ72" s="11"/>
       <c r="BK72" s="9"/>
@@ -9294,16 +10294,30 @@
       <c r="D73" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="9"/>
+      <c r="E73" s="4">
+        <v>7466</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I73" s="9">
+        <v>1</v>
+      </c>
+      <c r="J73" s="9">
+        <v>1</v>
+      </c>
       <c r="K73" s="9"/>
-      <c r="L73" s="9"/>
+      <c r="L73" s="9">
+        <v>1</v>
+      </c>
       <c r="M73" s="11"/>
       <c r="N73" s="9"/>
-      <c r="O73" s="9"/>
+      <c r="O73" s="9">
+        <v>1</v>
+      </c>
       <c r="P73" s="9"/>
       <c r="Q73" s="9"/>
       <c r="R73" s="9"/>
@@ -9312,19 +10326,29 @@
       <c r="U73" s="9"/>
       <c r="V73" s="9"/>
       <c r="W73" s="9"/>
-      <c r="X73" s="9"/>
+      <c r="X73" s="9">
+        <v>1</v>
+      </c>
       <c r="Y73" s="11"/>
-      <c r="Z73" s="9"/>
+      <c r="Z73" s="9">
+        <v>1</v>
+      </c>
       <c r="AA73" s="9"/>
-      <c r="AB73" s="9"/>
+      <c r="AB73" s="9">
+        <v>1</v>
+      </c>
       <c r="AC73" s="9"/>
       <c r="AD73" s="9"/>
       <c r="AE73" s="9"/>
       <c r="AF73" s="11"/>
-      <c r="AG73" s="9"/>
+      <c r="AG73" s="9">
+        <v>1</v>
+      </c>
       <c r="AH73" s="9"/>
       <c r="AI73" s="11"/>
-      <c r="AJ73" s="9"/>
+      <c r="AJ73" s="9">
+        <v>1</v>
+      </c>
       <c r="AK73" s="9"/>
       <c r="AL73" s="9"/>
       <c r="AM73" s="9"/>
@@ -9337,18 +10361,28 @@
       <c r="AT73" s="9"/>
       <c r="AU73" s="9"/>
       <c r="AV73" s="9"/>
-      <c r="AW73" s="9"/>
+      <c r="AW73" s="9">
+        <v>1</v>
+      </c>
       <c r="AX73" s="11"/>
       <c r="AY73" s="9"/>
-      <c r="AZ73" s="9"/>
+      <c r="AZ73" s="9">
+        <v>1</v>
+      </c>
       <c r="BA73" s="11"/>
-      <c r="BB73" s="9"/>
+      <c r="BB73" s="9">
+        <v>1</v>
+      </c>
       <c r="BC73" s="9"/>
       <c r="BD73" s="11"/>
       <c r="BE73" s="9"/>
-      <c r="BF73" s="9"/>
+      <c r="BF73" s="9">
+        <v>1</v>
+      </c>
       <c r="BG73" s="11"/>
-      <c r="BH73" s="9"/>
+      <c r="BH73" s="9">
+        <v>1</v>
+      </c>
       <c r="BI73" s="9"/>
       <c r="BJ73" s="11"/>
       <c r="BK73" s="9"/>
@@ -9370,16 +10404,28 @@
       <c r="D74" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="I74" s="9"/>
+      <c r="E74" s="4">
+        <v>35400</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="I74" s="9">
+        <v>1</v>
+      </c>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
-      <c r="L74" s="9"/>
+      <c r="L74" s="9">
+        <v>1</v>
+      </c>
       <c r="M74" s="11"/>
       <c r="N74" s="9"/>
-      <c r="O74" s="9"/>
+      <c r="O74" s="9">
+        <v>1</v>
+      </c>
       <c r="P74" s="9"/>
       <c r="Q74" s="9"/>
       <c r="R74" s="9"/>
@@ -9388,14 +10434,22 @@
       <c r="U74" s="9"/>
       <c r="V74" s="9"/>
       <c r="W74" s="9"/>
-      <c r="X74" s="9"/>
+      <c r="X74" s="9">
+        <v>1</v>
+      </c>
       <c r="Y74" s="11"/>
       <c r="Z74" s="9"/>
-      <c r="AA74" s="9"/>
+      <c r="AA74" s="9">
+        <v>1</v>
+      </c>
       <c r="AB74" s="9"/>
       <c r="AC74" s="9"/>
-      <c r="AD74" s="9"/>
-      <c r="AE74" s="9"/>
+      <c r="AD74" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE74" s="9">
+        <v>1</v>
+      </c>
       <c r="AF74" s="11"/>
       <c r="AG74" s="9"/>
       <c r="AH74" s="9"/>
@@ -9403,31 +10457,47 @@
       <c r="AJ74" s="9"/>
       <c r="AK74" s="9"/>
       <c r="AL74" s="9"/>
-      <c r="AM74" s="9"/>
+      <c r="AM74" s="9">
+        <v>1</v>
+      </c>
       <c r="AN74" s="11"/>
       <c r="AO74" s="9"/>
       <c r="AP74" s="9"/>
-      <c r="AQ74" s="9"/>
+      <c r="AQ74" s="9">
+        <v>1</v>
+      </c>
       <c r="AR74" s="11"/>
       <c r="AS74" s="9"/>
       <c r="AT74" s="9"/>
       <c r="AU74" s="9"/>
       <c r="AV74" s="9"/>
-      <c r="AW74" s="9"/>
+      <c r="AW74" s="9">
+        <v>1</v>
+      </c>
       <c r="AX74" s="11"/>
       <c r="AY74" s="9"/>
-      <c r="AZ74" s="9"/>
+      <c r="AZ74" s="9">
+        <v>1</v>
+      </c>
       <c r="BA74" s="11"/>
       <c r="BB74" s="9"/>
-      <c r="BC74" s="9"/>
+      <c r="BC74" s="9">
+        <v>1</v>
+      </c>
       <c r="BD74" s="11"/>
       <c r="BE74" s="9"/>
-      <c r="BF74" s="9"/>
+      <c r="BF74" s="9">
+        <v>1</v>
+      </c>
       <c r="BG74" s="11"/>
       <c r="BH74" s="9"/>
-      <c r="BI74" s="9"/>
+      <c r="BI74" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ74" s="11"/>
-      <c r="BK74" s="9"/>
+      <c r="BK74" s="9">
+        <v>1</v>
+      </c>
       <c r="BL74" s="9"/>
       <c r="BM74" s="11"/>
       <c r="BN74" s="9"/>
@@ -9446,42 +10516,68 @@
       <c r="D75" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="I75" s="9"/>
+      <c r="E75" s="4">
+        <v>15989</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="I75" s="9">
+        <v>1</v>
+      </c>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
+      <c r="L75" s="9">
+        <v>1</v>
+      </c>
       <c r="M75" s="11"/>
       <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
+      <c r="O75" s="9">
+        <v>1</v>
+      </c>
       <c r="P75" s="9"/>
       <c r="Q75" s="9"/>
       <c r="R75" s="9"/>
       <c r="S75" s="9"/>
       <c r="T75" s="11"/>
       <c r="U75" s="9"/>
-      <c r="V75" s="9"/>
+      <c r="V75" s="9">
+        <v>1</v>
+      </c>
       <c r="W75" s="9"/>
       <c r="X75" s="9"/>
       <c r="Y75" s="11"/>
       <c r="Z75" s="9"/>
-      <c r="AA75" s="9"/>
+      <c r="AA75" s="9">
+        <v>1</v>
+      </c>
       <c r="AB75" s="9"/>
       <c r="AC75" s="9"/>
-      <c r="AD75" s="9"/>
+      <c r="AD75" s="9">
+        <v>1</v>
+      </c>
       <c r="AE75" s="9"/>
       <c r="AF75" s="11"/>
       <c r="AG75" s="9"/>
-      <c r="AH75" s="9"/>
+      <c r="AH75" s="9">
+        <v>1</v>
+      </c>
       <c r="AI75" s="11"/>
       <c r="AJ75" s="9"/>
       <c r="AK75" s="9"/>
-      <c r="AL75" s="9"/>
-      <c r="AM75" s="9"/>
+      <c r="AL75" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM75" s="9">
+        <v>1</v>
+      </c>
       <c r="AN75" s="11"/>
-      <c r="AO75" s="9"/>
+      <c r="AO75" s="9">
+        <v>1</v>
+      </c>
       <c r="AP75" s="9"/>
       <c r="AQ75" s="9"/>
       <c r="AR75" s="11"/>
@@ -9489,24 +10585,38 @@
       <c r="AT75" s="9"/>
       <c r="AU75" s="9"/>
       <c r="AV75" s="9"/>
-      <c r="AW75" s="9"/>
+      <c r="AW75" s="9">
+        <v>1</v>
+      </c>
       <c r="AX75" s="11"/>
       <c r="AY75" s="9"/>
-      <c r="AZ75" s="9"/>
+      <c r="AZ75" s="9">
+        <v>1</v>
+      </c>
       <c r="BA75" s="11"/>
-      <c r="BB75" s="9"/>
+      <c r="BB75" s="9">
+        <v>1</v>
+      </c>
       <c r="BC75" s="9"/>
       <c r="BD75" s="11"/>
-      <c r="BE75" s="9"/>
+      <c r="BE75" s="9">
+        <v>1</v>
+      </c>
       <c r="BF75" s="9"/>
       <c r="BG75" s="11"/>
       <c r="BH75" s="9"/>
-      <c r="BI75" s="9"/>
+      <c r="BI75" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ75" s="11"/>
-      <c r="BK75" s="9"/>
+      <c r="BK75" s="9">
+        <v>1</v>
+      </c>
       <c r="BL75" s="9"/>
       <c r="BM75" s="11"/>
-      <c r="BN75" s="9"/>
+      <c r="BN75" s="9">
+        <v>1</v>
+      </c>
       <c r="BO75" s="9"/>
       <c r="BP75" s="9"/>
       <c r="BQ75" s="9"/>
@@ -9522,37 +10632,57 @@
       <c r="D76" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
+      <c r="E76" s="4">
+        <v>2025</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>536</v>
+      </c>
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
+      <c r="L76" s="9">
+        <v>1</v>
+      </c>
       <c r="M76" s="11"/>
-      <c r="N76" s="9"/>
+      <c r="N76" s="9">
+        <v>1</v>
+      </c>
       <c r="O76" s="9"/>
       <c r="P76" s="9"/>
       <c r="Q76" s="9"/>
       <c r="R76" s="9"/>
-      <c r="S76" s="9"/>
+      <c r="S76" s="9">
+        <v>1</v>
+      </c>
       <c r="T76" s="11"/>
       <c r="U76" s="9"/>
       <c r="V76" s="9"/>
       <c r="W76" s="9"/>
-      <c r="X76" s="9"/>
+      <c r="X76" s="9">
+        <v>1</v>
+      </c>
       <c r="Y76" s="11"/>
       <c r="Z76" s="9"/>
-      <c r="AA76" s="9"/>
+      <c r="AA76" s="9">
+        <v>1</v>
+      </c>
       <c r="AB76" s="9"/>
       <c r="AC76" s="9"/>
       <c r="AD76" s="9"/>
       <c r="AE76" s="9"/>
       <c r="AF76" s="11"/>
       <c r="AG76" s="9"/>
-      <c r="AH76" s="9"/>
+      <c r="AH76" s="9">
+        <v>1</v>
+      </c>
       <c r="AI76" s="11"/>
-      <c r="AJ76" s="9"/>
+      <c r="AJ76" s="9">
+        <v>1</v>
+      </c>
       <c r="AK76" s="9"/>
       <c r="AL76" s="9"/>
       <c r="AM76" s="9"/>
@@ -9562,24 +10692,36 @@
       <c r="AQ76" s="9"/>
       <c r="AR76" s="11"/>
       <c r="AS76" s="9"/>
-      <c r="AT76" s="9"/>
+      <c r="AT76" s="9">
+        <v>1</v>
+      </c>
       <c r="AU76" s="9"/>
       <c r="AV76" s="9"/>
       <c r="AW76" s="9"/>
       <c r="AX76" s="11"/>
       <c r="AY76" s="9"/>
-      <c r="AZ76" s="9"/>
+      <c r="AZ76" s="9">
+        <v>1</v>
+      </c>
       <c r="BA76" s="11"/>
-      <c r="BB76" s="9"/>
+      <c r="BB76" s="9">
+        <v>1</v>
+      </c>
       <c r="BC76" s="9"/>
       <c r="BD76" s="11"/>
-      <c r="BE76" s="9"/>
+      <c r="BE76" s="9">
+        <v>1</v>
+      </c>
       <c r="BF76" s="9"/>
       <c r="BG76" s="11"/>
-      <c r="BH76" s="9"/>
+      <c r="BH76" s="9">
+        <v>1</v>
+      </c>
       <c r="BI76" s="9"/>
       <c r="BJ76" s="11"/>
-      <c r="BK76" s="9"/>
+      <c r="BK76" s="9">
+        <v>1</v>
+      </c>
       <c r="BL76" s="9"/>
       <c r="BM76" s="11"/>
       <c r="BN76" s="9"/>
@@ -9598,37 +10740,59 @@
       <c r="D77" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
+      <c r="E77" s="4">
+        <v>25950</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
+      <c r="K77" s="9">
+        <v>1</v>
+      </c>
+      <c r="L77" s="9">
+        <v>1</v>
+      </c>
       <c r="M77" s="11"/>
       <c r="N77" s="9"/>
-      <c r="O77" s="9"/>
+      <c r="O77" s="9">
+        <v>1</v>
+      </c>
       <c r="P77" s="9"/>
       <c r="Q77" s="9"/>
       <c r="R77" s="9"/>
       <c r="S77" s="9"/>
       <c r="T77" s="11"/>
       <c r="U77" s="9"/>
-      <c r="V77" s="9"/>
+      <c r="V77" s="9">
+        <v>1</v>
+      </c>
       <c r="W77" s="9"/>
       <c r="X77" s="9"/>
       <c r="Y77" s="11"/>
       <c r="Z77" s="9"/>
-      <c r="AA77" s="9"/>
+      <c r="AA77" s="9">
+        <v>1</v>
+      </c>
       <c r="AB77" s="9"/>
       <c r="AC77" s="9"/>
-      <c r="AD77" s="9"/>
+      <c r="AD77" s="9">
+        <v>1</v>
+      </c>
       <c r="AE77" s="9"/>
       <c r="AF77" s="11"/>
-      <c r="AG77" s="9"/>
+      <c r="AG77" s="9">
+        <v>1</v>
+      </c>
       <c r="AH77" s="9"/>
       <c r="AI77" s="11"/>
-      <c r="AJ77" s="9"/>
+      <c r="AJ77" s="9">
+        <v>1</v>
+      </c>
       <c r="AK77" s="9"/>
       <c r="AL77" s="9"/>
       <c r="AM77" s="9"/>
@@ -9641,18 +10805,28 @@
       <c r="AT77" s="9"/>
       <c r="AU77" s="9"/>
       <c r="AV77" s="9"/>
-      <c r="AW77" s="9"/>
+      <c r="AW77" s="9">
+        <v>1</v>
+      </c>
       <c r="AX77" s="11"/>
       <c r="AY77" s="9"/>
-      <c r="AZ77" s="9"/>
+      <c r="AZ77" s="9">
+        <v>1</v>
+      </c>
       <c r="BA77" s="11"/>
-      <c r="BB77" s="9"/>
+      <c r="BB77" s="9">
+        <v>1</v>
+      </c>
       <c r="BC77" s="9"/>
       <c r="BD77" s="11"/>
-      <c r="BE77" s="9"/>
+      <c r="BE77" s="9">
+        <v>1</v>
+      </c>
       <c r="BF77" s="9"/>
       <c r="BG77" s="11"/>
-      <c r="BH77" s="9"/>
+      <c r="BH77" s="9">
+        <v>1</v>
+      </c>
       <c r="BI77" s="9"/>
       <c r="BJ77" s="11"/>
       <c r="BK77" s="9"/>
@@ -9674,16 +10848,26 @@
       <c r="D78" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
+      <c r="E78" s="4">
+        <v>778</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>535</v>
+      </c>
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
+      <c r="L78" s="9">
+        <v>1</v>
+      </c>
       <c r="M78" s="11"/>
       <c r="N78" s="9"/>
-      <c r="O78" s="9"/>
+      <c r="O78" s="9">
+        <v>1</v>
+      </c>
       <c r="P78" s="9"/>
       <c r="Q78" s="9"/>
       <c r="R78" s="9"/>
@@ -9692,19 +10876,31 @@
       <c r="U78" s="9"/>
       <c r="V78" s="9"/>
       <c r="W78" s="9"/>
-      <c r="X78" s="9"/>
+      <c r="X78" s="9">
+        <v>1</v>
+      </c>
       <c r="Y78" s="11"/>
-      <c r="Z78" s="9"/>
-      <c r="AA78" s="9"/>
+      <c r="Z78" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA78" s="9">
+        <v>1</v>
+      </c>
       <c r="AB78" s="9"/>
       <c r="AC78" s="9"/>
-      <c r="AD78" s="9"/>
+      <c r="AD78" s="9">
+        <v>1</v>
+      </c>
       <c r="AE78" s="9"/>
       <c r="AF78" s="11"/>
       <c r="AG78" s="9"/>
-      <c r="AH78" s="9"/>
+      <c r="AH78" s="9">
+        <v>1</v>
+      </c>
       <c r="AI78" s="11"/>
-      <c r="AJ78" s="9"/>
+      <c r="AJ78" s="9">
+        <v>1</v>
+      </c>
       <c r="AK78" s="9"/>
       <c r="AL78" s="9"/>
       <c r="AM78" s="9"/>
@@ -9717,18 +10913,28 @@
       <c r="AT78" s="9"/>
       <c r="AU78" s="9"/>
       <c r="AV78" s="9"/>
-      <c r="AW78" s="9"/>
+      <c r="AW78" s="9">
+        <v>1</v>
+      </c>
       <c r="AX78" s="11"/>
-      <c r="AY78" s="9"/>
+      <c r="AY78" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ78" s="9"/>
       <c r="BA78" s="11"/>
-      <c r="BB78" s="9"/>
+      <c r="BB78" s="9">
+        <v>1</v>
+      </c>
       <c r="BC78" s="9"/>
       <c r="BD78" s="11"/>
       <c r="BE78" s="9"/>
-      <c r="BF78" s="9"/>
+      <c r="BF78" s="9">
+        <v>1</v>
+      </c>
       <c r="BG78" s="11"/>
-      <c r="BH78" s="9"/>
+      <c r="BH78" s="9">
+        <v>1</v>
+      </c>
       <c r="BI78" s="9"/>
       <c r="BJ78" s="11"/>
       <c r="BK78" s="9"/>
@@ -9750,64 +10956,110 @@
       <c r="D79" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
+      <c r="E79" s="4">
+        <v>25093</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
-      <c r="L79" s="9"/>
+      <c r="L79" s="9">
+        <v>1</v>
+      </c>
       <c r="M79" s="11"/>
-      <c r="N79" s="9"/>
+      <c r="N79" s="9">
+        <v>1</v>
+      </c>
       <c r="O79" s="9"/>
-      <c r="P79" s="9"/>
-      <c r="Q79" s="9"/>
-      <c r="R79" s="9"/>
-      <c r="S79" s="9"/>
+      <c r="P79" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q79" s="9">
+        <v>1</v>
+      </c>
+      <c r="R79" s="9">
+        <v>1</v>
+      </c>
+      <c r="S79" s="9">
+        <v>1</v>
+      </c>
       <c r="T79" s="11"/>
       <c r="U79" s="9"/>
       <c r="V79" s="9"/>
       <c r="W79" s="9"/>
-      <c r="X79" s="9"/>
+      <c r="X79" s="9">
+        <v>1</v>
+      </c>
       <c r="Y79" s="11"/>
-      <c r="Z79" s="9"/>
-      <c r="AA79" s="9"/>
+      <c r="Z79" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA79" s="9">
+        <v>1</v>
+      </c>
       <c r="AB79" s="9"/>
       <c r="AC79" s="9"/>
-      <c r="AD79" s="9"/>
+      <c r="AD79" s="9">
+        <v>1</v>
+      </c>
       <c r="AE79" s="9"/>
       <c r="AF79" s="11"/>
       <c r="AG79" s="9"/>
-      <c r="AH79" s="9"/>
+      <c r="AH79" s="9">
+        <v>1</v>
+      </c>
       <c r="AI79" s="11"/>
       <c r="AJ79" s="9"/>
       <c r="AK79" s="9"/>
       <c r="AL79" s="9"/>
-      <c r="AM79" s="9"/>
+      <c r="AM79" s="9">
+        <v>1</v>
+      </c>
       <c r="AN79" s="11"/>
-      <c r="AO79" s="9"/>
+      <c r="AO79" s="9">
+        <v>1</v>
+      </c>
       <c r="AP79" s="9"/>
       <c r="AQ79" s="9"/>
       <c r="AR79" s="11"/>
       <c r="AS79" s="9"/>
       <c r="AT79" s="9"/>
-      <c r="AU79" s="9"/>
-      <c r="AV79" s="9"/>
+      <c r="AU79" s="9">
+        <v>1</v>
+      </c>
+      <c r="AV79" s="9">
+        <v>1</v>
+      </c>
       <c r="AW79" s="9"/>
       <c r="AX79" s="11"/>
       <c r="AY79" s="9"/>
-      <c r="AZ79" s="9"/>
+      <c r="AZ79" s="9">
+        <v>1</v>
+      </c>
       <c r="BA79" s="11"/>
-      <c r="BB79" s="9"/>
+      <c r="BB79" s="9">
+        <v>1</v>
+      </c>
       <c r="BC79" s="9"/>
       <c r="BD79" s="11"/>
       <c r="BE79" s="9"/>
-      <c r="BF79" s="9"/>
+      <c r="BF79" s="9">
+        <v>1</v>
+      </c>
       <c r="BG79" s="11"/>
-      <c r="BH79" s="9"/>
+      <c r="BH79" s="9">
+        <v>1</v>
+      </c>
       <c r="BI79" s="9"/>
       <c r="BJ79" s="11"/>
-      <c r="BK79" s="9"/>
+      <c r="BK79" s="9">
+        <v>1</v>
+      </c>
       <c r="BL79" s="9"/>
       <c r="BM79" s="11"/>
       <c r="BN79" s="9"/>
@@ -9826,16 +11078,26 @@
       <c r="D80" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
+      <c r="E80" s="4">
+        <v>6604</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>543</v>
+      </c>
       <c r="I80" s="9"/>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
-      <c r="L80" s="9"/>
+      <c r="L80" s="9">
+        <v>1</v>
+      </c>
       <c r="M80" s="11"/>
       <c r="N80" s="9"/>
-      <c r="O80" s="9"/>
+      <c r="O80" s="9">
+        <v>1</v>
+      </c>
       <c r="P80" s="9"/>
       <c r="Q80" s="9"/>
       <c r="R80" s="9"/>
@@ -9844,24 +11106,34 @@
       <c r="U80" s="9"/>
       <c r="V80" s="9"/>
       <c r="W80" s="9"/>
-      <c r="X80" s="9"/>
+      <c r="X80" s="9">
+        <v>1</v>
+      </c>
       <c r="Y80" s="11"/>
       <c r="Z80" s="9"/>
-      <c r="AA80" s="9"/>
+      <c r="AA80" s="9">
+        <v>1</v>
+      </c>
       <c r="AB80" s="9"/>
       <c r="AC80" s="9"/>
       <c r="AD80" s="9"/>
       <c r="AE80" s="9"/>
       <c r="AF80" s="11"/>
-      <c r="AG80" s="9"/>
+      <c r="AG80" s="9">
+        <v>1</v>
+      </c>
       <c r="AH80" s="9"/>
       <c r="AI80" s="11"/>
       <c r="AJ80" s="9"/>
       <c r="AK80" s="9"/>
-      <c r="AL80" s="9"/>
+      <c r="AL80" s="9">
+        <v>1</v>
+      </c>
       <c r="AM80" s="9"/>
       <c r="AN80" s="11"/>
-      <c r="AO80" s="9"/>
+      <c r="AO80" s="9">
+        <v>1</v>
+      </c>
       <c r="AP80" s="9"/>
       <c r="AQ80" s="9"/>
       <c r="AR80" s="11"/>
@@ -9869,18 +11141,28 @@
       <c r="AT80" s="9"/>
       <c r="AU80" s="9"/>
       <c r="AV80" s="9"/>
-      <c r="AW80" s="9"/>
+      <c r="AW80" s="9">
+        <v>1</v>
+      </c>
       <c r="AX80" s="11"/>
       <c r="AY80" s="9"/>
-      <c r="AZ80" s="9"/>
+      <c r="AZ80" s="9">
+        <v>1</v>
+      </c>
       <c r="BA80" s="11"/>
-      <c r="BB80" s="9"/>
+      <c r="BB80" s="9">
+        <v>1</v>
+      </c>
       <c r="BC80" s="9"/>
       <c r="BD80" s="11"/>
       <c r="BE80" s="9"/>
-      <c r="BF80" s="9"/>
+      <c r="BF80" s="9">
+        <v>1</v>
+      </c>
       <c r="BG80" s="11"/>
-      <c r="BH80" s="9"/>
+      <c r="BH80" s="9">
+        <v>1</v>
+      </c>
       <c r="BI80" s="9"/>
       <c r="BJ80" s="11"/>
       <c r="BK80" s="9"/>
@@ -9892,19 +11174,19 @@
       <c r="BQ80" s="9"/>
     </row>
     <row r="81" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4" t="s">
+      <c r="C81" s="26"/>
+      <c r="D81" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
@@ -9978,37 +11260,61 @@
       <c r="D82" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
+      <c r="E82" s="4">
+        <v>1040551</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>557</v>
+      </c>
       <c r="I82" s="9"/>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
-      <c r="L82" s="9"/>
+      <c r="L82" s="9">
+        <v>1</v>
+      </c>
       <c r="M82" s="11"/>
-      <c r="N82" s="9"/>
+      <c r="N82" s="9">
+        <v>1</v>
+      </c>
       <c r="O82" s="9"/>
-      <c r="P82" s="9"/>
-      <c r="Q82" s="9"/>
+      <c r="P82" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="9">
+        <v>1</v>
+      </c>
       <c r="R82" s="9"/>
       <c r="S82" s="9"/>
       <c r="T82" s="11"/>
       <c r="U82" s="9"/>
       <c r="V82" s="9"/>
       <c r="W82" s="9"/>
-      <c r="X82" s="9"/>
+      <c r="X82" s="9">
+        <v>1</v>
+      </c>
       <c r="Y82" s="11"/>
-      <c r="Z82" s="9"/>
-      <c r="AA82" s="9"/>
+      <c r="Z82" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA82" s="9">
+        <v>1</v>
+      </c>
       <c r="AB82" s="9"/>
       <c r="AC82" s="9"/>
       <c r="AD82" s="9"/>
       <c r="AE82" s="9"/>
       <c r="AF82" s="11"/>
       <c r="AG82" s="9"/>
-      <c r="AH82" s="9"/>
+      <c r="AH82" s="9">
+        <v>1</v>
+      </c>
       <c r="AI82" s="11"/>
-      <c r="AJ82" s="9"/>
+      <c r="AJ82" s="9">
+        <v>1</v>
+      </c>
       <c r="AK82" s="9"/>
       <c r="AL82" s="9"/>
       <c r="AM82" s="9"/>
@@ -10017,25 +11323,39 @@
       <c r="AP82" s="9"/>
       <c r="AQ82" s="9"/>
       <c r="AR82" s="11"/>
-      <c r="AS82" s="9"/>
+      <c r="AS82" s="9">
+        <v>1</v>
+      </c>
       <c r="AT82" s="9"/>
       <c r="AU82" s="9"/>
-      <c r="AV82" s="9"/>
+      <c r="AV82" s="9">
+        <v>1</v>
+      </c>
       <c r="AW82" s="9"/>
       <c r="AX82" s="11"/>
       <c r="AY82" s="9"/>
-      <c r="AZ82" s="9"/>
+      <c r="AZ82" s="9">
+        <v>1</v>
+      </c>
       <c r="BA82" s="11"/>
-      <c r="BB82" s="9"/>
+      <c r="BB82" s="9">
+        <v>1</v>
+      </c>
       <c r="BC82" s="9"/>
       <c r="BD82" s="11"/>
-      <c r="BE82" s="9"/>
+      <c r="BE82" s="9">
+        <v>1</v>
+      </c>
       <c r="BF82" s="9"/>
       <c r="BG82" s="11"/>
-      <c r="BH82" s="9"/>
+      <c r="BH82" s="9">
+        <v>1</v>
+      </c>
       <c r="BI82" s="9"/>
       <c r="BJ82" s="11"/>
-      <c r="BK82" s="9"/>
+      <c r="BK82" s="9">
+        <v>1</v>
+      </c>
       <c r="BL82" s="9"/>
       <c r="BM82" s="11"/>
       <c r="BN82" s="9"/>
@@ -10054,61 +11374,97 @@
       <c r="D83" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
+      <c r="E83" s="4">
+        <v>4555</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>543</v>
+      </c>
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
-      <c r="L83" s="9"/>
+      <c r="L83" s="9">
+        <v>1</v>
+      </c>
       <c r="M83" s="11"/>
       <c r="N83" s="9"/>
-      <c r="O83" s="9"/>
+      <c r="O83" s="9">
+        <v>1</v>
+      </c>
       <c r="P83" s="9"/>
       <c r="Q83" s="9"/>
       <c r="R83" s="9"/>
       <c r="S83" s="9"/>
       <c r="T83" s="11"/>
-      <c r="U83" s="9"/>
-      <c r="V83" s="9"/>
+      <c r="U83" s="9">
+        <v>1</v>
+      </c>
+      <c r="V83" s="9">
+        <v>1</v>
+      </c>
       <c r="W83" s="9"/>
       <c r="X83" s="9"/>
       <c r="Y83" s="11"/>
       <c r="Z83" s="9"/>
-      <c r="AA83" s="9"/>
+      <c r="AA83" s="9">
+        <v>1</v>
+      </c>
       <c r="AB83" s="9"/>
       <c r="AC83" s="9"/>
       <c r="AD83" s="9"/>
       <c r="AE83" s="9"/>
       <c r="AF83" s="11"/>
       <c r="AG83" s="9"/>
-      <c r="AH83" s="9"/>
+      <c r="AH83" s="9">
+        <v>1</v>
+      </c>
       <c r="AI83" s="11"/>
       <c r="AJ83" s="9"/>
       <c r="AK83" s="9"/>
-      <c r="AL83" s="9"/>
-      <c r="AM83" s="9"/>
+      <c r="AL83" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM83" s="9">
+        <v>1</v>
+      </c>
       <c r="AN83" s="11"/>
       <c r="AO83" s="9"/>
-      <c r="AP83" s="9"/>
-      <c r="AQ83" s="9"/>
+      <c r="AP83" s="9">
+        <v>1</v>
+      </c>
+      <c r="AQ83" s="9">
+        <v>1</v>
+      </c>
       <c r="AR83" s="11"/>
       <c r="AS83" s="9"/>
       <c r="AT83" s="9"/>
       <c r="AU83" s="9"/>
       <c r="AV83" s="9"/>
-      <c r="AW83" s="9"/>
+      <c r="AW83" s="9">
+        <v>1</v>
+      </c>
       <c r="AX83" s="11"/>
-      <c r="AY83" s="9"/>
+      <c r="AY83" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ83" s="9"/>
       <c r="BA83" s="11"/>
-      <c r="BB83" s="9"/>
+      <c r="BB83" s="9">
+        <v>1</v>
+      </c>
       <c r="BC83" s="9"/>
       <c r="BD83" s="11"/>
       <c r="BE83" s="9"/>
-      <c r="BF83" s="9"/>
+      <c r="BF83" s="9">
+        <v>1</v>
+      </c>
       <c r="BG83" s="11"/>
-      <c r="BH83" s="9"/>
+      <c r="BH83" s="9">
+        <v>1</v>
+      </c>
       <c r="BI83" s="9"/>
       <c r="BJ83" s="11"/>
       <c r="BK83" s="9"/>
@@ -10130,16 +11486,28 @@
       <c r="D84" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="I84" s="9"/>
+      <c r="E84" s="4">
+        <v>271498</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I84" s="9">
+        <v>1</v>
+      </c>
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
+      <c r="L84" s="9">
+        <v>1</v>
+      </c>
       <c r="M84" s="11"/>
       <c r="N84" s="9"/>
-      <c r="O84" s="9"/>
+      <c r="O84" s="9">
+        <v>1</v>
+      </c>
       <c r="P84" s="9"/>
       <c r="Q84" s="9"/>
       <c r="R84" s="9"/>
@@ -10147,44 +11515,66 @@
       <c r="T84" s="11"/>
       <c r="U84" s="9"/>
       <c r="V84" s="9"/>
-      <c r="W84" s="9"/>
+      <c r="W84" s="9">
+        <v>1</v>
+      </c>
       <c r="X84" s="9"/>
       <c r="Y84" s="11"/>
       <c r="Z84" s="9"/>
-      <c r="AA84" s="9"/>
+      <c r="AA84" s="9">
+        <v>1</v>
+      </c>
       <c r="AB84" s="9"/>
       <c r="AC84" s="9"/>
-      <c r="AD84" s="9"/>
+      <c r="AD84" s="9">
+        <v>1</v>
+      </c>
       <c r="AE84" s="9"/>
       <c r="AF84" s="11"/>
       <c r="AG84" s="9"/>
-      <c r="AH84" s="9"/>
+      <c r="AH84" s="9">
+        <v>1</v>
+      </c>
       <c r="AI84" s="11"/>
       <c r="AJ84" s="9"/>
       <c r="AK84" s="9"/>
-      <c r="AL84" s="9"/>
+      <c r="AL84" s="9">
+        <v>1</v>
+      </c>
       <c r="AM84" s="9"/>
       <c r="AN84" s="11"/>
       <c r="AO84" s="9"/>
-      <c r="AP84" s="9"/>
+      <c r="AP84" s="9">
+        <v>1</v>
+      </c>
       <c r="AQ84" s="9"/>
       <c r="AR84" s="11"/>
       <c r="AS84" s="9"/>
       <c r="AT84" s="9"/>
       <c r="AU84" s="9"/>
       <c r="AV84" s="9"/>
-      <c r="AW84" s="9"/>
+      <c r="AW84" s="9">
+        <v>1</v>
+      </c>
       <c r="AX84" s="11"/>
       <c r="AY84" s="9"/>
-      <c r="AZ84" s="9"/>
+      <c r="AZ84" s="9">
+        <v>1</v>
+      </c>
       <c r="BA84" s="11"/>
-      <c r="BB84" s="9"/>
+      <c r="BB84" s="9">
+        <v>1</v>
+      </c>
       <c r="BC84" s="9"/>
       <c r="BD84" s="11"/>
       <c r="BE84" s="9"/>
-      <c r="BF84" s="9"/>
+      <c r="BF84" s="9">
+        <v>1</v>
+      </c>
       <c r="BG84" s="11"/>
-      <c r="BH84" s="9"/>
+      <c r="BH84" s="9">
+        <v>1</v>
+      </c>
       <c r="BI84" s="9"/>
       <c r="BJ84" s="11"/>
       <c r="BK84" s="9"/>
@@ -10206,37 +11596,59 @@
       <c r="D85" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
+      <c r="E85" s="4">
+        <v>447669</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>551</v>
+      </c>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
-      <c r="L85" s="9"/>
+      <c r="L85" s="9">
+        <v>1</v>
+      </c>
       <c r="M85" s="11"/>
       <c r="N85" s="9"/>
-      <c r="O85" s="9"/>
+      <c r="O85" s="9">
+        <v>1</v>
+      </c>
       <c r="P85" s="9"/>
       <c r="Q85" s="9"/>
       <c r="R85" s="9"/>
       <c r="S85" s="9"/>
       <c r="T85" s="11"/>
       <c r="U85" s="9"/>
-      <c r="V85" s="9"/>
+      <c r="V85" s="9">
+        <v>1</v>
+      </c>
       <c r="W85" s="9"/>
       <c r="X85" s="9"/>
       <c r="Y85" s="11"/>
-      <c r="Z85" s="9"/>
+      <c r="Z85" s="9">
+        <v>1</v>
+      </c>
       <c r="AA85" s="9"/>
-      <c r="AB85" s="9"/>
+      <c r="AB85" s="9">
+        <v>1</v>
+      </c>
       <c r="AC85" s="9"/>
-      <c r="AD85" s="9"/>
+      <c r="AD85" s="9">
+        <v>1</v>
+      </c>
       <c r="AE85" s="9"/>
       <c r="AF85" s="11"/>
       <c r="AG85" s="9"/>
-      <c r="AH85" s="9"/>
+      <c r="AH85" s="9">
+        <v>1</v>
+      </c>
       <c r="AI85" s="11"/>
-      <c r="AJ85" s="9"/>
+      <c r="AJ85" s="9">
+        <v>1</v>
+      </c>
       <c r="AK85" s="9"/>
       <c r="AL85" s="9"/>
       <c r="AM85" s="9"/>
@@ -10249,21 +11661,33 @@
       <c r="AT85" s="9"/>
       <c r="AU85" s="9"/>
       <c r="AV85" s="9"/>
-      <c r="AW85" s="9"/>
+      <c r="AW85" s="9">
+        <v>1</v>
+      </c>
       <c r="AX85" s="11"/>
       <c r="AY85" s="9"/>
-      <c r="AZ85" s="9"/>
+      <c r="AZ85" s="9">
+        <v>1</v>
+      </c>
       <c r="BA85" s="11"/>
       <c r="BB85" s="9"/>
-      <c r="BC85" s="9"/>
+      <c r="BC85" s="9">
+        <v>1</v>
+      </c>
       <c r="BD85" s="11"/>
-      <c r="BE85" s="9"/>
+      <c r="BE85" s="9">
+        <v>1</v>
+      </c>
       <c r="BF85" s="9"/>
       <c r="BG85" s="11"/>
-      <c r="BH85" s="9"/>
+      <c r="BH85" s="9">
+        <v>1</v>
+      </c>
       <c r="BI85" s="9"/>
       <c r="BJ85" s="11"/>
-      <c r="BK85" s="9"/>
+      <c r="BK85" s="9">
+        <v>1</v>
+      </c>
       <c r="BL85" s="9"/>
       <c r="BM85" s="11"/>
       <c r="BN85" s="9"/>
@@ -10282,37 +11706,65 @@
       <c r="D86" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
+      <c r="E86" s="4">
+        <v>39203</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
-      <c r="L86" s="9"/>
+      <c r="L86" s="9">
+        <v>1</v>
+      </c>
       <c r="M86" s="11"/>
       <c r="N86" s="9"/>
-      <c r="O86" s="9"/>
+      <c r="O86" s="9">
+        <v>1</v>
+      </c>
       <c r="P86" s="9"/>
       <c r="Q86" s="9"/>
       <c r="R86" s="9"/>
       <c r="S86" s="9"/>
       <c r="T86" s="11"/>
       <c r="U86" s="9"/>
-      <c r="V86" s="9"/>
+      <c r="V86" s="9">
+        <v>1</v>
+      </c>
       <c r="W86" s="9"/>
-      <c r="X86" s="9"/>
+      <c r="X86" s="9">
+        <v>1</v>
+      </c>
       <c r="Y86" s="11"/>
-      <c r="Z86" s="9"/>
-      <c r="AA86" s="9"/>
-      <c r="AB86" s="9"/>
-      <c r="AC86" s="9"/>
-      <c r="AD86" s="9"/>
+      <c r="Z86" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA86" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB86" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC86" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD86" s="9">
+        <v>1</v>
+      </c>
       <c r="AE86" s="9"/>
       <c r="AF86" s="11"/>
       <c r="AG86" s="9"/>
-      <c r="AH86" s="9"/>
+      <c r="AH86" s="9">
+        <v>1</v>
+      </c>
       <c r="AI86" s="11"/>
-      <c r="AJ86" s="9"/>
+      <c r="AJ86" s="9">
+        <v>1</v>
+      </c>
       <c r="AK86" s="9"/>
       <c r="AL86" s="9"/>
       <c r="AM86" s="9"/>
@@ -10325,21 +11777,33 @@
       <c r="AT86" s="9"/>
       <c r="AU86" s="9"/>
       <c r="AV86" s="9"/>
-      <c r="AW86" s="9"/>
+      <c r="AW86" s="9">
+        <v>1</v>
+      </c>
       <c r="AX86" s="11"/>
       <c r="AY86" s="9"/>
-      <c r="AZ86" s="9"/>
+      <c r="AZ86" s="9">
+        <v>1</v>
+      </c>
       <c r="BA86" s="11"/>
-      <c r="BB86" s="9"/>
+      <c r="BB86" s="9">
+        <v>1</v>
+      </c>
       <c r="BC86" s="9"/>
       <c r="BD86" s="11"/>
       <c r="BE86" s="9"/>
-      <c r="BF86" s="9"/>
+      <c r="BF86" s="9">
+        <v>1</v>
+      </c>
       <c r="BG86" s="11"/>
-      <c r="BH86" s="9"/>
+      <c r="BH86" s="9">
+        <v>1</v>
+      </c>
       <c r="BI86" s="9"/>
       <c r="BJ86" s="11"/>
-      <c r="BK86" s="9"/>
+      <c r="BK86" s="9">
+        <v>1</v>
+      </c>
       <c r="BL86" s="9"/>
       <c r="BM86" s="11"/>
       <c r="BN86" s="9"/>
@@ -10358,37 +11822,61 @@
       <c r="D87" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
+      <c r="E87" s="4">
+        <v>5049119</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
-      <c r="L87" s="9"/>
+      <c r="L87" s="9">
+        <v>1</v>
+      </c>
       <c r="M87" s="11"/>
       <c r="N87" s="9"/>
       <c r="O87" s="9"/>
-      <c r="P87" s="9"/>
+      <c r="P87" s="9">
+        <v>1</v>
+      </c>
       <c r="Q87" s="9"/>
-      <c r="R87" s="9"/>
+      <c r="R87" s="9">
+        <v>1</v>
+      </c>
       <c r="S87" s="9"/>
       <c r="T87" s="11"/>
       <c r="U87" s="9"/>
       <c r="V87" s="9"/>
       <c r="W87" s="9"/>
-      <c r="X87" s="9"/>
+      <c r="X87" s="9">
+        <v>1</v>
+      </c>
       <c r="Y87" s="11"/>
-      <c r="Z87" s="9"/>
+      <c r="Z87" s="9">
+        <v>1</v>
+      </c>
       <c r="AA87" s="9"/>
-      <c r="AB87" s="9"/>
+      <c r="AB87" s="9">
+        <v>1</v>
+      </c>
       <c r="AC87" s="9"/>
-      <c r="AD87" s="9"/>
+      <c r="AD87" s="9">
+        <v>1</v>
+      </c>
       <c r="AE87" s="9"/>
       <c r="AF87" s="11"/>
-      <c r="AG87" s="9"/>
+      <c r="AG87" s="9">
+        <v>1</v>
+      </c>
       <c r="AH87" s="9"/>
       <c r="AI87" s="11"/>
-      <c r="AJ87" s="9"/>
+      <c r="AJ87" s="9">
+        <v>1</v>
+      </c>
       <c r="AK87" s="9"/>
       <c r="AL87" s="9"/>
       <c r="AM87" s="9"/>
@@ -10400,22 +11888,34 @@
       <c r="AS87" s="9"/>
       <c r="AT87" s="9"/>
       <c r="AU87" s="9"/>
-      <c r="AV87" s="9"/>
+      <c r="AV87" s="9">
+        <v>1</v>
+      </c>
       <c r="AW87" s="9"/>
       <c r="AX87" s="11"/>
-      <c r="AY87" s="9"/>
+      <c r="AY87" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ87" s="9"/>
       <c r="BA87" s="11"/>
       <c r="BB87" s="9"/>
-      <c r="BC87" s="9"/>
+      <c r="BC87" s="9">
+        <v>1</v>
+      </c>
       <c r="BD87" s="11"/>
-      <c r="BE87" s="9"/>
+      <c r="BE87" s="9">
+        <v>1</v>
+      </c>
       <c r="BF87" s="9"/>
       <c r="BG87" s="11"/>
-      <c r="BH87" s="9"/>
+      <c r="BH87" s="9">
+        <v>1</v>
+      </c>
       <c r="BI87" s="9"/>
       <c r="BJ87" s="11"/>
-      <c r="BK87" s="9"/>
+      <c r="BK87" s="9">
+        <v>1</v>
+      </c>
       <c r="BL87" s="9"/>
       <c r="BM87" s="11"/>
       <c r="BN87" s="9"/>
@@ -20316,119 +21816,119 @@
       </c>
       <c r="I217">
         <f>SUM(I3:I215)</f>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="J217">
         <f t="shared" ref="J217:BQ217" si="0">SUM(J3:J215)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K217">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L217">
         <f>SUM(L3:L215)</f>
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="N217">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O217">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="P217">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q217">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R217">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S217">
         <f>SUM(S3:S215)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U217">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="V217">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="W217">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X217">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="Z217">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="AA217">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="AB217">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AC217">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="AD217">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="AE217">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG217">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="AH217">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="AJ217">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="AK217">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL217">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="AM217">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AO217">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="AP217">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AQ217">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AR217" s="12">
         <f t="shared" si="0"/>
@@ -20436,35 +21936,35 @@
       </c>
       <c r="AS217">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AT217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU217">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AV217">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AW217">
         <f>SUM(AW3:AW215)</f>
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="AY217">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="AZ217">
         <f>SUM(AZ3:AZ215)</f>
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="BB217">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="BD217" s="12">
         <f t="shared" si="0"/>
@@ -20472,26 +21972,26 @@
       </c>
       <c r="BE217">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="BF217">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="BG217" s="12" t="s">
         <v>482</v>
       </c>
       <c r="BH217">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="BI217">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BK217">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="BL217">
         <f t="shared" si="0"/>
@@ -20499,7 +21999,7 @@
       </c>
       <c r="BN217">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BO217">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Task 2 - dodano "Transport:
</commit_message>
<xml_diff>
--- a/dane_aplikacji-zygol.xlsx
+++ b/dane_aplikacji-zygol.xlsx
@@ -14,15 +14,16 @@
   <sheets>
     <sheet name="Wykres1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Arkusz1" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="563">
   <si>
     <t>Id</t>
   </si>
@@ -1717,12 +1718,27 @@
   <si>
     <t>50kk-100kk</t>
   </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>100kk-500kk</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>1kkk-5kkk</t>
+  </si>
+  <si>
+    <t>15-11-2014</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1767,11 +1783,18 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
       <color rgb="FF8D8D8D"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1866,7 +1889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1927,7 +1950,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
@@ -1935,6 +1957,14 @@
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2033,27 +2063,28 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$AG$72</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$AH$72</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$AG$72</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:multiLvlStrRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2065,11 +2096,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="238939616"/>
-        <c:axId val="238940160"/>
+        <c:axId val="-42430672"/>
+        <c:axId val="-42426864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="238939616"/>
+        <c:axId val="-42430672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2112,7 +2143,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238940160"/>
+        <c:crossAx val="-42426864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2120,7 +2151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238940160"/>
+        <c:axId val="-42426864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2171,7 +2202,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238939616"/>
+        <c:crossAx val="-42430672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2762,7 +2793,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2773,7 +2804,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302238" cy="6083710"/>
+    <xdr:ext cx="9299408" cy="6065921"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Wykres 1"/>
@@ -3085,18 +3116,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="41.125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
-    <col min="4" max="5" width="14.75" customWidth="1"/>
-    <col min="6" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="15.75" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="14.75" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.75" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="1.375" customWidth="1"/>
     <col min="9" max="12" width="3.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="1.125" style="12" customWidth="1"/>
@@ -3133,7 +3164,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="92.25" customHeight="1">
-      <c r="E1" s="24"/>
+      <c r="E1" s="27"/>
       <c r="H1" t="s">
         <v>482</v>
       </c>
@@ -3238,7 +3269,7 @@
       <c r="BM1" s="10"/>
       <c r="BN1" s="7"/>
     </row>
-    <row r="2" spans="1:69" ht="141.75" thickBot="1">
+    <row r="2" spans="1:69" ht="143.25" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3415,7 +3446,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="3" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="3" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
@@ -3521,7 +3552,7 @@
       <c r="BP3" s="19"/>
       <c r="BQ3" s="19"/>
     </row>
-    <row r="4" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="4" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
@@ -3707,7 +3738,7 @@
       <c r="BP5" s="19"/>
       <c r="BQ5" s="19"/>
     </row>
-    <row r="6" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="6" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A6" s="22" t="s">
         <v>10</v>
       </c>
@@ -3783,7 +3814,7 @@
       <c r="BP6" s="19"/>
       <c r="BQ6" s="19"/>
     </row>
-    <row r="7" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="7" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -3891,7 +3922,7 @@
       <c r="BP7" s="19"/>
       <c r="BQ7" s="19"/>
     </row>
-    <row r="8" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -3997,7 +4028,7 @@
       <c r="BP8" s="19"/>
       <c r="BQ8" s="19"/>
     </row>
-    <row r="9" spans="1:69" s="18" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
+    <row r="9" spans="1:69" s="18" customFormat="1" ht="17.25" hidden="1" customHeight="1" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
@@ -4115,7 +4146,7 @@
       <c r="BP9" s="19"/>
       <c r="BQ9" s="19"/>
     </row>
-    <row r="10" spans="1:69" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:69" s="18" customFormat="1" ht="15" hidden="1" customHeight="1" thickBot="1">
       <c r="A10" s="16" t="s">
         <v>18</v>
       </c>
@@ -4229,7 +4260,7 @@
       <c r="BP10" s="19"/>
       <c r="BQ10" s="19"/>
     </row>
-    <row r="11" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="11" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
@@ -4335,7 +4366,7 @@
       <c r="BP11" s="19"/>
       <c r="BQ11" s="19"/>
     </row>
-    <row r="12" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="12" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
@@ -4451,7 +4482,7 @@
       <c r="BP12" s="19"/>
       <c r="BQ12" s="19"/>
     </row>
-    <row r="13" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="13" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
@@ -4569,7 +4600,7 @@
       <c r="BP13" s="19"/>
       <c r="BQ13" s="19"/>
     </row>
-    <row r="14" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="14" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A14" s="16" t="s">
         <v>26</v>
       </c>
@@ -4757,7 +4788,7 @@
       <c r="BP15" s="9"/>
       <c r="BQ15" s="9"/>
     </row>
-    <row r="16" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="16" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A16" s="16" t="s">
         <v>30</v>
       </c>
@@ -4863,7 +4894,7 @@
       <c r="BP16" s="19"/>
       <c r="BQ16" s="19"/>
     </row>
-    <row r="17" spans="1:69" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="17" spans="1:69" s="18" customFormat="1" ht="15" hidden="1" customHeight="1" thickBot="1">
       <c r="A17" s="16" t="s">
         <v>32</v>
       </c>
@@ -4971,7 +5002,7 @@
       <c r="BP17" s="19"/>
       <c r="BQ17" s="19"/>
     </row>
-    <row r="18" spans="1:69" s="18" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" customHeight="1" thickBot="1">
       <c r="A18" s="16" t="s">
         <v>34</v>
       </c>
@@ -5075,7 +5106,7 @@
       <c r="BP18" s="19"/>
       <c r="BQ18" s="19"/>
     </row>
-    <row r="19" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="19" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
@@ -5195,7 +5226,7 @@
       <c r="BP19" s="19"/>
       <c r="BQ19" s="19"/>
     </row>
-    <row r="20" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="20" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>38</v>
       </c>
@@ -5307,7 +5338,7 @@
       <c r="BP20" s="19"/>
       <c r="BQ20" s="19"/>
     </row>
-    <row r="21" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="21" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
@@ -5423,7 +5454,7 @@
       <c r="BP21" s="19"/>
       <c r="BQ21" s="19"/>
     </row>
-    <row r="22" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="22" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A22" s="16" t="s">
         <v>42</v>
       </c>
@@ -5537,7 +5568,7 @@
       <c r="BP22" s="19"/>
       <c r="BQ22" s="19"/>
     </row>
-    <row r="23" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="23" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A23" s="16" t="s">
         <v>44</v>
       </c>
@@ -5659,7 +5690,7 @@
       <c r="BP23" s="19"/>
       <c r="BQ23" s="19"/>
     </row>
-    <row r="24" spans="1:69" ht="16.5" thickBot="1">
+    <row r="24" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -5735,7 +5766,7 @@
       <c r="BP24" s="9"/>
       <c r="BQ24" s="9"/>
     </row>
-    <row r="25" spans="1:69" ht="16.5" thickBot="1">
+    <row r="25" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -5811,7 +5842,7 @@
       <c r="BP25" s="9"/>
       <c r="BQ25" s="9"/>
     </row>
-    <row r="26" spans="1:69" ht="16.5" thickBot="1">
+    <row r="26" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
@@ -5887,7 +5918,7 @@
       <c r="BP26" s="9"/>
       <c r="BQ26" s="9"/>
     </row>
-    <row r="27" spans="1:69" ht="16.5" thickBot="1">
+    <row r="27" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>53</v>
       </c>
@@ -5963,7 +5994,7 @@
       <c r="BP27" s="9"/>
       <c r="BQ27" s="9"/>
     </row>
-    <row r="28" spans="1:69" ht="16.5" thickBot="1">
+    <row r="28" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
@@ -6039,7 +6070,7 @@
       <c r="BP28" s="9"/>
       <c r="BQ28" s="9"/>
     </row>
-    <row r="29" spans="1:69" ht="16.5" thickBot="1">
+    <row r="29" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -6115,7 +6146,7 @@
       <c r="BP29" s="9"/>
       <c r="BQ29" s="9"/>
     </row>
-    <row r="30" spans="1:69" ht="16.5" thickBot="1">
+    <row r="30" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
@@ -6191,7 +6222,7 @@
       <c r="BP30" s="9"/>
       <c r="BQ30" s="9"/>
     </row>
-    <row r="31" spans="1:69" ht="16.5" thickBot="1">
+    <row r="31" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
@@ -6267,7 +6298,7 @@
       <c r="BP31" s="9"/>
       <c r="BQ31" s="9"/>
     </row>
-    <row r="32" spans="1:69" ht="16.5" thickBot="1">
+    <row r="32" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A32" s="3" t="s">
         <v>63</v>
       </c>
@@ -6343,7 +6374,7 @@
       <c r="BP32" s="9"/>
       <c r="BQ32" s="9"/>
     </row>
-    <row r="33" spans="1:69" ht="16.5" thickBot="1">
+    <row r="33" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -6419,7 +6450,7 @@
       <c r="BP33" s="9"/>
       <c r="BQ33" s="9"/>
     </row>
-    <row r="34" spans="1:69" ht="16.5" thickBot="1">
+    <row r="34" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A34" s="3" t="s">
         <v>67</v>
       </c>
@@ -6495,7 +6526,7 @@
       <c r="BP34" s="9"/>
       <c r="BQ34" s="9"/>
     </row>
-    <row r="35" spans="1:69" ht="16.5" thickBot="1">
+    <row r="35" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -6571,7 +6602,7 @@
       <c r="BP35" s="9"/>
       <c r="BQ35" s="9"/>
     </row>
-    <row r="36" spans="1:69" ht="16.5" thickBot="1">
+    <row r="36" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -6647,7 +6678,7 @@
       <c r="BP36" s="9"/>
       <c r="BQ36" s="9"/>
     </row>
-    <row r="37" spans="1:69" ht="16.5" thickBot="1">
+    <row r="37" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
@@ -6723,7 +6754,7 @@
       <c r="BP37" s="9"/>
       <c r="BQ37" s="9"/>
     </row>
-    <row r="38" spans="1:69" ht="16.5" thickBot="1">
+    <row r="38" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
@@ -6799,7 +6830,7 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:69" ht="16.5" thickBot="1">
+    <row r="39" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
@@ -6875,7 +6906,7 @@
       <c r="BP39" s="9"/>
       <c r="BQ39" s="9"/>
     </row>
-    <row r="40" spans="1:69" ht="16.5" thickBot="1">
+    <row r="40" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
@@ -6951,7 +6982,7 @@
       <c r="BP40" s="9"/>
       <c r="BQ40" s="9"/>
     </row>
-    <row r="41" spans="1:69" ht="16.5" thickBot="1">
+    <row r="41" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>81</v>
       </c>
@@ -7027,7 +7058,7 @@
       <c r="BP41" s="9"/>
       <c r="BQ41" s="9"/>
     </row>
-    <row r="42" spans="1:69" ht="16.5" thickBot="1">
+    <row r="42" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A42" s="3" t="s">
         <v>83</v>
       </c>
@@ -7103,7 +7134,7 @@
       <c r="BP42" s="9"/>
       <c r="BQ42" s="9"/>
     </row>
-    <row r="43" spans="1:69" ht="16.5" thickBot="1">
+    <row r="43" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A43" s="3" t="s">
         <v>85</v>
       </c>
@@ -7179,7 +7210,7 @@
       <c r="BP43" s="9"/>
       <c r="BQ43" s="9"/>
     </row>
-    <row r="44" spans="1:69" ht="16.5" thickBot="1">
+    <row r="44" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>87</v>
       </c>
@@ -7255,7 +7286,7 @@
       <c r="BP44" s="9"/>
       <c r="BQ44" s="9"/>
     </row>
-    <row r="45" spans="1:69" ht="16.5" thickBot="1">
+    <row r="45" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>89</v>
       </c>
@@ -7331,7 +7362,7 @@
       <c r="BP45" s="9"/>
       <c r="BQ45" s="9"/>
     </row>
-    <row r="46" spans="1:69" ht="16.5" thickBot="1">
+    <row r="46" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A46" s="3" t="s">
         <v>91</v>
       </c>
@@ -7439,7 +7470,7 @@
       <c r="BP46" s="9"/>
       <c r="BQ46" s="9"/>
     </row>
-    <row r="47" spans="1:69" ht="16.5" thickBot="1">
+    <row r="47" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A47" s="3" t="s">
         <v>94</v>
       </c>
@@ -7565,7 +7596,7 @@
       <c r="BP47" s="9"/>
       <c r="BQ47" s="9"/>
     </row>
-    <row r="48" spans="1:69" ht="16.5" thickBot="1">
+    <row r="48" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A48" s="3" t="s">
         <v>96</v>
       </c>
@@ -7681,7 +7712,7 @@
       <c r="BP48" s="9"/>
       <c r="BQ48" s="9"/>
     </row>
-    <row r="49" spans="1:69" ht="16.5" thickBot="1">
+    <row r="49" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>98</v>
       </c>
@@ -7801,20 +7832,20 @@
       <c r="BP49" s="9"/>
       <c r="BQ49" s="9"/>
     </row>
-    <row r="50" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A50" s="25" t="s">
+    <row r="50" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+      <c r="A50" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26" t="s">
+      <c r="C50" s="25"/>
+      <c r="D50" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -7877,7 +7908,7 @@
       <c r="BP50" s="9"/>
       <c r="BQ50" s="9"/>
     </row>
-    <row r="51" spans="1:69" ht="16.5" thickBot="1">
+    <row r="51" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A51" s="3" t="s">
         <v>102</v>
       </c>
@@ -7991,7 +8022,7 @@
       <c r="BP51" s="9"/>
       <c r="BQ51" s="9"/>
     </row>
-    <row r="52" spans="1:69" ht="16.5" thickBot="1">
+    <row r="52" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A52" s="3" t="s">
         <v>104</v>
       </c>
@@ -8099,7 +8130,7 @@
       <c r="BP52" s="9"/>
       <c r="BQ52" s="9"/>
     </row>
-    <row r="53" spans="1:69" ht="16.5" thickBot="1">
+    <row r="53" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A53" s="3" t="s">
         <v>106</v>
       </c>
@@ -8211,7 +8242,7 @@
       <c r="BP53" s="9"/>
       <c r="BQ53" s="9"/>
     </row>
-    <row r="54" spans="1:69" ht="16.5" thickBot="1">
+    <row r="54" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A54" s="3" t="s">
         <v>108</v>
       </c>
@@ -8325,7 +8356,7 @@
       <c r="BP54" s="9"/>
       <c r="BQ54" s="9"/>
     </row>
-    <row r="55" spans="1:69" ht="16.5" thickBot="1">
+    <row r="55" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
@@ -8437,20 +8468,20 @@
       <c r="BP55" s="9"/>
       <c r="BQ55" s="9"/>
     </row>
-    <row r="56" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A56" s="25" t="s">
+    <row r="56" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+      <c r="A56" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="B56" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26" t="s">
+      <c r="C56" s="25"/>
+      <c r="D56" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -8513,7 +8544,7 @@
       <c r="BP56" s="9"/>
       <c r="BQ56" s="9"/>
     </row>
-    <row r="57" spans="1:69" ht="16.5" thickBot="1">
+    <row r="57" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A57" s="3" t="s">
         <v>114</v>
       </c>
@@ -8627,7 +8658,7 @@
       <c r="BP57" s="9"/>
       <c r="BQ57" s="9"/>
     </row>
-    <row r="58" spans="1:69" ht="16.5" thickBot="1">
+    <row r="58" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A58" s="3" t="s">
         <v>116</v>
       </c>
@@ -8737,7 +8768,7 @@
       <c r="BP58" s="9"/>
       <c r="BQ58" s="9"/>
     </row>
-    <row r="59" spans="1:69" ht="16.5" thickBot="1">
+    <row r="59" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A59" s="3" t="s">
         <v>118</v>
       </c>
@@ -8845,7 +8876,7 @@
       <c r="BP59" s="9"/>
       <c r="BQ59" s="9"/>
     </row>
-    <row r="60" spans="1:69" ht="16.5" thickBot="1">
+    <row r="60" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A60" s="3" t="s">
         <v>120</v>
       </c>
@@ -8961,7 +8992,7 @@
       <c r="BP60" s="9"/>
       <c r="BQ60" s="9"/>
     </row>
-    <row r="61" spans="1:69" ht="16.5" thickBot="1">
+    <row r="61" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A61" s="3" t="s">
         <v>122</v>
       </c>
@@ -9079,7 +9110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:69" ht="16.5" thickBot="1">
+    <row r="62" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A62" s="3" t="s">
         <v>124</v>
       </c>
@@ -9197,7 +9228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:69" ht="15.75" customHeight="1" thickBot="1">
+    <row r="63" spans="1:69" ht="15.75" hidden="1" customHeight="1" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>126</v>
       </c>
@@ -9307,7 +9338,7 @@
       <c r="BP63" s="9"/>
       <c r="BQ63" s="9"/>
     </row>
-    <row r="64" spans="1:69" ht="16.5" thickBot="1">
+    <row r="64" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>128</v>
       </c>
@@ -9423,7 +9454,7 @@
       <c r="BP64" s="9"/>
       <c r="BQ64" s="9"/>
     </row>
-    <row r="65" spans="1:69" ht="16.5" thickBot="1">
+    <row r="65" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>130</v>
       </c>
@@ -9547,7 +9578,7 @@
       <c r="BP65" s="9"/>
       <c r="BQ65" s="9"/>
     </row>
-    <row r="66" spans="1:69" ht="16.5" thickBot="1">
+    <row r="66" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A66" s="3" t="s">
         <v>132</v>
       </c>
@@ -9667,14 +9698,16 @@
       <c r="BP66" s="9"/>
       <c r="BQ66" s="9"/>
     </row>
-    <row r="67" spans="1:69" ht="16.5" thickBot="1">
+    <row r="67" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A67" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="4"/>
+      <c r="C67" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D67" s="4" t="s">
         <v>136</v>
       </c>
@@ -9781,14 +9814,16 @@
       <c r="BP67" s="9"/>
       <c r="BQ67" s="9"/>
     </row>
-    <row r="68" spans="1:69" ht="16.5" thickBot="1">
+    <row r="68" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A68" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="4"/>
+      <c r="C68" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D68" s="4" t="s">
         <v>136</v>
       </c>
@@ -9885,20 +9920,20 @@
       <c r="BP68" s="9"/>
       <c r="BQ68" s="9"/>
     </row>
-    <row r="69" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A69" s="25" t="s">
+    <row r="69" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+      <c r="A69" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="26" t="s">
+      <c r="B69" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="26"/>
-      <c r="D69" s="26" t="s">
+      <c r="C69" s="4"/>
+      <c r="D69" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="E69" s="26"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="25"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -9961,14 +9996,16 @@
       <c r="BP69" s="9"/>
       <c r="BQ69" s="9"/>
     </row>
-    <row r="70" spans="1:69" ht="16.5" thickBot="1">
+    <row r="70" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A70" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="4"/>
+      <c r="C70" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D70" s="4" t="s">
         <v>136</v>
       </c>
@@ -10067,18 +10104,20 @@
       <c r="BP70" s="9"/>
       <c r="BQ70" s="9"/>
     </row>
-    <row r="71" spans="1:69" ht="32.25" thickBot="1">
+    <row r="71" spans="1:69" ht="32.25" hidden="1" thickBot="1">
       <c r="A71" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="4"/>
+      <c r="C71" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D71" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E71" s="27">
+      <c r="E71" s="26">
         <v>9029</v>
       </c>
       <c r="F71" s="4" t="s">
@@ -10177,14 +10216,16 @@
       <c r="BP71" s="9"/>
       <c r="BQ71" s="9"/>
     </row>
-    <row r="72" spans="1:69" ht="16.5" thickBot="1">
+    <row r="72" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A72" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="4"/>
+      <c r="C72" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D72" s="4" t="s">
         <v>136</v>
       </c>
@@ -10283,14 +10324,16 @@
       <c r="BP72" s="9"/>
       <c r="BQ72" s="9"/>
     </row>
-    <row r="73" spans="1:69" ht="16.5" thickBot="1">
+    <row r="73" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A73" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="4"/>
+      <c r="C73" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D73" s="4" t="s">
         <v>136</v>
       </c>
@@ -10393,14 +10436,16 @@
       <c r="BP73" s="9"/>
       <c r="BQ73" s="9"/>
     </row>
-    <row r="74" spans="1:69" ht="16.5" thickBot="1">
+    <row r="74" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A74" s="3" t="s">
         <v>149</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="4"/>
+      <c r="C74" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D74" s="4" t="s">
         <v>136</v>
       </c>
@@ -10505,14 +10550,16 @@
       <c r="BP74" s="9"/>
       <c r="BQ74" s="9"/>
     </row>
-    <row r="75" spans="1:69" ht="16.5" thickBot="1">
+    <row r="75" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A75" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="4"/>
+      <c r="C75" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D75" s="4" t="s">
         <v>136</v>
       </c>
@@ -10621,14 +10668,16 @@
       <c r="BP75" s="9"/>
       <c r="BQ75" s="9"/>
     </row>
-    <row r="76" spans="1:69" ht="16.5" thickBot="1">
+    <row r="76" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A76" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="4"/>
+      <c r="C76" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D76" s="4" t="s">
         <v>136</v>
       </c>
@@ -10729,14 +10778,16 @@
       <c r="BP76" s="9"/>
       <c r="BQ76" s="9"/>
     </row>
-    <row r="77" spans="1:69" ht="16.5" thickBot="1">
+    <row r="77" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A77" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="4"/>
+      <c r="C77" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D77" s="4" t="s">
         <v>136</v>
       </c>
@@ -10837,14 +10888,16 @@
       <c r="BP77" s="9"/>
       <c r="BQ77" s="9"/>
     </row>
-    <row r="78" spans="1:69" ht="16.5" thickBot="1">
+    <row r="78" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A78" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C78" s="4"/>
+      <c r="C78" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D78" s="4" t="s">
         <v>136</v>
       </c>
@@ -10945,14 +10998,16 @@
       <c r="BP78" s="9"/>
       <c r="BQ78" s="9"/>
     </row>
-    <row r="79" spans="1:69" ht="16.5" thickBot="1">
+    <row r="79" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A79" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="4"/>
+      <c r="C79" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D79" s="4" t="s">
         <v>136</v>
       </c>
@@ -11067,14 +11122,16 @@
       <c r="BP79" s="9"/>
       <c r="BQ79" s="9"/>
     </row>
-    <row r="80" spans="1:69" ht="16.5" thickBot="1">
+    <row r="80" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A80" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C80" s="4"/>
+      <c r="C80" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D80" s="4" t="s">
         <v>136</v>
       </c>
@@ -11173,20 +11230,20 @@
       <c r="BP80" s="9"/>
       <c r="BQ80" s="9"/>
     </row>
-    <row r="81" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A81" s="25" t="s">
+    <row r="81" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+      <c r="A81" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26" t="s">
+      <c r="C81" s="4"/>
+      <c r="D81" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="E81" s="26"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="26"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="25"/>
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
@@ -11249,14 +11306,16 @@
       <c r="BP81" s="9"/>
       <c r="BQ81" s="9"/>
     </row>
-    <row r="82" spans="1:69" ht="16.5" thickBot="1">
+    <row r="82" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A82" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="4"/>
+      <c r="C82" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D82" s="4" t="s">
         <v>136</v>
       </c>
@@ -11363,14 +11422,16 @@
       <c r="BP82" s="9"/>
       <c r="BQ82" s="9"/>
     </row>
-    <row r="83" spans="1:69" ht="16.5" thickBot="1">
+    <row r="83" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A83" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C83" s="4"/>
+      <c r="C83" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D83" s="4" t="s">
         <v>136</v>
       </c>
@@ -11475,14 +11536,16 @@
       <c r="BP83" s="9"/>
       <c r="BQ83" s="9"/>
     </row>
-    <row r="84" spans="1:69" ht="16.5" thickBot="1">
+    <row r="84" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A84" s="3" t="s">
         <v>169</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C84" s="4"/>
+      <c r="C84" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D84" s="4" t="s">
         <v>136</v>
       </c>
@@ -11585,14 +11648,16 @@
       <c r="BP84" s="9"/>
       <c r="BQ84" s="9"/>
     </row>
-    <row r="85" spans="1:69" ht="16.5" thickBot="1">
+    <row r="85" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A85" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C85" s="4"/>
+      <c r="C85" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D85" s="4" t="s">
         <v>136</v>
       </c>
@@ -11695,14 +11760,16 @@
       <c r="BP85" s="9"/>
       <c r="BQ85" s="9"/>
     </row>
-    <row r="86" spans="1:69" ht="16.5" thickBot="1">
+    <row r="86" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A86" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C86" s="4"/>
+      <c r="C86" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D86" s="4" t="s">
         <v>136</v>
       </c>
@@ -11811,14 +11878,16 @@
       <c r="BP86" s="9"/>
       <c r="BQ86" s="9"/>
     </row>
-    <row r="87" spans="1:69" ht="16.5" thickBot="1">
+    <row r="87" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A87" s="3" t="s">
         <v>175</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C87" s="4"/>
+      <c r="C87" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D87" s="4" t="s">
         <v>136</v>
       </c>
@@ -11923,27 +11992,41 @@
       <c r="BP87" s="9"/>
       <c r="BQ87" s="9"/>
     </row>
-    <row r="88" spans="1:69" ht="16.5" thickBot="1">
+    <row r="88" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A88" s="3" t="s">
         <v>177</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C88" s="4"/>
+      <c r="C88" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D88" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="I88" s="9"/>
+      <c r="E88" s="4">
+        <v>7474</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I88" s="9">
+        <v>1</v>
+      </c>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
-      <c r="L88" s="9"/>
+      <c r="L88" s="9">
+        <v>1</v>
+      </c>
       <c r="M88" s="11"/>
       <c r="N88" s="9"/>
-      <c r="O88" s="9"/>
+      <c r="O88" s="9">
+        <v>1</v>
+      </c>
       <c r="P88" s="9"/>
       <c r="Q88" s="9"/>
       <c r="R88" s="9"/>
@@ -11952,9 +12035,13 @@
       <c r="U88" s="9"/>
       <c r="V88" s="9"/>
       <c r="W88" s="9"/>
-      <c r="X88" s="9"/>
+      <c r="X88" s="9">
+        <v>1</v>
+      </c>
       <c r="Y88" s="11"/>
-      <c r="Z88" s="9"/>
+      <c r="Z88" s="9">
+        <v>1</v>
+      </c>
       <c r="AA88" s="9"/>
       <c r="AB88" s="9"/>
       <c r="AC88" s="9"/>
@@ -11962,11 +12049,15 @@
       <c r="AE88" s="9"/>
       <c r="AF88" s="11"/>
       <c r="AG88" s="9"/>
-      <c r="AH88" s="9"/>
+      <c r="AH88" s="9">
+        <v>1</v>
+      </c>
       <c r="AI88" s="11"/>
       <c r="AJ88" s="9"/>
       <c r="AK88" s="9"/>
-      <c r="AL88" s="9"/>
+      <c r="AL88" s="9">
+        <v>1</v>
+      </c>
       <c r="AM88" s="9"/>
       <c r="AN88" s="11"/>
       <c r="AO88" s="9"/>
@@ -11977,21 +12068,33 @@
       <c r="AT88" s="9"/>
       <c r="AU88" s="9"/>
       <c r="AV88" s="9"/>
-      <c r="AW88" s="9"/>
+      <c r="AW88" s="9">
+        <v>1</v>
+      </c>
       <c r="AX88" s="11"/>
       <c r="AY88" s="9"/>
-      <c r="AZ88" s="9"/>
+      <c r="AZ88" s="9">
+        <v>1</v>
+      </c>
       <c r="BA88" s="11"/>
-      <c r="BB88" s="9"/>
+      <c r="BB88" s="9">
+        <v>1</v>
+      </c>
       <c r="BC88" s="9"/>
       <c r="BD88" s="11"/>
-      <c r="BE88" s="9"/>
+      <c r="BE88" s="9">
+        <v>1</v>
+      </c>
       <c r="BF88" s="9"/>
       <c r="BG88" s="11"/>
-      <c r="BH88" s="9"/>
+      <c r="BH88" s="9">
+        <v>1</v>
+      </c>
       <c r="BI88" s="9"/>
       <c r="BJ88" s="11"/>
-      <c r="BK88" s="9"/>
+      <c r="BK88" s="9">
+        <v>1</v>
+      </c>
       <c r="BL88" s="9"/>
       <c r="BM88" s="11"/>
       <c r="BN88" s="9"/>
@@ -11999,48 +12102,84 @@
       <c r="BP88" s="9"/>
       <c r="BQ88" s="9"/>
     </row>
-    <row r="89" spans="1:69" ht="16.5" thickBot="1">
+    <row r="89" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A89" s="3" t="s">
         <v>180</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="4"/>
+      <c r="C89" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D89" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
-      <c r="G89" s="4"/>
-      <c r="I89" s="9"/>
+      <c r="E89" s="4">
+        <v>4533</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="I89" s="9">
+        <v>1</v>
+      </c>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
-      <c r="L89" s="9"/>
+      <c r="L89" s="9">
+        <v>1</v>
+      </c>
       <c r="M89" s="11"/>
-      <c r="N89" s="9"/>
+      <c r="N89" s="9">
+        <v>1</v>
+      </c>
       <c r="O89" s="9"/>
-      <c r="P89" s="9"/>
-      <c r="Q89" s="9"/>
+      <c r="P89" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q89" s="9">
+        <v>1</v>
+      </c>
       <c r="R89" s="9"/>
-      <c r="S89" s="9"/>
+      <c r="S89" s="9">
+        <v>1</v>
+      </c>
       <c r="T89" s="11"/>
-      <c r="U89" s="9"/>
-      <c r="V89" s="9"/>
+      <c r="U89" s="9">
+        <v>1</v>
+      </c>
+      <c r="V89" s="9">
+        <v>1</v>
+      </c>
       <c r="W89" s="9"/>
-      <c r="X89" s="9"/>
+      <c r="X89" s="9">
+        <v>1</v>
+      </c>
       <c r="Y89" s="11"/>
-      <c r="Z89" s="9"/>
+      <c r="Z89" s="9">
+        <v>1</v>
+      </c>
       <c r="AA89" s="9"/>
-      <c r="AB89" s="9"/>
+      <c r="AB89" s="9">
+        <v>1</v>
+      </c>
       <c r="AC89" s="9"/>
-      <c r="AD89" s="9"/>
+      <c r="AD89" s="9">
+        <v>1</v>
+      </c>
       <c r="AE89" s="9"/>
       <c r="AF89" s="11"/>
       <c r="AG89" s="9"/>
-      <c r="AH89" s="9"/>
+      <c r="AH89" s="9">
+        <v>1</v>
+      </c>
       <c r="AI89" s="11"/>
-      <c r="AJ89" s="9"/>
+      <c r="AJ89" s="9">
+        <v>1</v>
+      </c>
       <c r="AK89" s="9"/>
       <c r="AL89" s="9"/>
       <c r="AM89" s="9"/>
@@ -12049,25 +12188,39 @@
       <c r="AP89" s="9"/>
       <c r="AQ89" s="9"/>
       <c r="AR89" s="11"/>
-      <c r="AS89" s="9"/>
+      <c r="AS89" s="9">
+        <v>1</v>
+      </c>
       <c r="AT89" s="9"/>
       <c r="AU89" s="9"/>
-      <c r="AV89" s="9"/>
+      <c r="AV89" s="9">
+        <v>1</v>
+      </c>
       <c r="AW89" s="9"/>
       <c r="AX89" s="11"/>
       <c r="AY89" s="9"/>
-      <c r="AZ89" s="9"/>
+      <c r="AZ89" s="9">
+        <v>1</v>
+      </c>
       <c r="BA89" s="11"/>
-      <c r="BB89" s="9"/>
+      <c r="BB89" s="9">
+        <v>1</v>
+      </c>
       <c r="BC89" s="9"/>
       <c r="BD89" s="11"/>
-      <c r="BE89" s="9"/>
+      <c r="BE89" s="9">
+        <v>1</v>
+      </c>
       <c r="BF89" s="9"/>
       <c r="BG89" s="11"/>
-      <c r="BH89" s="9"/>
+      <c r="BH89" s="9">
+        <v>1</v>
+      </c>
       <c r="BI89" s="9"/>
       <c r="BJ89" s="11"/>
-      <c r="BK89" s="9"/>
+      <c r="BK89" s="9">
+        <v>1</v>
+      </c>
       <c r="BL89" s="9"/>
       <c r="BM89" s="11"/>
       <c r="BN89" s="9"/>
@@ -12075,53 +12228,81 @@
       <c r="BP89" s="9"/>
       <c r="BQ89" s="9"/>
     </row>
-    <row r="90" spans="1:69" ht="16.5" thickBot="1">
+    <row r="90" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A90" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C90" s="4"/>
+      <c r="C90" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D90" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="I90" s="9"/>
+      <c r="E90" s="4">
+        <v>1997</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="I90" s="9">
+        <v>1</v>
+      </c>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
-      <c r="L90" s="9"/>
+      <c r="L90" s="9">
+        <v>1</v>
+      </c>
       <c r="M90" s="11"/>
       <c r="N90" s="9"/>
-      <c r="O90" s="9"/>
+      <c r="O90" s="9">
+        <v>1</v>
+      </c>
       <c r="P90" s="9"/>
       <c r="Q90" s="9"/>
       <c r="R90" s="9"/>
       <c r="S90" s="9"/>
       <c r="T90" s="11"/>
       <c r="U90" s="9"/>
-      <c r="V90" s="9"/>
+      <c r="V90" s="9">
+        <v>1</v>
+      </c>
       <c r="W90" s="9"/>
-      <c r="X90" s="9"/>
+      <c r="X90" s="9">
+        <v>1</v>
+      </c>
       <c r="Y90" s="11"/>
-      <c r="Z90" s="9"/>
+      <c r="Z90" s="9">
+        <v>1</v>
+      </c>
       <c r="AA90" s="9"/>
       <c r="AB90" s="9"/>
       <c r="AC90" s="9"/>
-      <c r="AD90" s="9"/>
+      <c r="AD90" s="9">
+        <v>1</v>
+      </c>
       <c r="AE90" s="9"/>
       <c r="AF90" s="11"/>
       <c r="AG90" s="9"/>
-      <c r="AH90" s="9"/>
+      <c r="AH90" s="9">
+        <v>1</v>
+      </c>
       <c r="AI90" s="11"/>
       <c r="AJ90" s="9"/>
       <c r="AK90" s="9"/>
-      <c r="AL90" s="9"/>
+      <c r="AL90" s="9">
+        <v>1</v>
+      </c>
       <c r="AM90" s="9"/>
       <c r="AN90" s="11"/>
-      <c r="AO90" s="9"/>
+      <c r="AO90" s="9">
+        <v>1</v>
+      </c>
       <c r="AP90" s="9"/>
       <c r="AQ90" s="9"/>
       <c r="AR90" s="11"/>
@@ -12129,21 +12310,33 @@
       <c r="AT90" s="9"/>
       <c r="AU90" s="9"/>
       <c r="AV90" s="9"/>
-      <c r="AW90" s="9"/>
+      <c r="AW90" s="9">
+        <v>1</v>
+      </c>
       <c r="AX90" s="11"/>
       <c r="AY90" s="9"/>
-      <c r="AZ90" s="9"/>
+      <c r="AZ90" s="9">
+        <v>1</v>
+      </c>
       <c r="BA90" s="11"/>
       <c r="BB90" s="9"/>
-      <c r="BC90" s="9"/>
+      <c r="BC90" s="9">
+        <v>1</v>
+      </c>
       <c r="BD90" s="11"/>
-      <c r="BE90" s="9"/>
+      <c r="BE90" s="9">
+        <v>1</v>
+      </c>
       <c r="BF90" s="9"/>
       <c r="BG90" s="11"/>
-      <c r="BH90" s="9"/>
+      <c r="BH90" s="9">
+        <v>1</v>
+      </c>
       <c r="BI90" s="9"/>
       <c r="BJ90" s="11"/>
-      <c r="BK90" s="9"/>
+      <c r="BK90" s="9">
+        <v>1</v>
+      </c>
       <c r="BL90" s="9"/>
       <c r="BM90" s="11"/>
       <c r="BN90" s="9"/>
@@ -12152,19 +12345,20 @@
       <c r="BQ90" s="9"/>
     </row>
     <row r="91" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4" t="s">
+      <c r="C91" s="15"/>
+      <c r="D91" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="28"/>
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
@@ -12227,48 +12421,78 @@
       <c r="BP91" s="9"/>
       <c r="BQ91" s="9"/>
     </row>
-    <row r="92" spans="1:69" ht="16.5" thickBot="1">
+    <row r="92" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A92" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C92" s="4"/>
+      <c r="C92" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D92" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
+      <c r="E92" s="4">
+        <v>38324</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
+      <c r="J92" s="9">
+        <v>1</v>
+      </c>
       <c r="K92" s="9"/>
-      <c r="L92" s="9"/>
+      <c r="L92" s="9">
+        <v>1</v>
+      </c>
       <c r="M92" s="11"/>
-      <c r="N92" s="9"/>
+      <c r="N92" s="9">
+        <v>1</v>
+      </c>
       <c r="O92" s="9"/>
-      <c r="P92" s="9"/>
+      <c r="P92" s="9">
+        <v>1</v>
+      </c>
       <c r="Q92" s="9"/>
-      <c r="R92" s="9"/>
+      <c r="R92" s="9">
+        <v>1</v>
+      </c>
       <c r="S92" s="9"/>
       <c r="T92" s="11"/>
       <c r="U92" s="9"/>
       <c r="V92" s="9"/>
       <c r="W92" s="9"/>
-      <c r="X92" s="9"/>
+      <c r="X92" s="9">
+        <v>1</v>
+      </c>
       <c r="Y92" s="11"/>
-      <c r="Z92" s="9"/>
-      <c r="AA92" s="9"/>
+      <c r="Z92" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA92" s="9">
+        <v>1</v>
+      </c>
       <c r="AB92" s="9"/>
       <c r="AC92" s="9"/>
-      <c r="AD92" s="9"/>
+      <c r="AD92" s="9">
+        <v>1</v>
+      </c>
       <c r="AE92" s="9"/>
       <c r="AF92" s="11"/>
       <c r="AG92" s="9"/>
-      <c r="AH92" s="9"/>
+      <c r="AH92" s="9">
+        <v>1</v>
+      </c>
       <c r="AI92" s="11"/>
-      <c r="AJ92" s="9"/>
+      <c r="AJ92" s="9">
+        <v>1</v>
+      </c>
       <c r="AK92" s="9"/>
       <c r="AL92" s="9"/>
       <c r="AM92" s="9"/>
@@ -12281,21 +12505,33 @@
       <c r="AT92" s="9"/>
       <c r="AU92" s="9"/>
       <c r="AV92" s="9"/>
-      <c r="AW92" s="9"/>
+      <c r="AW92" s="9">
+        <v>1</v>
+      </c>
       <c r="AX92" s="11"/>
-      <c r="AY92" s="9"/>
+      <c r="AY92" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ92" s="9"/>
       <c r="BA92" s="11"/>
       <c r="BB92" s="9"/>
-      <c r="BC92" s="9"/>
+      <c r="BC92" s="9">
+        <v>1</v>
+      </c>
       <c r="BD92" s="11"/>
-      <c r="BE92" s="9"/>
+      <c r="BE92" s="9">
+        <v>1</v>
+      </c>
       <c r="BF92" s="9"/>
       <c r="BG92" s="11"/>
       <c r="BH92" s="9"/>
-      <c r="BI92" s="9"/>
+      <c r="BI92" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ92" s="11"/>
-      <c r="BK92" s="9"/>
+      <c r="BK92" s="9">
+        <v>1</v>
+      </c>
       <c r="BL92" s="9"/>
       <c r="BM92" s="11"/>
       <c r="BN92" s="9"/>
@@ -12303,48 +12539,78 @@
       <c r="BP92" s="9"/>
       <c r="BQ92" s="9"/>
     </row>
-    <row r="93" spans="1:69" ht="16.5" thickBot="1">
+    <row r="93" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A93" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C93" s="4"/>
+      <c r="C93" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D93" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-      <c r="I93" s="9"/>
+      <c r="E93" s="4">
+        <v>5740</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I93" s="9">
+        <v>1</v>
+      </c>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
-      <c r="L93" s="9"/>
+      <c r="L93" s="9">
+        <v>1</v>
+      </c>
       <c r="M93" s="11"/>
-      <c r="N93" s="9"/>
+      <c r="N93" s="9">
+        <v>1</v>
+      </c>
       <c r="O93" s="9"/>
-      <c r="P93" s="9"/>
-      <c r="Q93" s="9"/>
+      <c r="P93" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q93" s="9">
+        <v>1</v>
+      </c>
       <c r="R93" s="9"/>
       <c r="S93" s="9"/>
       <c r="T93" s="11"/>
       <c r="U93" s="9"/>
       <c r="V93" s="9"/>
-      <c r="W93" s="9"/>
-      <c r="X93" s="9"/>
+      <c r="W93" s="9">
+        <v>1</v>
+      </c>
+      <c r="X93" s="9">
+        <v>1</v>
+      </c>
       <c r="Y93" s="11"/>
-      <c r="Z93" s="9"/>
+      <c r="Z93" s="9">
+        <v>1</v>
+      </c>
       <c r="AA93" s="9"/>
       <c r="AB93" s="9"/>
       <c r="AC93" s="9"/>
-      <c r="AD93" s="9"/>
+      <c r="AD93" s="9">
+        <v>1</v>
+      </c>
       <c r="AE93" s="9"/>
       <c r="AF93" s="11"/>
       <c r="AG93" s="9"/>
-      <c r="AH93" s="9"/>
+      <c r="AH93" s="9">
+        <v>1</v>
+      </c>
       <c r="AI93" s="11"/>
-      <c r="AJ93" s="9"/>
+      <c r="AJ93" s="9">
+        <v>1</v>
+      </c>
       <c r="AK93" s="9"/>
       <c r="AL93" s="9"/>
       <c r="AM93" s="9"/>
@@ -12357,21 +12623,33 @@
       <c r="AT93" s="9"/>
       <c r="AU93" s="9"/>
       <c r="AV93" s="9"/>
-      <c r="AW93" s="9"/>
+      <c r="AW93" s="9">
+        <v>1</v>
+      </c>
       <c r="AX93" s="11"/>
-      <c r="AY93" s="9"/>
+      <c r="AY93" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ93" s="9"/>
       <c r="BA93" s="11"/>
       <c r="BB93" s="9"/>
-      <c r="BC93" s="9"/>
+      <c r="BC93" s="9">
+        <v>1</v>
+      </c>
       <c r="BD93" s="11"/>
-      <c r="BE93" s="9"/>
+      <c r="BE93" s="9">
+        <v>1</v>
+      </c>
       <c r="BF93" s="9"/>
       <c r="BG93" s="11"/>
-      <c r="BH93" s="9"/>
+      <c r="BH93" s="9">
+        <v>1</v>
+      </c>
       <c r="BI93" s="9"/>
       <c r="BJ93" s="11"/>
-      <c r="BK93" s="9"/>
+      <c r="BK93" s="9">
+        <v>1</v>
+      </c>
       <c r="BL93" s="9"/>
       <c r="BM93" s="11"/>
       <c r="BN93" s="9"/>
@@ -12379,48 +12657,78 @@
       <c r="BP93" s="9"/>
       <c r="BQ93" s="9"/>
     </row>
-    <row r="94" spans="1:69" ht="16.5" thickBot="1">
+    <row r="94" spans="1:69" ht="32.25" hidden="1" thickBot="1">
       <c r="A94" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C94" s="4"/>
+      <c r="C94" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D94" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="I94" s="9"/>
+      <c r="E94" s="4">
+        <v>1047420</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="I94" s="9">
+        <v>1</v>
+      </c>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
-      <c r="L94" s="9"/>
+      <c r="L94" s="9">
+        <v>1</v>
+      </c>
       <c r="M94" s="11"/>
       <c r="N94" s="9"/>
       <c r="O94" s="9"/>
-      <c r="P94" s="9"/>
+      <c r="P94" s="9">
+        <v>1</v>
+      </c>
       <c r="Q94" s="9"/>
-      <c r="R94" s="9"/>
+      <c r="R94" s="9">
+        <v>1</v>
+      </c>
       <c r="S94" s="9"/>
       <c r="T94" s="11"/>
       <c r="U94" s="9"/>
-      <c r="V94" s="9"/>
+      <c r="V94" s="9">
+        <v>1</v>
+      </c>
       <c r="W94" s="9"/>
-      <c r="X94" s="9"/>
+      <c r="X94" s="9">
+        <v>1</v>
+      </c>
       <c r="Y94" s="11"/>
-      <c r="Z94" s="9"/>
-      <c r="AA94" s="9"/>
+      <c r="Z94" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA94" s="9">
+        <v>1</v>
+      </c>
       <c r="AB94" s="9"/>
       <c r="AC94" s="9"/>
-      <c r="AD94" s="9"/>
+      <c r="AD94" s="9">
+        <v>1</v>
+      </c>
       <c r="AE94" s="9"/>
       <c r="AF94" s="11"/>
-      <c r="AG94" s="9"/>
+      <c r="AG94" s="9">
+        <v>1</v>
+      </c>
       <c r="AH94" s="9"/>
       <c r="AI94" s="11"/>
-      <c r="AJ94" s="9"/>
+      <c r="AJ94" s="9">
+        <v>1</v>
+      </c>
       <c r="AK94" s="9"/>
       <c r="AL94" s="9"/>
       <c r="AM94" s="9"/>
@@ -12432,22 +12740,34 @@
       <c r="AS94" s="9"/>
       <c r="AT94" s="9"/>
       <c r="AU94" s="9"/>
-      <c r="AV94" s="9"/>
+      <c r="AV94" s="9">
+        <v>1</v>
+      </c>
       <c r="AW94" s="9"/>
       <c r="AX94" s="11"/>
-      <c r="AY94" s="9"/>
+      <c r="AY94" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ94" s="9"/>
       <c r="BA94" s="11"/>
-      <c r="BB94" s="9"/>
+      <c r="BB94" s="9">
+        <v>1</v>
+      </c>
       <c r="BC94" s="9"/>
       <c r="BD94" s="11"/>
-      <c r="BE94" s="9"/>
+      <c r="BE94" s="9">
+        <v>1</v>
+      </c>
       <c r="BF94" s="9"/>
       <c r="BG94" s="11"/>
-      <c r="BH94" s="9"/>
+      <c r="BH94" s="9">
+        <v>1</v>
+      </c>
       <c r="BI94" s="9"/>
       <c r="BJ94" s="11"/>
-      <c r="BK94" s="9"/>
+      <c r="BK94" s="9">
+        <v>1</v>
+      </c>
       <c r="BL94" s="9"/>
       <c r="BM94" s="11"/>
       <c r="BN94" s="9"/>
@@ -12455,27 +12775,43 @@
       <c r="BP94" s="9"/>
       <c r="BQ94" s="9"/>
     </row>
-    <row r="95" spans="1:69" ht="16.5" thickBot="1">
+    <row r="95" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A95" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C95" s="4"/>
+      <c r="C95" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D95" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
-      <c r="I95" s="9"/>
+      <c r="E95" s="4">
+        <v>105964</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I95" s="9">
+        <v>1</v>
+      </c>
       <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
+      <c r="K95" s="9">
+        <v>1</v>
+      </c>
+      <c r="L95" s="9">
+        <v>1</v>
+      </c>
       <c r="M95" s="11"/>
       <c r="N95" s="9"/>
-      <c r="O95" s="9"/>
+      <c r="O95" s="9">
+        <v>1</v>
+      </c>
       <c r="P95" s="9"/>
       <c r="Q95" s="9"/>
       <c r="R95" s="9"/>
@@ -12484,24 +12820,36 @@
       <c r="U95" s="9"/>
       <c r="V95" s="9"/>
       <c r="W95" s="9"/>
-      <c r="X95" s="9"/>
+      <c r="X95" s="9">
+        <v>1</v>
+      </c>
       <c r="Y95" s="11"/>
-      <c r="Z95" s="9"/>
+      <c r="Z95" s="9">
+        <v>1</v>
+      </c>
       <c r="AA95" s="9"/>
       <c r="AB95" s="9"/>
       <c r="AC95" s="9"/>
-      <c r="AD95" s="9"/>
+      <c r="AD95" s="9">
+        <v>1</v>
+      </c>
       <c r="AE95" s="9"/>
       <c r="AF95" s="11"/>
       <c r="AG95" s="9"/>
-      <c r="AH95" s="9"/>
+      <c r="AH95" s="9">
+        <v>1</v>
+      </c>
       <c r="AI95" s="11"/>
       <c r="AJ95" s="9"/>
       <c r="AK95" s="9"/>
-      <c r="AL95" s="9"/>
+      <c r="AL95" s="9">
+        <v>1</v>
+      </c>
       <c r="AM95" s="9"/>
       <c r="AN95" s="11"/>
-      <c r="AO95" s="9"/>
+      <c r="AO95" s="9">
+        <v>1</v>
+      </c>
       <c r="AP95" s="9"/>
       <c r="AQ95" s="9"/>
       <c r="AR95" s="11"/>
@@ -12509,18 +12857,28 @@
       <c r="AT95" s="9"/>
       <c r="AU95" s="9"/>
       <c r="AV95" s="9"/>
-      <c r="AW95" s="9"/>
+      <c r="AW95" s="9">
+        <v>1</v>
+      </c>
       <c r="AX95" s="11"/>
       <c r="AY95" s="9"/>
-      <c r="AZ95" s="9"/>
+      <c r="AZ95" s="9">
+        <v>1</v>
+      </c>
       <c r="BA95" s="11"/>
       <c r="BB95" s="9"/>
-      <c r="BC95" s="9"/>
+      <c r="BC95" s="9">
+        <v>1</v>
+      </c>
       <c r="BD95" s="11"/>
-      <c r="BE95" s="9"/>
+      <c r="BE95" s="9">
+        <v>1</v>
+      </c>
       <c r="BF95" s="9"/>
       <c r="BG95" s="11"/>
-      <c r="BH95" s="9"/>
+      <c r="BH95" s="9">
+        <v>1</v>
+      </c>
       <c r="BI95" s="9"/>
       <c r="BJ95" s="11"/>
       <c r="BK95" s="9"/>
@@ -12531,75 +12889,119 @@
       <c r="BP95" s="9"/>
       <c r="BQ95" s="9"/>
     </row>
-    <row r="96" spans="1:69" ht="16.5" thickBot="1">
+    <row r="96" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A96" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C96" s="4"/>
+      <c r="C96" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D96" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4"/>
-      <c r="G96" s="4"/>
-      <c r="I96" s="9"/>
+      <c r="E96" s="4">
+        <v>10295</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="I96" s="9">
+        <v>1</v>
+      </c>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
-      <c r="L96" s="9"/>
+      <c r="L96" s="9">
+        <v>1</v>
+      </c>
       <c r="M96" s="11"/>
       <c r="N96" s="9"/>
-      <c r="O96" s="9"/>
+      <c r="O96" s="9">
+        <v>1</v>
+      </c>
       <c r="P96" s="9"/>
       <c r="Q96" s="9"/>
       <c r="R96" s="9"/>
       <c r="S96" s="9"/>
       <c r="T96" s="11"/>
-      <c r="U96" s="9"/>
-      <c r="V96" s="9"/>
+      <c r="U96" s="9">
+        <v>1</v>
+      </c>
+      <c r="V96" s="9">
+        <v>1</v>
+      </c>
       <c r="W96" s="9"/>
-      <c r="X96" s="9"/>
+      <c r="X96" s="9">
+        <v>1</v>
+      </c>
       <c r="Y96" s="11"/>
-      <c r="Z96" s="9"/>
-      <c r="AA96" s="9"/>
+      <c r="Z96" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA96" s="9">
+        <v>1</v>
+      </c>
       <c r="AB96" s="9"/>
       <c r="AC96" s="9"/>
-      <c r="AD96" s="9"/>
+      <c r="AD96" s="9">
+        <v>1</v>
+      </c>
       <c r="AE96" s="9"/>
       <c r="AF96" s="11"/>
       <c r="AG96" s="9"/>
-      <c r="AH96" s="9"/>
+      <c r="AH96" s="9">
+        <v>1</v>
+      </c>
       <c r="AI96" s="11"/>
       <c r="AJ96" s="9"/>
       <c r="AK96" s="9"/>
-      <c r="AL96" s="9"/>
+      <c r="AL96" s="9">
+        <v>1</v>
+      </c>
       <c r="AM96" s="9"/>
       <c r="AN96" s="11"/>
       <c r="AO96" s="9"/>
-      <c r="AP96" s="9"/>
+      <c r="AP96" s="9">
+        <v>1</v>
+      </c>
       <c r="AQ96" s="9"/>
       <c r="AR96" s="11"/>
       <c r="AS96" s="9"/>
       <c r="AT96" s="9"/>
       <c r="AU96" s="9"/>
       <c r="AV96" s="9"/>
-      <c r="AW96" s="9"/>
+      <c r="AW96" s="9">
+        <v>1</v>
+      </c>
       <c r="AX96" s="11"/>
-      <c r="AY96" s="9"/>
+      <c r="AY96" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ96" s="9"/>
       <c r="BA96" s="11"/>
       <c r="BB96" s="9"/>
-      <c r="BC96" s="9"/>
+      <c r="BC96" s="9">
+        <v>1</v>
+      </c>
       <c r="BD96" s="11"/>
-      <c r="BE96" s="9"/>
+      <c r="BE96" s="9">
+        <v>1</v>
+      </c>
       <c r="BF96" s="9"/>
       <c r="BG96" s="11"/>
-      <c r="BH96" s="9"/>
+      <c r="BH96" s="9">
+        <v>1</v>
+      </c>
       <c r="BI96" s="9"/>
       <c r="BJ96" s="11"/>
-      <c r="BK96" s="9"/>
+      <c r="BK96" s="9">
+        <v>1</v>
+      </c>
       <c r="BL96" s="9"/>
       <c r="BM96" s="11"/>
       <c r="BN96" s="9"/>
@@ -12607,27 +13009,43 @@
       <c r="BP96" s="9"/>
       <c r="BQ96" s="9"/>
     </row>
-    <row r="97" spans="1:69" ht="16.5" thickBot="1">
+    <row r="97" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A97" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C97" s="4"/>
+      <c r="C97" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D97" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="I97" s="9"/>
-      <c r="J97" s="9"/>
+      <c r="E97" s="4">
+        <v>513771</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I97" s="9">
+        <v>1</v>
+      </c>
+      <c r="J97" s="9">
+        <v>1</v>
+      </c>
       <c r="K97" s="9"/>
-      <c r="L97" s="9"/>
+      <c r="L97" s="9">
+        <v>1</v>
+      </c>
       <c r="M97" s="11"/>
       <c r="N97" s="9"/>
-      <c r="O97" s="9"/>
+      <c r="O97" s="9">
+        <v>1</v>
+      </c>
       <c r="P97" s="9"/>
       <c r="Q97" s="9"/>
       <c r="R97" s="9"/>
@@ -12635,25 +13053,39 @@
       <c r="T97" s="11"/>
       <c r="U97" s="9"/>
       <c r="V97" s="9"/>
-      <c r="W97" s="9"/>
-      <c r="X97" s="9"/>
+      <c r="W97" s="9">
+        <v>1</v>
+      </c>
+      <c r="X97" s="9">
+        <v>1</v>
+      </c>
       <c r="Y97" s="11"/>
-      <c r="Z97" s="9"/>
-      <c r="AA97" s="9"/>
+      <c r="Z97" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA97" s="9">
+        <v>1</v>
+      </c>
       <c r="AB97" s="9"/>
       <c r="AC97" s="9"/>
       <c r="AD97" s="9"/>
       <c r="AE97" s="9"/>
       <c r="AF97" s="11"/>
       <c r="AG97" s="9"/>
-      <c r="AH97" s="9"/>
+      <c r="AH97" s="9">
+        <v>1</v>
+      </c>
       <c r="AI97" s="11"/>
       <c r="AJ97" s="9"/>
       <c r="AK97" s="9"/>
-      <c r="AL97" s="9"/>
+      <c r="AL97" s="9">
+        <v>1</v>
+      </c>
       <c r="AM97" s="9"/>
       <c r="AN97" s="11"/>
-      <c r="AO97" s="9"/>
+      <c r="AO97" s="9">
+        <v>1</v>
+      </c>
       <c r="AP97" s="9"/>
       <c r="AQ97" s="9"/>
       <c r="AR97" s="11"/>
@@ -12661,21 +13093,33 @@
       <c r="AT97" s="9"/>
       <c r="AU97" s="9"/>
       <c r="AV97" s="9"/>
-      <c r="AW97" s="9"/>
+      <c r="AW97" s="9">
+        <v>1</v>
+      </c>
       <c r="AX97" s="11"/>
       <c r="AY97" s="9"/>
-      <c r="AZ97" s="9"/>
+      <c r="AZ97" s="9">
+        <v>1</v>
+      </c>
       <c r="BA97" s="11"/>
       <c r="BB97" s="9"/>
-      <c r="BC97" s="9"/>
+      <c r="BC97" s="9">
+        <v>1</v>
+      </c>
       <c r="BD97" s="11"/>
-      <c r="BE97" s="9"/>
+      <c r="BE97" s="9">
+        <v>1</v>
+      </c>
       <c r="BF97" s="9"/>
       <c r="BG97" s="11"/>
       <c r="BH97" s="9"/>
-      <c r="BI97" s="9"/>
+      <c r="BI97" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ97" s="11"/>
-      <c r="BK97" s="9"/>
+      <c r="BK97" s="9">
+        <v>1</v>
+      </c>
       <c r="BL97" s="9"/>
       <c r="BM97" s="11"/>
       <c r="BN97" s="9"/>
@@ -12683,48 +13127,76 @@
       <c r="BP97" s="9"/>
       <c r="BQ97" s="9"/>
     </row>
-    <row r="98" spans="1:69" ht="16.5" thickBot="1">
+    <row r="98" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A98" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C98" s="4"/>
+      <c r="C98" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D98" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="E98" s="4">
+        <v>4286978</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
+      <c r="L98" s="9">
+        <v>1</v>
+      </c>
       <c r="M98" s="11"/>
       <c r="N98" s="9"/>
       <c r="O98" s="9"/>
-      <c r="P98" s="9"/>
+      <c r="P98" s="9">
+        <v>1</v>
+      </c>
       <c r="Q98" s="9"/>
-      <c r="R98" s="9"/>
+      <c r="R98" s="9">
+        <v>1</v>
+      </c>
       <c r="S98" s="9"/>
       <c r="T98" s="11"/>
       <c r="U98" s="9"/>
-      <c r="V98" s="9"/>
+      <c r="V98" s="9">
+        <v>1</v>
+      </c>
       <c r="W98" s="9"/>
-      <c r="X98" s="9"/>
+      <c r="X98" s="9">
+        <v>1</v>
+      </c>
       <c r="Y98" s="11"/>
-      <c r="Z98" s="9"/>
+      <c r="Z98" s="9">
+        <v>1</v>
+      </c>
       <c r="AA98" s="9"/>
       <c r="AB98" s="9"/>
-      <c r="AC98" s="9"/>
-      <c r="AD98" s="9"/>
+      <c r="AC98" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD98" s="9">
+        <v>1</v>
+      </c>
       <c r="AE98" s="9"/>
       <c r="AF98" s="11"/>
       <c r="AG98" s="9"/>
-      <c r="AH98" s="9"/>
+      <c r="AH98" s="9">
+        <v>1</v>
+      </c>
       <c r="AI98" s="11"/>
-      <c r="AJ98" s="9"/>
+      <c r="AJ98" s="9">
+        <v>1</v>
+      </c>
       <c r="AK98" s="9"/>
       <c r="AL98" s="9"/>
       <c r="AM98" s="9"/>
@@ -12736,22 +13208,34 @@
       <c r="AS98" s="9"/>
       <c r="AT98" s="9"/>
       <c r="AU98" s="9"/>
-      <c r="AV98" s="9"/>
+      <c r="AV98" s="9">
+        <v>1</v>
+      </c>
       <c r="AW98" s="9"/>
       <c r="AX98" s="11"/>
-      <c r="AY98" s="9"/>
+      <c r="AY98" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ98" s="9"/>
       <c r="BA98" s="11"/>
       <c r="BB98" s="9"/>
-      <c r="BC98" s="9"/>
+      <c r="BC98" s="9">
+        <v>1</v>
+      </c>
       <c r="BD98" s="11"/>
-      <c r="BE98" s="9"/>
+      <c r="BE98" s="9">
+        <v>1</v>
+      </c>
       <c r="BF98" s="9"/>
       <c r="BG98" s="11"/>
-      <c r="BH98" s="9"/>
+      <c r="BH98" s="9">
+        <v>1</v>
+      </c>
       <c r="BI98" s="9"/>
       <c r="BJ98" s="11"/>
-      <c r="BK98" s="9"/>
+      <c r="BK98" s="9">
+        <v>1</v>
+      </c>
       <c r="BL98" s="9"/>
       <c r="BM98" s="11"/>
       <c r="BN98" s="9"/>
@@ -12759,27 +13243,39 @@
       <c r="BP98" s="9"/>
       <c r="BQ98" s="9"/>
     </row>
-    <row r="99" spans="1:69" ht="16.5" thickBot="1">
+    <row r="99" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A99" s="3" t="s">
         <v>201</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C99" s="4"/>
+      <c r="C99" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D99" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="E99" s="4">
+        <v>4901</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>543</v>
+      </c>
       <c r="I99" s="9"/>
-      <c r="J99" s="9"/>
+      <c r="J99" s="9">
+        <v>1</v>
+      </c>
       <c r="K99" s="9"/>
       <c r="L99" s="9"/>
       <c r="M99" s="11"/>
       <c r="N99" s="9"/>
-      <c r="O99" s="9"/>
+      <c r="O99" s="9">
+        <v>1</v>
+      </c>
       <c r="P99" s="9"/>
       <c r="Q99" s="9"/>
       <c r="R99" s="9"/>
@@ -12788,24 +13284,36 @@
       <c r="U99" s="9"/>
       <c r="V99" s="9"/>
       <c r="W99" s="9"/>
-      <c r="X99" s="9"/>
+      <c r="X99" s="9">
+        <v>1</v>
+      </c>
       <c r="Y99" s="11"/>
-      <c r="Z99" s="9"/>
-      <c r="AA99" s="9"/>
+      <c r="Z99" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA99" s="9">
+        <v>1</v>
+      </c>
       <c r="AB99" s="9"/>
       <c r="AC99" s="9"/>
       <c r="AD99" s="9"/>
       <c r="AE99" s="9"/>
       <c r="AF99" s="11"/>
       <c r="AG99" s="9"/>
-      <c r="AH99" s="9"/>
+      <c r="AH99" s="9">
+        <v>1</v>
+      </c>
       <c r="AI99" s="11"/>
       <c r="AJ99" s="9"/>
       <c r="AK99" s="9"/>
-      <c r="AL99" s="9"/>
+      <c r="AL99" s="9">
+        <v>1</v>
+      </c>
       <c r="AM99" s="9"/>
       <c r="AN99" s="11"/>
-      <c r="AO99" s="9"/>
+      <c r="AO99" s="9">
+        <v>1</v>
+      </c>
       <c r="AP99" s="9"/>
       <c r="AQ99" s="9"/>
       <c r="AR99" s="11"/>
@@ -12813,21 +13321,33 @@
       <c r="AT99" s="9"/>
       <c r="AU99" s="9"/>
       <c r="AV99" s="9"/>
-      <c r="AW99" s="9"/>
+      <c r="AW99" s="9">
+        <v>1</v>
+      </c>
       <c r="AX99" s="11"/>
       <c r="AY99" s="9"/>
-      <c r="AZ99" s="9"/>
+      <c r="AZ99" s="9">
+        <v>1</v>
+      </c>
       <c r="BA99" s="11"/>
       <c r="BB99" s="9"/>
-      <c r="BC99" s="9"/>
+      <c r="BC99" s="9">
+        <v>1</v>
+      </c>
       <c r="BD99" s="11"/>
       <c r="BE99" s="9"/>
-      <c r="BF99" s="9"/>
+      <c r="BF99" s="9">
+        <v>1</v>
+      </c>
       <c r="BG99" s="11"/>
       <c r="BH99" s="9"/>
-      <c r="BI99" s="9"/>
+      <c r="BI99" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ99" s="11"/>
-      <c r="BK99" s="9"/>
+      <c r="BK99" s="9">
+        <v>1</v>
+      </c>
       <c r="BL99" s="9"/>
       <c r="BM99" s="11"/>
       <c r="BN99" s="9"/>
@@ -12835,27 +13355,41 @@
       <c r="BP99" s="9"/>
       <c r="BQ99" s="9"/>
     </row>
-    <row r="100" spans="1:69" ht="16.5" thickBot="1">
+    <row r="100" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A100" s="3" t="s">
         <v>203</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C100" s="4"/>
+      <c r="C100" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D100" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="I100" s="9"/>
+      <c r="E100" s="4">
+        <v>422</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="I100" s="9">
+        <v>1</v>
+      </c>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
-      <c r="L100" s="9"/>
+      <c r="L100" s="9">
+        <v>1</v>
+      </c>
       <c r="M100" s="11"/>
       <c r="N100" s="9"/>
-      <c r="O100" s="9"/>
+      <c r="O100" s="9">
+        <v>1</v>
+      </c>
       <c r="P100" s="9"/>
       <c r="Q100" s="9"/>
       <c r="R100" s="9"/>
@@ -12863,20 +13397,32 @@
       <c r="T100" s="11"/>
       <c r="U100" s="9"/>
       <c r="V100" s="9"/>
-      <c r="W100" s="9"/>
-      <c r="X100" s="9"/>
+      <c r="W100" s="9">
+        <v>1</v>
+      </c>
+      <c r="X100" s="9">
+        <v>1</v>
+      </c>
       <c r="Y100" s="11"/>
-      <c r="Z100" s="9"/>
+      <c r="Z100" s="9">
+        <v>1</v>
+      </c>
       <c r="AA100" s="9"/>
-      <c r="AB100" s="9"/>
+      <c r="AB100" s="9">
+        <v>1</v>
+      </c>
       <c r="AC100" s="9"/>
       <c r="AD100" s="9"/>
       <c r="AE100" s="9"/>
       <c r="AF100" s="11"/>
       <c r="AG100" s="9"/>
-      <c r="AH100" s="9"/>
+      <c r="AH100" s="9">
+        <v>1</v>
+      </c>
       <c r="AI100" s="11"/>
-      <c r="AJ100" s="9"/>
+      <c r="AJ100" s="9">
+        <v>1</v>
+      </c>
       <c r="AK100" s="9"/>
       <c r="AL100" s="9"/>
       <c r="AM100" s="9"/>
@@ -12889,21 +13435,33 @@
       <c r="AT100" s="9"/>
       <c r="AU100" s="9"/>
       <c r="AV100" s="9"/>
-      <c r="AW100" s="9"/>
+      <c r="AW100" s="9">
+        <v>1</v>
+      </c>
       <c r="AX100" s="11"/>
       <c r="AY100" s="9"/>
-      <c r="AZ100" s="9"/>
+      <c r="AZ100" s="9">
+        <v>1</v>
+      </c>
       <c r="BA100" s="11"/>
-      <c r="BB100" s="9"/>
+      <c r="BB100" s="9">
+        <v>1</v>
+      </c>
       <c r="BC100" s="9"/>
       <c r="BD100" s="11"/>
-      <c r="BE100" s="9"/>
+      <c r="BE100" s="9">
+        <v>1</v>
+      </c>
       <c r="BF100" s="9"/>
       <c r="BG100" s="11"/>
-      <c r="BH100" s="9"/>
+      <c r="BH100" s="9">
+        <v>1</v>
+      </c>
       <c r="BI100" s="9"/>
       <c r="BJ100" s="11"/>
-      <c r="BK100" s="9"/>
+      <c r="BK100" s="9">
+        <v>1</v>
+      </c>
       <c r="BL100" s="9"/>
       <c r="BM100" s="11"/>
       <c r="BN100" s="9"/>
@@ -12911,27 +13469,43 @@
       <c r="BP100" s="9"/>
       <c r="BQ100" s="9"/>
     </row>
-    <row r="101" spans="1:69" ht="16.5" thickBot="1">
+    <row r="101" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A101" s="3" t="s">
         <v>205</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C101" s="4"/>
+      <c r="C101" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D101" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="I101" s="9"/>
-      <c r="J101" s="9"/>
+      <c r="E101" s="4">
+        <v>213</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="I101" s="9">
+        <v>1</v>
+      </c>
+      <c r="J101" s="9">
+        <v>1</v>
+      </c>
       <c r="K101" s="9"/>
-      <c r="L101" s="9"/>
+      <c r="L101" s="9">
+        <v>1</v>
+      </c>
       <c r="M101" s="11"/>
       <c r="N101" s="9"/>
-      <c r="O101" s="9"/>
+      <c r="O101" s="9">
+        <v>1</v>
+      </c>
       <c r="P101" s="9"/>
       <c r="Q101" s="9"/>
       <c r="R101" s="9"/>
@@ -12940,19 +13514,31 @@
       <c r="U101" s="9"/>
       <c r="V101" s="9"/>
       <c r="W101" s="9"/>
-      <c r="X101" s="9"/>
+      <c r="X101" s="9">
+        <v>1</v>
+      </c>
       <c r="Y101" s="11"/>
-      <c r="Z101" s="9"/>
+      <c r="Z101" s="9">
+        <v>1</v>
+      </c>
       <c r="AA101" s="9"/>
-      <c r="AB101" s="9"/>
+      <c r="AB101" s="9">
+        <v>1</v>
+      </c>
       <c r="AC101" s="9"/>
       <c r="AD101" s="9"/>
-      <c r="AE101" s="9"/>
+      <c r="AE101" s="9">
+        <v>1</v>
+      </c>
       <c r="AF101" s="11"/>
       <c r="AG101" s="9"/>
-      <c r="AH101" s="9"/>
+      <c r="AH101" s="9">
+        <v>1</v>
+      </c>
       <c r="AI101" s="11"/>
-      <c r="AJ101" s="9"/>
+      <c r="AJ101" s="9">
+        <v>1</v>
+      </c>
       <c r="AK101" s="9"/>
       <c r="AL101" s="9"/>
       <c r="AM101" s="9"/>
@@ -12965,21 +13551,33 @@
       <c r="AT101" s="9"/>
       <c r="AU101" s="9"/>
       <c r="AV101" s="9"/>
-      <c r="AW101" s="9"/>
+      <c r="AW101" s="9">
+        <v>1</v>
+      </c>
       <c r="AX101" s="11"/>
-      <c r="AY101" s="9"/>
+      <c r="AY101" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ101" s="9"/>
       <c r="BA101" s="11"/>
-      <c r="BB101" s="9"/>
+      <c r="BB101" s="9">
+        <v>1</v>
+      </c>
       <c r="BC101" s="9"/>
       <c r="BD101" s="11"/>
-      <c r="BE101" s="9"/>
+      <c r="BE101" s="9">
+        <v>1</v>
+      </c>
       <c r="BF101" s="9"/>
       <c r="BG101" s="11"/>
-      <c r="BH101" s="9"/>
+      <c r="BH101" s="9">
+        <v>1</v>
+      </c>
       <c r="BI101" s="9"/>
       <c r="BJ101" s="11"/>
-      <c r="BK101" s="9"/>
+      <c r="BK101" s="9">
+        <v>1</v>
+      </c>
       <c r="BL101" s="9"/>
       <c r="BM101" s="11"/>
       <c r="BN101" s="9"/>
@@ -12988,19 +13586,19 @@
       <c r="BQ101" s="9"/>
     </row>
     <row r="102" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C102" s="4"/>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E102" s="4"/>
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
       <c r="I102" s="9"/>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
@@ -13064,19 +13662,19 @@
       <c r="BQ102" s="9"/>
     </row>
     <row r="103" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="15" t="s">
         <v>210</v>
       </c>
       <c r="C103" s="4"/>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="15"/>
       <c r="I103" s="9"/>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
@@ -13139,48 +13737,74 @@
       <c r="BP103" s="9"/>
       <c r="BQ103" s="9"/>
     </row>
-    <row r="104" spans="1:69" ht="16.5" thickBot="1">
+    <row r="104" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A104" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C104" s="4"/>
+      <c r="C104" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D104" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
+      <c r="E104" s="4">
+        <v>229</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>545</v>
+      </c>
       <c r="I104" s="9"/>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
+      <c r="L104" s="9">
+        <v>1</v>
+      </c>
       <c r="M104" s="11"/>
-      <c r="N104" s="9"/>
+      <c r="N104" s="9">
+        <v>1</v>
+      </c>
       <c r="O104" s="9"/>
       <c r="P104" s="9"/>
       <c r="Q104" s="9"/>
       <c r="R104" s="9"/>
-      <c r="S104" s="9"/>
+      <c r="S104" s="9">
+        <v>1</v>
+      </c>
       <c r="T104" s="11"/>
       <c r="U104" s="9"/>
-      <c r="V104" s="9"/>
+      <c r="V104" s="9">
+        <v>1</v>
+      </c>
       <c r="W104" s="9"/>
-      <c r="X104" s="9"/>
+      <c r="X104" s="9">
+        <v>1</v>
+      </c>
       <c r="Y104" s="11"/>
-      <c r="Z104" s="9"/>
+      <c r="Z104" s="9">
+        <v>1</v>
+      </c>
       <c r="AA104" s="9"/>
-      <c r="AB104" s="9"/>
+      <c r="AB104" s="9">
+        <v>1</v>
+      </c>
       <c r="AC104" s="9"/>
       <c r="AD104" s="9"/>
       <c r="AE104" s="9"/>
       <c r="AF104" s="11"/>
       <c r="AG104" s="9"/>
-      <c r="AH104" s="9"/>
+      <c r="AH104" s="9">
+        <v>1</v>
+      </c>
       <c r="AI104" s="11"/>
-      <c r="AJ104" s="9"/>
+      <c r="AJ104" s="9">
+        <v>1</v>
+      </c>
       <c r="AK104" s="9"/>
       <c r="AL104" s="9"/>
       <c r="AM104" s="9"/>
@@ -13189,25 +13813,37 @@
       <c r="AP104" s="9"/>
       <c r="AQ104" s="9"/>
       <c r="AR104" s="11"/>
-      <c r="AS104" s="9"/>
+      <c r="AS104" s="9">
+        <v>1</v>
+      </c>
       <c r="AT104" s="9"/>
       <c r="AU104" s="9"/>
       <c r="AV104" s="9"/>
       <c r="AW104" s="9"/>
       <c r="AX104" s="11"/>
       <c r="AY104" s="9"/>
-      <c r="AZ104" s="9"/>
+      <c r="AZ104" s="9">
+        <v>1</v>
+      </c>
       <c r="BA104" s="11"/>
-      <c r="BB104" s="9"/>
+      <c r="BB104" s="9">
+        <v>1</v>
+      </c>
       <c r="BC104" s="9"/>
       <c r="BD104" s="11"/>
-      <c r="BE104" s="9"/>
+      <c r="BE104" s="9">
+        <v>1</v>
+      </c>
       <c r="BF104" s="9"/>
       <c r="BG104" s="11"/>
-      <c r="BH104" s="9"/>
+      <c r="BH104" s="9">
+        <v>1</v>
+      </c>
       <c r="BI104" s="9"/>
       <c r="BJ104" s="11"/>
-      <c r="BK104" s="9"/>
+      <c r="BK104" s="9">
+        <v>1</v>
+      </c>
       <c r="BL104" s="9"/>
       <c r="BM104" s="11"/>
       <c r="BN104" s="9"/>
@@ -13215,48 +13851,78 @@
       <c r="BP104" s="9"/>
       <c r="BQ104" s="9"/>
     </row>
-    <row r="105" spans="1:69" ht="16.5" thickBot="1">
+    <row r="105" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A105" s="3" t="s">
         <v>213</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C105" s="4"/>
+      <c r="C105" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D105" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="I105" s="9"/>
+      <c r="E105" s="4">
+        <v>625</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="I105" s="9">
+        <v>1</v>
+      </c>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
-      <c r="L105" s="9"/>
+      <c r="L105" s="9">
+        <v>1</v>
+      </c>
       <c r="M105" s="11"/>
       <c r="N105" s="9"/>
       <c r="O105" s="9"/>
-      <c r="P105" s="9"/>
-      <c r="Q105" s="9"/>
+      <c r="P105" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q105" s="9">
+        <v>1</v>
+      </c>
       <c r="R105" s="9"/>
-      <c r="S105" s="9"/>
+      <c r="S105" s="9">
+        <v>1</v>
+      </c>
       <c r="T105" s="11"/>
       <c r="U105" s="9"/>
       <c r="V105" s="9"/>
       <c r="W105" s="9"/>
-      <c r="X105" s="9"/>
+      <c r="X105" s="9">
+        <v>1</v>
+      </c>
       <c r="Y105" s="11"/>
-      <c r="Z105" s="9"/>
+      <c r="Z105" s="9">
+        <v>1</v>
+      </c>
       <c r="AA105" s="9"/>
       <c r="AB105" s="9"/>
-      <c r="AC105" s="9"/>
+      <c r="AC105" s="9">
+        <v>1</v>
+      </c>
       <c r="AD105" s="9"/>
-      <c r="AE105" s="9"/>
+      <c r="AE105" s="9">
+        <v>1</v>
+      </c>
       <c r="AF105" s="11"/>
       <c r="AG105" s="9"/>
-      <c r="AH105" s="9"/>
+      <c r="AH105" s="9">
+        <v>1</v>
+      </c>
       <c r="AI105" s="11"/>
-      <c r="AJ105" s="9"/>
+      <c r="AJ105" s="9">
+        <v>1</v>
+      </c>
       <c r="AK105" s="9"/>
       <c r="AL105" s="9"/>
       <c r="AM105" s="9"/>
@@ -13268,22 +13934,34 @@
       <c r="AS105" s="9"/>
       <c r="AT105" s="9"/>
       <c r="AU105" s="9"/>
-      <c r="AV105" s="9"/>
+      <c r="AV105" s="9">
+        <v>1</v>
+      </c>
       <c r="AW105" s="9"/>
       <c r="AX105" s="11"/>
       <c r="AY105" s="9"/>
-      <c r="AZ105" s="9"/>
+      <c r="AZ105" s="9">
+        <v>1</v>
+      </c>
       <c r="BA105" s="11"/>
       <c r="BB105" s="9"/>
-      <c r="BC105" s="9"/>
+      <c r="BC105" s="9">
+        <v>1</v>
+      </c>
       <c r="BD105" s="11"/>
-      <c r="BE105" s="9"/>
+      <c r="BE105" s="9">
+        <v>1</v>
+      </c>
       <c r="BF105" s="9"/>
       <c r="BG105" s="11"/>
-      <c r="BH105" s="9"/>
+      <c r="BH105" s="9">
+        <v>1</v>
+      </c>
       <c r="BI105" s="9"/>
       <c r="BJ105" s="11"/>
-      <c r="BK105" s="9"/>
+      <c r="BK105" s="9">
+        <v>1</v>
+      </c>
       <c r="BL105" s="9"/>
       <c r="BM105" s="11"/>
       <c r="BN105" s="9"/>
@@ -13291,38 +13969,56 @@
       <c r="BP105" s="9"/>
       <c r="BQ105" s="9"/>
     </row>
-    <row r="106" spans="1:69" ht="16.5" thickBot="1">
+    <row r="106" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A106" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C106" s="4"/>
+      <c r="C106" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D106" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
+      <c r="E106" s="4">
+        <v>2779</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>536</v>
+      </c>
       <c r="I106" s="9"/>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
-      <c r="L106" s="9"/>
+      <c r="L106" s="9">
+        <v>1</v>
+      </c>
       <c r="M106" s="11"/>
-      <c r="N106" s="9"/>
+      <c r="N106" s="9">
+        <v>1</v>
+      </c>
       <c r="O106" s="9"/>
       <c r="P106" s="9"/>
       <c r="Q106" s="9"/>
       <c r="R106" s="9"/>
-      <c r="S106" s="9"/>
+      <c r="S106" s="9">
+        <v>1</v>
+      </c>
       <c r="T106" s="11"/>
       <c r="U106" s="9"/>
       <c r="V106" s="9"/>
       <c r="W106" s="9"/>
-      <c r="X106" s="9"/>
+      <c r="X106" s="9">
+        <v>1</v>
+      </c>
       <c r="Y106" s="11"/>
-      <c r="Z106" s="9"/>
+      <c r="Z106" s="9">
+        <v>1</v>
+      </c>
       <c r="AA106" s="9"/>
       <c r="AB106" s="9"/>
       <c r="AC106" s="9"/>
@@ -13330,36 +14026,54 @@
       <c r="AE106" s="9"/>
       <c r="AF106" s="11"/>
       <c r="AG106" s="9"/>
-      <c r="AH106" s="9"/>
+      <c r="AH106" s="9">
+        <v>1</v>
+      </c>
       <c r="AI106" s="11"/>
       <c r="AJ106" s="9"/>
       <c r="AK106" s="9"/>
-      <c r="AL106" s="9"/>
+      <c r="AL106" s="9">
+        <v>1</v>
+      </c>
       <c r="AM106" s="9"/>
       <c r="AN106" s="11"/>
       <c r="AO106" s="9"/>
-      <c r="AP106" s="9"/>
+      <c r="AP106" s="9">
+        <v>1</v>
+      </c>
       <c r="AQ106" s="9"/>
       <c r="AR106" s="11"/>
-      <c r="AS106" s="9"/>
+      <c r="AS106" s="9">
+        <v>1</v>
+      </c>
       <c r="AT106" s="9"/>
       <c r="AU106" s="9"/>
       <c r="AV106" s="9"/>
       <c r="AW106" s="9"/>
       <c r="AX106" s="11"/>
       <c r="AY106" s="9"/>
-      <c r="AZ106" s="9"/>
+      <c r="AZ106" s="9">
+        <v>1</v>
+      </c>
       <c r="BA106" s="11"/>
       <c r="BB106" s="9"/>
-      <c r="BC106" s="9"/>
+      <c r="BC106" s="9">
+        <v>1</v>
+      </c>
       <c r="BD106" s="11"/>
-      <c r="BE106" s="9"/>
+      <c r="BE106" s="9">
+        <v>1</v>
+      </c>
       <c r="BF106" s="9"/>
       <c r="BG106" s="11"/>
-      <c r="BH106" s="9"/>
+      <c r="BH106" s="9">
+        <v>1</v>
+      </c>
       <c r="BI106" s="9"/>
       <c r="BJ106" s="11"/>
-      <c r="BK106" s="9"/>
+      <c r="BK106" s="9">
+        <v>1</v>
+      </c>
       <c r="BL106" s="9"/>
       <c r="BM106" s="11"/>
       <c r="BN106" s="9"/>
@@ -13367,48 +14081,74 @@
       <c r="BP106" s="9"/>
       <c r="BQ106" s="9"/>
     </row>
-    <row r="107" spans="1:69" ht="16.5" thickBot="1">
+    <row r="107" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A107" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C107" s="4"/>
+      <c r="C107" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D107" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
+      <c r="E107" s="4">
+        <v>7922</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I107" s="9"/>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
+      <c r="L107" s="9">
+        <v>1</v>
+      </c>
       <c r="M107" s="11"/>
-      <c r="N107" s="9"/>
+      <c r="N107" s="9">
+        <v>1</v>
+      </c>
       <c r="O107" s="9"/>
       <c r="P107" s="9"/>
       <c r="Q107" s="9"/>
       <c r="R107" s="9"/>
-      <c r="S107" s="9"/>
+      <c r="S107" s="9">
+        <v>1</v>
+      </c>
       <c r="T107" s="11"/>
       <c r="U107" s="9"/>
       <c r="V107" s="9"/>
       <c r="W107" s="9"/>
-      <c r="X107" s="9"/>
+      <c r="X107" s="9">
+        <v>1</v>
+      </c>
       <c r="Y107" s="11"/>
-      <c r="Z107" s="9"/>
+      <c r="Z107" s="9">
+        <v>1</v>
+      </c>
       <c r="AA107" s="9"/>
-      <c r="AB107" s="9"/>
+      <c r="AB107" s="9">
+        <v>1</v>
+      </c>
       <c r="AC107" s="9"/>
-      <c r="AD107" s="9"/>
+      <c r="AD107" s="9">
+        <v>1</v>
+      </c>
       <c r="AE107" s="9"/>
       <c r="AF107" s="11"/>
       <c r="AG107" s="9"/>
-      <c r="AH107" s="9"/>
+      <c r="AH107" s="9">
+        <v>1</v>
+      </c>
       <c r="AI107" s="11"/>
-      <c r="AJ107" s="9"/>
+      <c r="AJ107" s="9">
+        <v>1</v>
+      </c>
       <c r="AK107" s="9"/>
       <c r="AL107" s="9"/>
       <c r="AM107" s="9"/>
@@ -13417,25 +14157,37 @@
       <c r="AP107" s="9"/>
       <c r="AQ107" s="9"/>
       <c r="AR107" s="11"/>
-      <c r="AS107" s="9"/>
+      <c r="AS107" s="9">
+        <v>1</v>
+      </c>
       <c r="AT107" s="9"/>
       <c r="AU107" s="9"/>
       <c r="AV107" s="9"/>
       <c r="AW107" s="9"/>
       <c r="AX107" s="11"/>
       <c r="AY107" s="9"/>
-      <c r="AZ107" s="9"/>
+      <c r="AZ107" s="9">
+        <v>1</v>
+      </c>
       <c r="BA107" s="11"/>
       <c r="BB107" s="9"/>
-      <c r="BC107" s="9"/>
+      <c r="BC107" s="9">
+        <v>1</v>
+      </c>
       <c r="BD107" s="11"/>
-      <c r="BE107" s="9"/>
+      <c r="BE107" s="9">
+        <v>1</v>
+      </c>
       <c r="BF107" s="9"/>
       <c r="BG107" s="11"/>
-      <c r="BH107" s="9"/>
+      <c r="BH107" s="9">
+        <v>1</v>
+      </c>
       <c r="BI107" s="9"/>
       <c r="BJ107" s="11"/>
-      <c r="BK107" s="9"/>
+      <c r="BK107" s="9">
+        <v>1</v>
+      </c>
       <c r="BL107" s="9"/>
       <c r="BM107" s="11"/>
       <c r="BN107" s="9"/>
@@ -13443,75 +14195,123 @@
       <c r="BP107" s="9"/>
       <c r="BQ107" s="9"/>
     </row>
-    <row r="108" spans="1:69" ht="16.5" thickBot="1">
+    <row r="108" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A108" s="3" t="s">
         <v>219</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C108" s="4"/>
+      <c r="C108" s="4" t="s">
+        <v>562</v>
+      </c>
       <c r="D108" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="I108" s="9"/>
-      <c r="J108" s="9"/>
+      <c r="E108" s="4">
+        <v>36584</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="I108" s="9">
+        <v>1</v>
+      </c>
+      <c r="J108" s="9">
+        <v>1</v>
+      </c>
       <c r="K108" s="9"/>
-      <c r="L108" s="9"/>
+      <c r="L108" s="9">
+        <v>1</v>
+      </c>
       <c r="M108" s="11"/>
-      <c r="N108" s="9"/>
+      <c r="N108" s="9">
+        <v>1</v>
+      </c>
       <c r="O108" s="9"/>
-      <c r="P108" s="9"/>
-      <c r="Q108" s="9"/>
+      <c r="P108" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q108" s="9">
+        <v>1</v>
+      </c>
       <c r="R108" s="9"/>
-      <c r="S108" s="9"/>
+      <c r="S108" s="9">
+        <v>1</v>
+      </c>
       <c r="T108" s="11"/>
       <c r="U108" s="9"/>
       <c r="V108" s="9"/>
       <c r="W108" s="9"/>
       <c r="X108" s="9"/>
       <c r="Y108" s="11"/>
-      <c r="Z108" s="9"/>
-      <c r="AA108" s="9"/>
-      <c r="AB108" s="9"/>
+      <c r="Z108" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA108" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB108" s="9">
+        <v>1</v>
+      </c>
       <c r="AC108" s="9"/>
       <c r="AD108" s="9"/>
       <c r="AE108" s="9"/>
       <c r="AF108" s="11"/>
-      <c r="AG108" s="9"/>
+      <c r="AG108" s="9">
+        <v>1</v>
+      </c>
       <c r="AH108" s="9"/>
       <c r="AI108" s="11"/>
       <c r="AJ108" s="9"/>
       <c r="AK108" s="9"/>
-      <c r="AL108" s="9"/>
+      <c r="AL108" s="9">
+        <v>1</v>
+      </c>
       <c r="AM108" s="9"/>
       <c r="AN108" s="11"/>
-      <c r="AO108" s="9"/>
+      <c r="AO108" s="9">
+        <v>1</v>
+      </c>
       <c r="AP108" s="9"/>
       <c r="AQ108" s="9"/>
       <c r="AR108" s="11"/>
-      <c r="AS108" s="9"/>
+      <c r="AS108" s="9">
+        <v>1</v>
+      </c>
       <c r="AT108" s="9"/>
       <c r="AU108" s="9"/>
-      <c r="AV108" s="9"/>
+      <c r="AV108" s="9">
+        <v>1</v>
+      </c>
       <c r="AW108" s="9"/>
       <c r="AX108" s="11"/>
-      <c r="AY108" s="9"/>
+      <c r="AY108" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ108" s="9"/>
       <c r="BA108" s="11"/>
-      <c r="BB108" s="9"/>
+      <c r="BB108" s="9">
+        <v>1</v>
+      </c>
       <c r="BC108" s="9"/>
       <c r="BD108" s="11"/>
-      <c r="BE108" s="9"/>
+      <c r="BE108" s="9">
+        <v>1</v>
+      </c>
       <c r="BF108" s="9"/>
       <c r="BG108" s="11"/>
-      <c r="BH108" s="9"/>
+      <c r="BH108" s="9">
+        <v>1</v>
+      </c>
       <c r="BI108" s="9"/>
       <c r="BJ108" s="11"/>
-      <c r="BK108" s="9"/>
+      <c r="BK108" s="9">
+        <v>1</v>
+      </c>
       <c r="BL108" s="9"/>
       <c r="BM108" s="11"/>
       <c r="BN108" s="9"/>
@@ -13520,10 +14320,10 @@
       <c r="BQ108" s="9"/>
     </row>
     <row r="109" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="30" t="s">
         <v>222</v>
       </c>
       <c r="C109" s="4"/>
@@ -21816,95 +22616,95 @@
       </c>
       <c r="I217">
         <f>SUM(I3:I215)</f>
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="J217">
         <f t="shared" ref="J217:BQ217" si="0">SUM(J3:J215)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K217">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L217">
         <f>SUM(L3:L215)</f>
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="N217">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="O217">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="P217">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="Q217">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R217">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S217">
         <f>SUM(S3:S215)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="U217">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="V217">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="W217">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="X217">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="Z217">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="AA217">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="AB217">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="AC217">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AD217">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="AE217">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AG217">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AH217">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="AJ217">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="AK217">
         <f t="shared" si="0"/>
@@ -21912,7 +22712,7 @@
       </c>
       <c r="AL217">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="AM217">
         <f t="shared" si="0"/>
@@ -21920,11 +22720,11 @@
       </c>
       <c r="AO217">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AP217">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AQ217">
         <f t="shared" si="0"/>
@@ -21936,7 +22736,7 @@
       </c>
       <c r="AS217">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AT217">
         <f t="shared" si="0"/>
@@ -21948,23 +22748,23 @@
       </c>
       <c r="AV217">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="AW217">
         <f>SUM(AW3:AW215)</f>
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="AY217">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="AZ217">
         <f>SUM(AZ3:AZ215)</f>
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="BB217">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="BD217" s="12">
         <f t="shared" si="0"/>
@@ -21972,26 +22772,26 @@
       </c>
       <c r="BE217">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="BF217">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BG217" s="12" t="s">
         <v>482</v>
       </c>
       <c r="BH217">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="BI217">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="BK217">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="BL217">
         <f t="shared" si="0"/>
@@ -22045,4 +22845,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Task 2 - dodano "Produktywność"
</commit_message>
<xml_diff>
--- a/dane_aplikacji-zygol.xlsx
+++ b/dane_aplikacji-zygol.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="566">
   <si>
     <t>Id</t>
   </si>
@@ -1732,6 +1732,15 @@
   </si>
   <si>
     <t>15-11-2014</t>
+  </si>
+  <si>
+    <t>16-11-2014</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>3.3</t>
   </si>
 </sst>
 </file>
@@ -1999,7 +2008,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2096,11 +2104,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-42430672"/>
-        <c:axId val="-42426864"/>
+        <c:axId val="-656160624"/>
+        <c:axId val="-656167696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-42430672"/>
+        <c:axId val="-656160624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,7 +2151,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-42426864"/>
+        <c:crossAx val="-656167696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2151,7 +2159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-42426864"/>
+        <c:axId val="-656167696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2202,7 +2210,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-42430672"/>
+        <c:crossAx val="-656160624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3117,17 +3125,17 @@
   <dimension ref="A1:BQ218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+      <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="41.125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="15.75" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="14.75" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="5" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="15.25" customWidth="1"/>
     <col min="8" max="8" width="1.375" customWidth="1"/>
     <col min="9" max="12" width="3.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="1.125" style="12" customWidth="1"/>
@@ -3662,7 +3670,7 @@
       <c r="BP4" s="19"/>
       <c r="BQ4" s="19"/>
     </row>
-    <row r="5" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
+    <row r="5" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
@@ -4712,7 +4720,7 @@
       <c r="BP14" s="19"/>
       <c r="BQ14" s="19"/>
     </row>
-    <row r="15" spans="1:69" ht="16.5" thickBot="1">
+    <row r="15" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A15" s="14" t="s">
         <v>28</v>
       </c>
@@ -12344,7 +12352,7 @@
       <c r="BP90" s="9"/>
       <c r="BQ90" s="9"/>
     </row>
-    <row r="91" spans="1:69" ht="16.5" thickBot="1">
+    <row r="91" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A91" s="14" t="s">
         <v>184</v>
       </c>
@@ -13585,7 +13593,7 @@
       <c r="BP101" s="9"/>
       <c r="BQ101" s="9"/>
     </row>
-    <row r="102" spans="1:69" ht="16.5" thickBot="1">
+    <row r="102" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A102" s="14" t="s">
         <v>207</v>
       </c>
@@ -13661,7 +13669,7 @@
       <c r="BP102" s="9"/>
       <c r="BQ102" s="9"/>
     </row>
-    <row r="103" spans="1:69" ht="16.5" thickBot="1">
+    <row r="103" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A103" s="14" t="s">
         <v>209</v>
       </c>
@@ -14319,7 +14327,7 @@
       <c r="BP108" s="9"/>
       <c r="BQ108" s="9"/>
     </row>
-    <row r="109" spans="1:69" ht="16.5" thickBot="1">
+    <row r="109" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A109" s="29" t="s">
         <v>221</v>
       </c>
@@ -14395,7 +14403,7 @@
       <c r="BP109" s="9"/>
       <c r="BQ109" s="9"/>
     </row>
-    <row r="110" spans="1:69" ht="16.5" thickBot="1">
+    <row r="110" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A110" s="3" t="s">
         <v>224</v>
       </c>
@@ -14471,7 +14479,7 @@
       <c r="BP110" s="9"/>
       <c r="BQ110" s="9"/>
     </row>
-    <row r="111" spans="1:69" ht="16.5" thickBot="1">
+    <row r="111" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A111" s="3" t="s">
         <v>226</v>
       </c>
@@ -14547,7 +14555,7 @@
       <c r="BP111" s="9"/>
       <c r="BQ111" s="9"/>
     </row>
-    <row r="112" spans="1:69" ht="16.5" thickBot="1">
+    <row r="112" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A112" s="3" t="s">
         <v>228</v>
       </c>
@@ -14623,7 +14631,7 @@
       <c r="BP112" s="9"/>
       <c r="BQ112" s="9"/>
     </row>
-    <row r="113" spans="1:69" ht="16.5" thickBot="1">
+    <row r="113" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A113" s="3" t="s">
         <v>230</v>
       </c>
@@ -14699,7 +14707,7 @@
       <c r="BP113" s="9"/>
       <c r="BQ113" s="9"/>
     </row>
-    <row r="114" spans="1:69" ht="16.5" thickBot="1">
+    <row r="114" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A114" s="3" t="s">
         <v>232</v>
       </c>
@@ -14775,7 +14783,7 @@
       <c r="BP114" s="9"/>
       <c r="BQ114" s="9"/>
     </row>
-    <row r="115" spans="1:69" ht="16.5" thickBot="1">
+    <row r="115" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A115" s="3" t="s">
         <v>234</v>
       </c>
@@ -14851,7 +14859,7 @@
       <c r="BP115" s="9"/>
       <c r="BQ115" s="9"/>
     </row>
-    <row r="116" spans="1:69" ht="16.5" thickBot="1">
+    <row r="116" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A116" s="3" t="s">
         <v>235</v>
       </c>
@@ -14927,7 +14935,7 @@
       <c r="BP116" s="9"/>
       <c r="BQ116" s="9"/>
     </row>
-    <row r="117" spans="1:69" ht="16.5" thickBot="1">
+    <row r="117" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A117" s="3" t="s">
         <v>236</v>
       </c>
@@ -15003,7 +15011,7 @@
       <c r="BP117" s="9"/>
       <c r="BQ117" s="9"/>
     </row>
-    <row r="118" spans="1:69" ht="16.5" thickBot="1">
+    <row r="118" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A118" s="3" t="s">
         <v>238</v>
       </c>
@@ -15079,7 +15087,7 @@
       <c r="BP118" s="9"/>
       <c r="BQ118" s="9"/>
     </row>
-    <row r="119" spans="1:69" ht="16.5" thickBot="1">
+    <row r="119" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A119" s="3" t="s">
         <v>240</v>
       </c>
@@ -15155,7 +15163,7 @@
       <c r="BP119" s="9"/>
       <c r="BQ119" s="9"/>
     </row>
-    <row r="120" spans="1:69" ht="16.5" thickBot="1">
+    <row r="120" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A120" s="3" t="s">
         <v>242</v>
       </c>
@@ -15231,7 +15239,7 @@
       <c r="BP120" s="9"/>
       <c r="BQ120" s="9"/>
     </row>
-    <row r="121" spans="1:69" ht="16.5" thickBot="1">
+    <row r="121" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A121" s="3" t="s">
         <v>244</v>
       </c>
@@ -15307,7 +15315,7 @@
       <c r="BP121" s="9"/>
       <c r="BQ121" s="9"/>
     </row>
-    <row r="122" spans="1:69" ht="16.5" thickBot="1">
+    <row r="122" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A122" s="3" t="s">
         <v>246</v>
       </c>
@@ -15383,7 +15391,7 @@
       <c r="BP122" s="9"/>
       <c r="BQ122" s="9"/>
     </row>
-    <row r="123" spans="1:69" ht="16.5" thickBot="1">
+    <row r="123" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A123" s="3" t="s">
         <v>248</v>
       </c>
@@ -15459,7 +15467,7 @@
       <c r="BP123" s="9"/>
       <c r="BQ123" s="9"/>
     </row>
-    <row r="124" spans="1:69" ht="16.5" thickBot="1">
+    <row r="124" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A124" s="3" t="s">
         <v>250</v>
       </c>
@@ -15535,7 +15543,7 @@
       <c r="BP124" s="9"/>
       <c r="BQ124" s="9"/>
     </row>
-    <row r="125" spans="1:69" ht="16.5" thickBot="1">
+    <row r="125" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A125" s="3" t="s">
         <v>252</v>
       </c>
@@ -15611,7 +15619,7 @@
       <c r="BP125" s="9"/>
       <c r="BQ125" s="9"/>
     </row>
-    <row r="126" spans="1:69" ht="16.5" thickBot="1">
+    <row r="126" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A126" s="3" t="s">
         <v>254</v>
       </c>
@@ -15687,7 +15695,7 @@
       <c r="BP126" s="9"/>
       <c r="BQ126" s="9"/>
     </row>
-    <row r="127" spans="1:69" ht="16.5" thickBot="1">
+    <row r="127" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A127" s="3" t="s">
         <v>256</v>
       </c>
@@ -15763,7 +15771,7 @@
       <c r="BP127" s="9"/>
       <c r="BQ127" s="9"/>
     </row>
-    <row r="128" spans="1:69" ht="16.5" thickBot="1">
+    <row r="128" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A128" s="3" t="s">
         <v>258</v>
       </c>
@@ -15839,7 +15847,7 @@
       <c r="BP128" s="9"/>
       <c r="BQ128" s="9"/>
     </row>
-    <row r="129" spans="1:69" ht="32.25" thickBot="1">
+    <row r="129" spans="1:69" ht="32.25" hidden="1" thickBot="1">
       <c r="A129" s="3" t="s">
         <v>260</v>
       </c>
@@ -15915,53 +15923,83 @@
       <c r="BP129" s="9"/>
       <c r="BQ129" s="9"/>
     </row>
-    <row r="130" spans="1:69" ht="16.5" thickBot="1">
+    <row r="130" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A130" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C130" s="4"/>
+      <c r="C130" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D130" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E130" s="4"/>
-      <c r="F130" s="4"/>
-      <c r="G130" s="4"/>
+      <c r="E130" s="4">
+        <v>116711</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I130" s="9"/>
-      <c r="J130" s="9"/>
-      <c r="K130" s="9"/>
-      <c r="L130" s="9"/>
+      <c r="J130" s="9">
+        <v>1</v>
+      </c>
+      <c r="K130" s="9">
+        <v>1</v>
+      </c>
+      <c r="L130" s="9">
+        <v>1</v>
+      </c>
       <c r="M130" s="11"/>
       <c r="N130" s="9"/>
-      <c r="O130" s="9"/>
+      <c r="O130" s="9">
+        <v>1</v>
+      </c>
       <c r="P130" s="9"/>
       <c r="Q130" s="9"/>
       <c r="R130" s="9"/>
       <c r="S130" s="9"/>
       <c r="T130" s="11"/>
-      <c r="U130" s="9"/>
-      <c r="V130" s="9"/>
+      <c r="U130" s="9">
+        <v>1</v>
+      </c>
+      <c r="V130" s="9">
+        <v>1</v>
+      </c>
       <c r="W130" s="9"/>
       <c r="X130" s="9"/>
       <c r="Y130" s="11"/>
-      <c r="Z130" s="9"/>
-      <c r="AA130" s="9"/>
+      <c r="Z130" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA130" s="9">
+        <v>1</v>
+      </c>
       <c r="AB130" s="9"/>
       <c r="AC130" s="9"/>
       <c r="AD130" s="9"/>
       <c r="AE130" s="9"/>
       <c r="AF130" s="11"/>
-      <c r="AG130" s="9"/>
+      <c r="AG130" s="9">
+        <v>1</v>
+      </c>
       <c r="AH130" s="9"/>
       <c r="AI130" s="11"/>
       <c r="AJ130" s="9"/>
       <c r="AK130" s="9"/>
-      <c r="AL130" s="9"/>
+      <c r="AL130" s="9">
+        <v>1</v>
+      </c>
       <c r="AM130" s="9"/>
       <c r="AN130" s="11"/>
-      <c r="AO130" s="9"/>
+      <c r="AO130" s="9">
+        <v>1</v>
+      </c>
       <c r="AP130" s="9"/>
       <c r="AQ130" s="9"/>
       <c r="AR130" s="11"/>
@@ -15969,21 +16007,33 @@
       <c r="AT130" s="9"/>
       <c r="AU130" s="9"/>
       <c r="AV130" s="9"/>
-      <c r="AW130" s="9"/>
+      <c r="AW130" s="9">
+        <v>1</v>
+      </c>
       <c r="AX130" s="11"/>
-      <c r="AY130" s="9"/>
+      <c r="AY130" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ130" s="9"/>
       <c r="BA130" s="11"/>
-      <c r="BB130" s="9"/>
+      <c r="BB130" s="9">
+        <v>1</v>
+      </c>
       <c r="BC130" s="9"/>
       <c r="BD130" s="11"/>
-      <c r="BE130" s="9"/>
+      <c r="BE130" s="9">
+        <v>1</v>
+      </c>
       <c r="BF130" s="9"/>
       <c r="BG130" s="11"/>
-      <c r="BH130" s="9"/>
+      <c r="BH130" s="9">
+        <v>1</v>
+      </c>
       <c r="BI130" s="9"/>
       <c r="BJ130" s="11"/>
-      <c r="BK130" s="9"/>
+      <c r="BK130" s="9">
+        <v>1</v>
+      </c>
       <c r="BL130" s="9"/>
       <c r="BM130" s="11"/>
       <c r="BN130" s="9"/>
@@ -15991,48 +16041,78 @@
       <c r="BP130" s="9"/>
       <c r="BQ130" s="9"/>
     </row>
-    <row r="131" spans="1:69" ht="16.5" thickBot="1">
+    <row r="131" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A131" s="3" t="s">
         <v>265</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C131" s="4"/>
+      <c r="C131" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D131" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E131" s="4"/>
-      <c r="F131" s="4"/>
-      <c r="G131" s="4"/>
+      <c r="E131" s="4">
+        <v>1582651</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>536</v>
+      </c>
       <c r="I131" s="9"/>
       <c r="J131" s="9"/>
       <c r="K131" s="9"/>
-      <c r="L131" s="9"/>
+      <c r="L131" s="9">
+        <v>1</v>
+      </c>
       <c r="M131" s="11"/>
-      <c r="N131" s="9"/>
+      <c r="N131" s="9">
+        <v>1</v>
+      </c>
       <c r="O131" s="9"/>
-      <c r="P131" s="9"/>
+      <c r="P131" s="9">
+        <v>1</v>
+      </c>
       <c r="Q131" s="9"/>
       <c r="R131" s="9"/>
-      <c r="S131" s="9"/>
+      <c r="S131" s="9">
+        <v>1</v>
+      </c>
       <c r="T131" s="11"/>
       <c r="U131" s="9"/>
-      <c r="V131" s="9"/>
+      <c r="V131" s="9">
+        <v>1</v>
+      </c>
       <c r="W131" s="9"/>
-      <c r="X131" s="9"/>
+      <c r="X131" s="9">
+        <v>1</v>
+      </c>
       <c r="Y131" s="11"/>
-      <c r="Z131" s="9"/>
+      <c r="Z131" s="9">
+        <v>1</v>
+      </c>
       <c r="AA131" s="9"/>
-      <c r="AB131" s="9"/>
+      <c r="AB131" s="9">
+        <v>1</v>
+      </c>
       <c r="AC131" s="9"/>
-      <c r="AD131" s="9"/>
+      <c r="AD131" s="9">
+        <v>1</v>
+      </c>
       <c r="AE131" s="9"/>
       <c r="AF131" s="11"/>
-      <c r="AG131" s="9"/>
+      <c r="AG131" s="9">
+        <v>1</v>
+      </c>
       <c r="AH131" s="9"/>
       <c r="AI131" s="11"/>
-      <c r="AJ131" s="9"/>
+      <c r="AJ131" s="9">
+        <v>1</v>
+      </c>
       <c r="AK131" s="9"/>
       <c r="AL131" s="9"/>
       <c r="AM131" s="9"/>
@@ -16041,25 +16121,39 @@
       <c r="AP131" s="9"/>
       <c r="AQ131" s="9"/>
       <c r="AR131" s="11"/>
-      <c r="AS131" s="9"/>
+      <c r="AS131" s="9">
+        <v>1</v>
+      </c>
       <c r="AT131" s="9"/>
       <c r="AU131" s="9"/>
-      <c r="AV131" s="9"/>
+      <c r="AV131" s="9">
+        <v>1</v>
+      </c>
       <c r="AW131" s="9"/>
       <c r="AX131" s="11"/>
       <c r="AY131" s="9"/>
-      <c r="AZ131" s="9"/>
+      <c r="AZ131" s="9">
+        <v>1</v>
+      </c>
       <c r="BA131" s="11"/>
       <c r="BB131" s="9"/>
-      <c r="BC131" s="9"/>
+      <c r="BC131" s="9">
+        <v>1</v>
+      </c>
       <c r="BD131" s="11"/>
-      <c r="BE131" s="9"/>
+      <c r="BE131" s="9">
+        <v>1</v>
+      </c>
       <c r="BF131" s="9"/>
       <c r="BG131" s="11"/>
-      <c r="BH131" s="9"/>
+      <c r="BH131" s="9">
+        <v>1</v>
+      </c>
       <c r="BI131" s="9"/>
       <c r="BJ131" s="11"/>
-      <c r="BK131" s="9"/>
+      <c r="BK131" s="9">
+        <v>1</v>
+      </c>
       <c r="BL131" s="9"/>
       <c r="BM131" s="11"/>
       <c r="BN131" s="9"/>
@@ -16067,27 +16161,43 @@
       <c r="BP131" s="9"/>
       <c r="BQ131" s="9"/>
     </row>
-    <row r="132" spans="1:69" ht="16.5" thickBot="1">
+    <row r="132" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A132" s="3" t="s">
         <v>267</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C132" s="4"/>
+      <c r="C132" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D132" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
-      <c r="I132" s="9"/>
-      <c r="J132" s="9"/>
-      <c r="K132" s="9"/>
+      <c r="E132" s="4">
+        <v>539559</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G132" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="I132" s="9">
+        <v>1</v>
+      </c>
+      <c r="J132" s="9">
+        <v>1</v>
+      </c>
+      <c r="K132" s="9">
+        <v>1</v>
+      </c>
       <c r="L132" s="9"/>
       <c r="M132" s="11"/>
       <c r="N132" s="9"/>
-      <c r="O132" s="9"/>
+      <c r="O132" s="9">
+        <v>1</v>
+      </c>
       <c r="P132" s="9"/>
       <c r="Q132" s="9"/>
       <c r="R132" s="9"/>
@@ -16096,24 +16206,36 @@
       <c r="U132" s="9"/>
       <c r="V132" s="9"/>
       <c r="W132" s="9"/>
-      <c r="X132" s="9"/>
+      <c r="X132" s="9">
+        <v>1</v>
+      </c>
       <c r="Y132" s="11"/>
-      <c r="Z132" s="9"/>
+      <c r="Z132" s="9">
+        <v>1</v>
+      </c>
       <c r="AA132" s="9"/>
       <c r="AB132" s="9"/>
       <c r="AC132" s="9"/>
-      <c r="AD132" s="9"/>
+      <c r="AD132" s="9">
+        <v>1</v>
+      </c>
       <c r="AE132" s="9"/>
       <c r="AF132" s="11"/>
       <c r="AG132" s="9"/>
-      <c r="AH132" s="9"/>
+      <c r="AH132" s="9">
+        <v>1</v>
+      </c>
       <c r="AI132" s="11"/>
       <c r="AJ132" s="9"/>
       <c r="AK132" s="9"/>
-      <c r="AL132" s="9"/>
+      <c r="AL132" s="9">
+        <v>1</v>
+      </c>
       <c r="AM132" s="9"/>
       <c r="AN132" s="11"/>
-      <c r="AO132" s="9"/>
+      <c r="AO132" s="9">
+        <v>1</v>
+      </c>
       <c r="AP132" s="9"/>
       <c r="AQ132" s="9"/>
       <c r="AR132" s="11"/>
@@ -16121,21 +16243,33 @@
       <c r="AT132" s="9"/>
       <c r="AU132" s="9"/>
       <c r="AV132" s="9"/>
-      <c r="AW132" s="9"/>
+      <c r="AW132" s="9">
+        <v>1</v>
+      </c>
       <c r="AX132" s="11"/>
       <c r="AY132" s="9"/>
-      <c r="AZ132" s="9"/>
+      <c r="AZ132" s="9">
+        <v>1</v>
+      </c>
       <c r="BA132" s="11"/>
       <c r="BB132" s="9"/>
-      <c r="BC132" s="9"/>
+      <c r="BC132" s="9">
+        <v>1</v>
+      </c>
       <c r="BD132" s="11"/>
-      <c r="BE132" s="9"/>
+      <c r="BE132" s="9">
+        <v>1</v>
+      </c>
       <c r="BF132" s="9"/>
       <c r="BG132" s="11"/>
-      <c r="BH132" s="9"/>
+      <c r="BH132" s="9">
+        <v>1</v>
+      </c>
       <c r="BI132" s="9"/>
       <c r="BJ132" s="11"/>
-      <c r="BK132" s="9"/>
+      <c r="BK132" s="9">
+        <v>1</v>
+      </c>
       <c r="BL132" s="9"/>
       <c r="BM132" s="11"/>
       <c r="BN132" s="9"/>
@@ -16143,27 +16277,43 @@
       <c r="BP132" s="9"/>
       <c r="BQ132" s="9"/>
     </row>
-    <row r="133" spans="1:69" ht="16.5" thickBot="1">
+    <row r="133" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A133" s="3" t="s">
         <v>269</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C133" s="4"/>
+      <c r="C133" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D133" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E133" s="4"/>
-      <c r="F133" s="4"/>
-      <c r="G133" s="4"/>
-      <c r="I133" s="9"/>
+      <c r="E133" s="4">
+        <v>208684</v>
+      </c>
+      <c r="F133" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="G133" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I133" s="9">
+        <v>1</v>
+      </c>
       <c r="J133" s="9"/>
-      <c r="K133" s="9"/>
-      <c r="L133" s="9"/>
+      <c r="K133" s="9">
+        <v>1</v>
+      </c>
+      <c r="L133" s="9">
+        <v>1</v>
+      </c>
       <c r="M133" s="11"/>
       <c r="N133" s="9"/>
-      <c r="O133" s="9"/>
+      <c r="O133" s="9">
+        <v>1</v>
+      </c>
       <c r="P133" s="9"/>
       <c r="Q133" s="9"/>
       <c r="R133" s="9"/>
@@ -16171,25 +16321,39 @@
       <c r="T133" s="11"/>
       <c r="U133" s="9"/>
       <c r="V133" s="9"/>
-      <c r="W133" s="9"/>
+      <c r="W133" s="9">
+        <v>1</v>
+      </c>
       <c r="X133" s="9"/>
       <c r="Y133" s="11"/>
-      <c r="Z133" s="9"/>
+      <c r="Z133" s="9">
+        <v>1</v>
+      </c>
       <c r="AA133" s="9"/>
       <c r="AB133" s="9"/>
       <c r="AC133" s="9"/>
-      <c r="AD133" s="9"/>
-      <c r="AE133" s="9"/>
+      <c r="AD133" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE133" s="9">
+        <v>1</v>
+      </c>
       <c r="AF133" s="11"/>
       <c r="AG133" s="9"/>
-      <c r="AH133" s="9"/>
+      <c r="AH133" s="9">
+        <v>1</v>
+      </c>
       <c r="AI133" s="11"/>
       <c r="AJ133" s="9"/>
       <c r="AK133" s="9"/>
-      <c r="AL133" s="9"/>
+      <c r="AL133" s="9">
+        <v>1</v>
+      </c>
       <c r="AM133" s="9"/>
       <c r="AN133" s="11"/>
-      <c r="AO133" s="9"/>
+      <c r="AO133" s="9">
+        <v>1</v>
+      </c>
       <c r="AP133" s="9"/>
       <c r="AQ133" s="9"/>
       <c r="AR133" s="11"/>
@@ -16197,21 +16361,33 @@
       <c r="AT133" s="9"/>
       <c r="AU133" s="9"/>
       <c r="AV133" s="9"/>
-      <c r="AW133" s="9"/>
+      <c r="AW133" s="9">
+        <v>1</v>
+      </c>
       <c r="AX133" s="11"/>
       <c r="AY133" s="9"/>
-      <c r="AZ133" s="9"/>
+      <c r="AZ133" s="9">
+        <v>1</v>
+      </c>
       <c r="BA133" s="11"/>
       <c r="BB133" s="9"/>
-      <c r="BC133" s="9"/>
+      <c r="BC133" s="9">
+        <v>1</v>
+      </c>
       <c r="BD133" s="11"/>
-      <c r="BE133" s="9"/>
+      <c r="BE133" s="9">
+        <v>1</v>
+      </c>
       <c r="BF133" s="9"/>
       <c r="BG133" s="11"/>
       <c r="BH133" s="9"/>
-      <c r="BI133" s="9"/>
+      <c r="BI133" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ133" s="11"/>
-      <c r="BK133" s="9"/>
+      <c r="BK133" s="9">
+        <v>1</v>
+      </c>
       <c r="BL133" s="9"/>
       <c r="BM133" s="11"/>
       <c r="BN133" s="9"/>
@@ -16219,27 +16395,39 @@
       <c r="BP133" s="9"/>
       <c r="BQ133" s="9"/>
     </row>
-    <row r="134" spans="1:69" ht="16.5" thickBot="1">
+    <row r="134" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A134" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C134" s="4"/>
+      <c r="C134" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D134" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E134" s="4"/>
-      <c r="F134" s="4"/>
-      <c r="G134" s="4"/>
-      <c r="I134" s="9"/>
+      <c r="E134" s="4">
+        <v>220270</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G134" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I134" s="9">
+        <v>1</v>
+      </c>
       <c r="J134" s="9"/>
       <c r="K134" s="9"/>
       <c r="L134" s="9"/>
       <c r="M134" s="11"/>
       <c r="N134" s="9"/>
-      <c r="O134" s="9"/>
+      <c r="O134" s="9">
+        <v>1</v>
+      </c>
       <c r="P134" s="9"/>
       <c r="Q134" s="9"/>
       <c r="R134" s="9"/>
@@ -16247,25 +16435,41 @@
       <c r="T134" s="11"/>
       <c r="U134" s="9"/>
       <c r="V134" s="9"/>
-      <c r="W134" s="9"/>
-      <c r="X134" s="9"/>
+      <c r="W134" s="9">
+        <v>1</v>
+      </c>
+      <c r="X134" s="9">
+        <v>1</v>
+      </c>
       <c r="Y134" s="11"/>
-      <c r="Z134" s="9"/>
-      <c r="AA134" s="9"/>
+      <c r="Z134" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA134" s="9">
+        <v>1</v>
+      </c>
       <c r="AB134" s="9"/>
       <c r="AC134" s="9"/>
-      <c r="AD134" s="9"/>
+      <c r="AD134" s="9">
+        <v>1</v>
+      </c>
       <c r="AE134" s="9"/>
       <c r="AF134" s="11"/>
       <c r="AG134" s="9"/>
-      <c r="AH134" s="9"/>
+      <c r="AH134" s="9">
+        <v>1</v>
+      </c>
       <c r="AI134" s="11"/>
       <c r="AJ134" s="9"/>
       <c r="AK134" s="9"/>
-      <c r="AL134" s="9"/>
+      <c r="AL134" s="9">
+        <v>1</v>
+      </c>
       <c r="AM134" s="9"/>
       <c r="AN134" s="11"/>
-      <c r="AO134" s="9"/>
+      <c r="AO134" s="9">
+        <v>1</v>
+      </c>
       <c r="AP134" s="9"/>
       <c r="AQ134" s="9"/>
       <c r="AR134" s="11"/>
@@ -16273,21 +16477,33 @@
       <c r="AT134" s="9"/>
       <c r="AU134" s="9"/>
       <c r="AV134" s="9"/>
-      <c r="AW134" s="9"/>
+      <c r="AW134" s="9">
+        <v>1</v>
+      </c>
       <c r="AX134" s="11"/>
       <c r="AY134" s="9"/>
-      <c r="AZ134" s="9"/>
+      <c r="AZ134" s="9">
+        <v>1</v>
+      </c>
       <c r="BA134" s="11"/>
       <c r="BB134" s="9"/>
-      <c r="BC134" s="9"/>
+      <c r="BC134" s="9">
+        <v>1</v>
+      </c>
       <c r="BD134" s="11"/>
-      <c r="BE134" s="9"/>
+      <c r="BE134" s="9">
+        <v>1</v>
+      </c>
       <c r="BF134" s="9"/>
       <c r="BG134" s="11"/>
-      <c r="BH134" s="9"/>
+      <c r="BH134" s="9">
+        <v>1</v>
+      </c>
       <c r="BI134" s="9"/>
       <c r="BJ134" s="11"/>
-      <c r="BK134" s="9"/>
+      <c r="BK134" s="9">
+        <v>1</v>
+      </c>
       <c r="BL134" s="9"/>
       <c r="BM134" s="11"/>
       <c r="BN134" s="9"/>
@@ -16295,27 +16511,39 @@
       <c r="BP134" s="9"/>
       <c r="BQ134" s="9"/>
     </row>
-    <row r="135" spans="1:69" ht="16.5" thickBot="1">
+    <row r="135" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A135" s="3" t="s">
         <v>273</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C135" s="4"/>
+      <c r="C135" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D135" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E135" s="4"/>
-      <c r="F135" s="4"/>
-      <c r="G135" s="4"/>
-      <c r="I135" s="9"/>
+      <c r="E135" s="4">
+        <v>5445</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I135" s="9">
+        <v>1</v>
+      </c>
       <c r="J135" s="9"/>
       <c r="K135" s="9"/>
       <c r="L135" s="9"/>
       <c r="M135" s="11"/>
       <c r="N135" s="9"/>
-      <c r="O135" s="9"/>
+      <c r="O135" s="9">
+        <v>1</v>
+      </c>
       <c r="P135" s="9"/>
       <c r="Q135" s="9"/>
       <c r="R135" s="9"/>
@@ -16324,24 +16552,36 @@
       <c r="U135" s="9"/>
       <c r="V135" s="9"/>
       <c r="W135" s="9"/>
-      <c r="X135" s="9"/>
+      <c r="X135" s="9">
+        <v>1</v>
+      </c>
       <c r="Y135" s="11"/>
-      <c r="Z135" s="9"/>
+      <c r="Z135" s="9">
+        <v>1</v>
+      </c>
       <c r="AA135" s="9"/>
       <c r="AB135" s="9"/>
       <c r="AC135" s="9"/>
-      <c r="AD135" s="9"/>
+      <c r="AD135" s="9">
+        <v>1</v>
+      </c>
       <c r="AE135" s="9"/>
       <c r="AF135" s="11"/>
       <c r="AG135" s="9"/>
-      <c r="AH135" s="9"/>
+      <c r="AH135" s="9">
+        <v>1</v>
+      </c>
       <c r="AI135" s="11"/>
       <c r="AJ135" s="9"/>
       <c r="AK135" s="9"/>
-      <c r="AL135" s="9"/>
+      <c r="AL135" s="9">
+        <v>1</v>
+      </c>
       <c r="AM135" s="9"/>
       <c r="AN135" s="11"/>
-      <c r="AO135" s="9"/>
+      <c r="AO135" s="9">
+        <v>1</v>
+      </c>
       <c r="AP135" s="9"/>
       <c r="AQ135" s="9"/>
       <c r="AR135" s="11"/>
@@ -16349,21 +16589,33 @@
       <c r="AT135" s="9"/>
       <c r="AU135" s="9"/>
       <c r="AV135" s="9"/>
-      <c r="AW135" s="9"/>
+      <c r="AW135" s="9">
+        <v>1</v>
+      </c>
       <c r="AX135" s="11"/>
       <c r="AY135" s="9"/>
-      <c r="AZ135" s="9"/>
+      <c r="AZ135" s="9">
+        <v>1</v>
+      </c>
       <c r="BA135" s="11"/>
       <c r="BB135" s="9"/>
-      <c r="BC135" s="9"/>
+      <c r="BC135" s="9">
+        <v>1</v>
+      </c>
       <c r="BD135" s="11"/>
-      <c r="BE135" s="9"/>
+      <c r="BE135" s="9">
+        <v>1</v>
+      </c>
       <c r="BF135" s="9"/>
       <c r="BG135" s="11"/>
-      <c r="BH135" s="9"/>
+      <c r="BH135" s="9">
+        <v>1</v>
+      </c>
       <c r="BI135" s="9"/>
       <c r="BJ135" s="11"/>
-      <c r="BK135" s="9"/>
+      <c r="BK135" s="9">
+        <v>1</v>
+      </c>
       <c r="BL135" s="9"/>
       <c r="BM135" s="11"/>
       <c r="BN135" s="9"/>
@@ -16371,27 +16623,43 @@
       <c r="BP135" s="9"/>
       <c r="BQ135" s="9"/>
     </row>
-    <row r="136" spans="1:69" ht="16.5" thickBot="1">
+    <row r="136" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A136" s="3" t="s">
         <v>275</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C136" s="4"/>
+      <c r="C136" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D136" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E136" s="4"/>
-      <c r="F136" s="4"/>
-      <c r="G136" s="4"/>
-      <c r="I136" s="9"/>
-      <c r="J136" s="9"/>
+      <c r="E136" s="4">
+        <v>1008020</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G136" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="I136" s="9">
+        <v>1</v>
+      </c>
+      <c r="J136" s="9">
+        <v>1</v>
+      </c>
       <c r="K136" s="9"/>
-      <c r="L136" s="9"/>
+      <c r="L136" s="9">
+        <v>1</v>
+      </c>
       <c r="M136" s="11"/>
       <c r="N136" s="9"/>
-      <c r="O136" s="9"/>
+      <c r="O136" s="9">
+        <v>1</v>
+      </c>
       <c r="P136" s="9"/>
       <c r="Q136" s="9"/>
       <c r="R136" s="9"/>
@@ -16400,24 +16668,40 @@
       <c r="U136" s="9"/>
       <c r="V136" s="9"/>
       <c r="W136" s="9"/>
-      <c r="X136" s="9"/>
+      <c r="X136" s="9">
+        <v>1</v>
+      </c>
       <c r="Y136" s="11"/>
-      <c r="Z136" s="9"/>
-      <c r="AA136" s="9"/>
-      <c r="AB136" s="9"/>
+      <c r="Z136" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA136" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB136" s="9">
+        <v>1</v>
+      </c>
       <c r="AC136" s="9"/>
-      <c r="AD136" s="9"/>
+      <c r="AD136" s="9">
+        <v>1</v>
+      </c>
       <c r="AE136" s="9"/>
       <c r="AF136" s="11"/>
       <c r="AG136" s="9"/>
-      <c r="AH136" s="9"/>
+      <c r="AH136" s="9">
+        <v>1</v>
+      </c>
       <c r="AI136" s="11"/>
       <c r="AJ136" s="9"/>
       <c r="AK136" s="9"/>
-      <c r="AL136" s="9"/>
+      <c r="AL136" s="9">
+        <v>1</v>
+      </c>
       <c r="AM136" s="9"/>
       <c r="AN136" s="11"/>
-      <c r="AO136" s="9"/>
+      <c r="AO136" s="9">
+        <v>1</v>
+      </c>
       <c r="AP136" s="9"/>
       <c r="AQ136" s="9"/>
       <c r="AR136" s="11"/>
@@ -16425,21 +16709,33 @@
       <c r="AT136" s="9"/>
       <c r="AU136" s="9"/>
       <c r="AV136" s="9"/>
-      <c r="AW136" s="9"/>
+      <c r="AW136" s="9">
+        <v>1</v>
+      </c>
       <c r="AX136" s="11"/>
       <c r="AY136" s="9"/>
-      <c r="AZ136" s="9"/>
+      <c r="AZ136" s="9">
+        <v>1</v>
+      </c>
       <c r="BA136" s="11"/>
       <c r="BB136" s="9"/>
-      <c r="BC136" s="9"/>
+      <c r="BC136" s="9">
+        <v>1</v>
+      </c>
       <c r="BD136" s="11"/>
-      <c r="BE136" s="9"/>
+      <c r="BE136" s="9">
+        <v>1</v>
+      </c>
       <c r="BF136" s="9"/>
       <c r="BG136" s="11"/>
-      <c r="BH136" s="9"/>
+      <c r="BH136" s="9">
+        <v>1</v>
+      </c>
       <c r="BI136" s="9"/>
       <c r="BJ136" s="11"/>
-      <c r="BK136" s="9"/>
+      <c r="BK136" s="9">
+        <v>1</v>
+      </c>
       <c r="BL136" s="9"/>
       <c r="BM136" s="11"/>
       <c r="BN136" s="9"/>
@@ -16447,26 +16743,42 @@
       <c r="BP136" s="9"/>
       <c r="BQ136" s="9"/>
     </row>
-    <row r="137" spans="1:69" ht="16.5" thickBot="1">
+    <row r="137" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A137" s="3" t="s">
         <v>277</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="C137" s="4"/>
+      <c r="C137" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D137" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E137" s="4"/>
-      <c r="F137" s="4"/>
-      <c r="G137" s="4"/>
-      <c r="I137" s="9"/>
+      <c r="E137" s="4">
+        <v>750271</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G137" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="I137" s="9">
+        <v>1</v>
+      </c>
       <c r="J137" s="9"/>
-      <c r="K137" s="9"/>
-      <c r="L137" s="9"/>
+      <c r="K137" s="9">
+        <v>1</v>
+      </c>
+      <c r="L137" s="9">
+        <v>1</v>
+      </c>
       <c r="M137" s="11"/>
-      <c r="N137" s="9"/>
+      <c r="N137" s="9">
+        <v>1</v>
+      </c>
       <c r="O137" s="9"/>
       <c r="P137" s="9"/>
       <c r="Q137" s="9"/>
@@ -16476,19 +16788,31 @@
       <c r="U137" s="9"/>
       <c r="V137" s="9"/>
       <c r="W137" s="9"/>
-      <c r="X137" s="9"/>
+      <c r="X137" s="9">
+        <v>1</v>
+      </c>
       <c r="Y137" s="11"/>
-      <c r="Z137" s="9"/>
+      <c r="Z137" s="9">
+        <v>1</v>
+      </c>
       <c r="AA137" s="9"/>
       <c r="AB137" s="9"/>
       <c r="AC137" s="9"/>
-      <c r="AD137" s="9"/>
-      <c r="AE137" s="9"/>
+      <c r="AD137" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE137" s="9">
+        <v>1</v>
+      </c>
       <c r="AF137" s="11"/>
       <c r="AG137" s="9"/>
-      <c r="AH137" s="9"/>
+      <c r="AH137" s="9">
+        <v>1</v>
+      </c>
       <c r="AI137" s="11"/>
-      <c r="AJ137" s="9"/>
+      <c r="AJ137" s="9">
+        <v>1</v>
+      </c>
       <c r="AK137" s="9"/>
       <c r="AL137" s="9"/>
       <c r="AM137" s="9"/>
@@ -16497,25 +16821,37 @@
       <c r="AP137" s="9"/>
       <c r="AQ137" s="9"/>
       <c r="AR137" s="11"/>
-      <c r="AS137" s="9"/>
+      <c r="AS137" s="9">
+        <v>1</v>
+      </c>
       <c r="AT137" s="9"/>
       <c r="AU137" s="9"/>
       <c r="AV137" s="9"/>
       <c r="AW137" s="9"/>
       <c r="AX137" s="11"/>
       <c r="AY137" s="9"/>
-      <c r="AZ137" s="9"/>
+      <c r="AZ137" s="9">
+        <v>1</v>
+      </c>
       <c r="BA137" s="11"/>
       <c r="BB137" s="9"/>
-      <c r="BC137" s="9"/>
+      <c r="BC137" s="9">
+        <v>1</v>
+      </c>
       <c r="BD137" s="11"/>
-      <c r="BE137" s="9"/>
+      <c r="BE137" s="9">
+        <v>1</v>
+      </c>
       <c r="BF137" s="9"/>
       <c r="BG137" s="11"/>
-      <c r="BH137" s="9"/>
+      <c r="BH137" s="9">
+        <v>1</v>
+      </c>
       <c r="BI137" s="9"/>
       <c r="BJ137" s="11"/>
-      <c r="BK137" s="9"/>
+      <c r="BK137" s="9">
+        <v>1</v>
+      </c>
       <c r="BL137" s="9"/>
       <c r="BM137" s="11"/>
       <c r="BN137" s="9"/>
@@ -16523,26 +16859,42 @@
       <c r="BP137" s="9"/>
       <c r="BQ137" s="9"/>
     </row>
-    <row r="138" spans="1:69" ht="16.5" thickBot="1">
+    <row r="138" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A138" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C138" s="4"/>
+      <c r="C138" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D138" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E138" s="4"/>
-      <c r="F138" s="4"/>
-      <c r="G138" s="4"/>
-      <c r="I138" s="9"/>
+      <c r="E138" s="4">
+        <v>919452</v>
+      </c>
+      <c r="F138" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G138" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="I138" s="9">
+        <v>1</v>
+      </c>
       <c r="J138" s="9"/>
-      <c r="K138" s="9"/>
-      <c r="L138" s="9"/>
+      <c r="K138" s="9">
+        <v>1</v>
+      </c>
+      <c r="L138" s="9">
+        <v>1</v>
+      </c>
       <c r="M138" s="11"/>
-      <c r="N138" s="9"/>
+      <c r="N138" s="9">
+        <v>1</v>
+      </c>
       <c r="O138" s="9"/>
       <c r="P138" s="9"/>
       <c r="Q138" s="9"/>
@@ -16551,20 +16903,34 @@
       <c r="T138" s="11"/>
       <c r="U138" s="9"/>
       <c r="V138" s="9"/>
-      <c r="W138" s="9"/>
-      <c r="X138" s="9"/>
+      <c r="W138" s="9">
+        <v>1</v>
+      </c>
+      <c r="X138" s="9">
+        <v>1</v>
+      </c>
       <c r="Y138" s="11"/>
-      <c r="Z138" s="9"/>
+      <c r="Z138" s="9">
+        <v>1</v>
+      </c>
       <c r="AA138" s="9"/>
       <c r="AB138" s="9"/>
       <c r="AC138" s="9"/>
-      <c r="AD138" s="9"/>
-      <c r="AE138" s="9"/>
+      <c r="AD138" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE138" s="9">
+        <v>1</v>
+      </c>
       <c r="AF138" s="11"/>
       <c r="AG138" s="9"/>
-      <c r="AH138" s="9"/>
+      <c r="AH138" s="9">
+        <v>1</v>
+      </c>
       <c r="AI138" s="11"/>
-      <c r="AJ138" s="9"/>
+      <c r="AJ138" s="9">
+        <v>1</v>
+      </c>
       <c r="AK138" s="9"/>
       <c r="AL138" s="9"/>
       <c r="AM138" s="9"/>
@@ -16573,25 +16939,37 @@
       <c r="AP138" s="9"/>
       <c r="AQ138" s="9"/>
       <c r="AR138" s="11"/>
-      <c r="AS138" s="9"/>
+      <c r="AS138" s="9">
+        <v>1</v>
+      </c>
       <c r="AT138" s="9"/>
       <c r="AU138" s="9"/>
       <c r="AV138" s="9"/>
       <c r="AW138" s="9"/>
       <c r="AX138" s="11"/>
       <c r="AY138" s="9"/>
-      <c r="AZ138" s="9"/>
+      <c r="AZ138" s="9">
+        <v>1</v>
+      </c>
       <c r="BA138" s="11"/>
       <c r="BB138" s="9"/>
-      <c r="BC138" s="9"/>
+      <c r="BC138" s="9">
+        <v>1</v>
+      </c>
       <c r="BD138" s="11"/>
-      <c r="BE138" s="9"/>
+      <c r="BE138" s="9">
+        <v>1</v>
+      </c>
       <c r="BF138" s="9"/>
       <c r="BG138" s="11"/>
-      <c r="BH138" s="9"/>
+      <c r="BH138" s="9">
+        <v>1</v>
+      </c>
       <c r="BI138" s="9"/>
       <c r="BJ138" s="11"/>
-      <c r="BK138" s="9"/>
+      <c r="BK138" s="9">
+        <v>1</v>
+      </c>
       <c r="BL138" s="9"/>
       <c r="BM138" s="11"/>
       <c r="BN138" s="9"/>
@@ -16599,26 +16977,38 @@
       <c r="BP138" s="9"/>
       <c r="BQ138" s="9"/>
     </row>
-    <row r="139" spans="1:69" ht="16.5" thickBot="1">
+    <row r="139" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A139" s="3" t="s">
         <v>281</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C139" s="4"/>
+      <c r="C139" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D139" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E139" s="4"/>
-      <c r="F139" s="4"/>
-      <c r="G139" s="4"/>
-      <c r="I139" s="9"/>
+      <c r="E139" s="4">
+        <v>6265</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G139" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I139" s="9">
+        <v>1</v>
+      </c>
       <c r="J139" s="9"/>
       <c r="K139" s="9"/>
       <c r="L139" s="9"/>
       <c r="M139" s="11"/>
-      <c r="N139" s="9"/>
+      <c r="N139" s="9">
+        <v>1</v>
+      </c>
       <c r="O139" s="9"/>
       <c r="P139" s="9"/>
       <c r="Q139" s="9"/>
@@ -16628,19 +17018,33 @@
       <c r="U139" s="9"/>
       <c r="V139" s="9"/>
       <c r="W139" s="9"/>
-      <c r="X139" s="9"/>
+      <c r="X139" s="9">
+        <v>1</v>
+      </c>
       <c r="Y139" s="11"/>
-      <c r="Z139" s="9"/>
-      <c r="AA139" s="9"/>
-      <c r="AB139" s="9"/>
+      <c r="Z139" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA139" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB139" s="9">
+        <v>1</v>
+      </c>
       <c r="AC139" s="9"/>
-      <c r="AD139" s="9"/>
+      <c r="AD139" s="9">
+        <v>1</v>
+      </c>
       <c r="AE139" s="9"/>
       <c r="AF139" s="11"/>
       <c r="AG139" s="9"/>
-      <c r="AH139" s="9"/>
+      <c r="AH139" s="9">
+        <v>1</v>
+      </c>
       <c r="AI139" s="11"/>
-      <c r="AJ139" s="9"/>
+      <c r="AJ139" s="9">
+        <v>1</v>
+      </c>
       <c r="AK139" s="9"/>
       <c r="AL139" s="9"/>
       <c r="AM139" s="9"/>
@@ -16653,21 +17057,33 @@
       <c r="AT139" s="9"/>
       <c r="AU139" s="9"/>
       <c r="AV139" s="9"/>
-      <c r="AW139" s="9"/>
+      <c r="AW139" s="9">
+        <v>1</v>
+      </c>
       <c r="AX139" s="11"/>
       <c r="AY139" s="9"/>
-      <c r="AZ139" s="9"/>
+      <c r="AZ139" s="9">
+        <v>1</v>
+      </c>
       <c r="BA139" s="11"/>
-      <c r="BB139" s="9"/>
+      <c r="BB139" s="9">
+        <v>1</v>
+      </c>
       <c r="BC139" s="9"/>
       <c r="BD139" s="11"/>
-      <c r="BE139" s="9"/>
+      <c r="BE139" s="9">
+        <v>1</v>
+      </c>
       <c r="BF139" s="9"/>
       <c r="BG139" s="11"/>
-      <c r="BH139" s="9"/>
+      <c r="BH139" s="9">
+        <v>1</v>
+      </c>
       <c r="BI139" s="9"/>
       <c r="BJ139" s="11"/>
-      <c r="BK139" s="9"/>
+      <c r="BK139" s="9">
+        <v>1</v>
+      </c>
       <c r="BL139" s="9"/>
       <c r="BM139" s="11"/>
       <c r="BN139" s="9"/>
@@ -16675,48 +17091,78 @@
       <c r="BP139" s="9"/>
       <c r="BQ139" s="9"/>
     </row>
-    <row r="140" spans="1:69" ht="16.5" thickBot="1">
+    <row r="140" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A140" s="3" t="s">
         <v>283</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C140" s="4"/>
+      <c r="C140" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D140" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E140" s="4"/>
-      <c r="F140" s="4"/>
-      <c r="G140" s="4"/>
-      <c r="I140" s="9"/>
+      <c r="E140" s="4">
+        <v>617102</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G140" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="I140" s="9">
+        <v>1</v>
+      </c>
       <c r="J140" s="9"/>
       <c r="K140" s="9"/>
-      <c r="L140" s="9"/>
+      <c r="L140" s="9">
+        <v>1</v>
+      </c>
       <c r="M140" s="11"/>
       <c r="N140" s="9"/>
       <c r="O140" s="9"/>
-      <c r="P140" s="9"/>
+      <c r="P140" s="9">
+        <v>1</v>
+      </c>
       <c r="Q140" s="9"/>
-      <c r="R140" s="9"/>
+      <c r="R140" s="9">
+        <v>1</v>
+      </c>
       <c r="S140" s="9"/>
       <c r="T140" s="11"/>
       <c r="U140" s="9"/>
       <c r="V140" s="9"/>
-      <c r="W140" s="9"/>
-      <c r="X140" s="9"/>
+      <c r="W140" s="9">
+        <v>1</v>
+      </c>
+      <c r="X140" s="9">
+        <v>1</v>
+      </c>
       <c r="Y140" s="11"/>
-      <c r="Z140" s="9"/>
-      <c r="AA140" s="9"/>
+      <c r="Z140" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA140" s="9">
+        <v>1</v>
+      </c>
       <c r="AB140" s="9"/>
       <c r="AC140" s="9"/>
-      <c r="AD140" s="9"/>
+      <c r="AD140" s="9">
+        <v>1</v>
+      </c>
       <c r="AE140" s="9"/>
       <c r="AF140" s="11"/>
-      <c r="AG140" s="9"/>
+      <c r="AG140" s="9">
+        <v>1</v>
+      </c>
       <c r="AH140" s="9"/>
       <c r="AI140" s="11"/>
-      <c r="AJ140" s="9"/>
+      <c r="AJ140" s="9">
+        <v>1</v>
+      </c>
       <c r="AK140" s="9"/>
       <c r="AL140" s="9"/>
       <c r="AM140" s="9"/>
@@ -16728,22 +17174,34 @@
       <c r="AS140" s="9"/>
       <c r="AT140" s="9"/>
       <c r="AU140" s="9"/>
-      <c r="AV140" s="9"/>
+      <c r="AV140" s="9">
+        <v>1</v>
+      </c>
       <c r="AW140" s="9"/>
       <c r="AX140" s="11"/>
       <c r="AY140" s="9"/>
-      <c r="AZ140" s="9"/>
+      <c r="AZ140" s="9">
+        <v>1</v>
+      </c>
       <c r="BA140" s="11"/>
       <c r="BB140" s="9"/>
-      <c r="BC140" s="9"/>
+      <c r="BC140" s="9">
+        <v>1</v>
+      </c>
       <c r="BD140" s="11"/>
-      <c r="BE140" s="9"/>
+      <c r="BE140" s="9">
+        <v>1</v>
+      </c>
       <c r="BF140" s="9"/>
       <c r="BG140" s="11"/>
-      <c r="BH140" s="9"/>
+      <c r="BH140" s="9">
+        <v>1</v>
+      </c>
       <c r="BI140" s="9"/>
       <c r="BJ140" s="11"/>
-      <c r="BK140" s="9"/>
+      <c r="BK140" s="9">
+        <v>1</v>
+      </c>
       <c r="BL140" s="9"/>
       <c r="BM140" s="11"/>
       <c r="BN140" s="9"/>
@@ -16751,34 +17209,50 @@
       <c r="BP140" s="9"/>
       <c r="BQ140" s="9"/>
     </row>
-    <row r="141" spans="1:69" ht="16.5" thickBot="1">
+    <row r="141" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A141" s="3" t="s">
         <v>285</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="C141" s="4"/>
+      <c r="C141" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D141" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E141" s="4"/>
-      <c r="F141" s="4"/>
-      <c r="G141" s="4"/>
-      <c r="I141" s="9"/>
+      <c r="E141" s="4">
+        <v>263211</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="G141" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I141" s="9">
+        <v>1</v>
+      </c>
       <c r="J141" s="9"/>
-      <c r="K141" s="9"/>
+      <c r="K141" s="9">
+        <v>1</v>
+      </c>
       <c r="L141" s="9"/>
       <c r="M141" s="11"/>
       <c r="N141" s="9"/>
-      <c r="O141" s="9"/>
+      <c r="O141" s="9">
+        <v>1</v>
+      </c>
       <c r="P141" s="9"/>
       <c r="Q141" s="9"/>
       <c r="R141" s="9"/>
       <c r="S141" s="9"/>
       <c r="T141" s="11"/>
       <c r="U141" s="9"/>
-      <c r="V141" s="9"/>
+      <c r="V141" s="9">
+        <v>1</v>
+      </c>
       <c r="W141" s="9"/>
       <c r="X141" s="9"/>
       <c r="Y141" s="11"/>
@@ -16787,12 +17261,18 @@
       <c r="AB141" s="9"/>
       <c r="AC141" s="9"/>
       <c r="AD141" s="9"/>
-      <c r="AE141" s="9"/>
+      <c r="AE141" s="9">
+        <v>1</v>
+      </c>
       <c r="AF141" s="11"/>
-      <c r="AG141" s="9"/>
+      <c r="AG141" s="9">
+        <v>1</v>
+      </c>
       <c r="AH141" s="9"/>
       <c r="AI141" s="11"/>
-      <c r="AJ141" s="9"/>
+      <c r="AJ141" s="9">
+        <v>1</v>
+      </c>
       <c r="AK141" s="9"/>
       <c r="AL141" s="9"/>
       <c r="AM141" s="9"/>
@@ -16805,21 +17285,33 @@
       <c r="AT141" s="9"/>
       <c r="AU141" s="9"/>
       <c r="AV141" s="9"/>
-      <c r="AW141" s="9"/>
+      <c r="AW141" s="9">
+        <v>1</v>
+      </c>
       <c r="AX141" s="11"/>
-      <c r="AY141" s="9"/>
+      <c r="AY141" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ141" s="9"/>
       <c r="BA141" s="11"/>
-      <c r="BB141" s="9"/>
+      <c r="BB141" s="9">
+        <v>1</v>
+      </c>
       <c r="BC141" s="9"/>
       <c r="BD141" s="11"/>
-      <c r="BE141" s="9"/>
+      <c r="BE141" s="9">
+        <v>1</v>
+      </c>
       <c r="BF141" s="9"/>
       <c r="BG141" s="11"/>
-      <c r="BH141" s="9"/>
+      <c r="BH141" s="9">
+        <v>1</v>
+      </c>
       <c r="BI141" s="9"/>
       <c r="BJ141" s="11"/>
-      <c r="BK141" s="9"/>
+      <c r="BK141" s="9">
+        <v>1</v>
+      </c>
       <c r="BL141" s="9"/>
       <c r="BM141" s="11"/>
       <c r="BN141" s="9"/>
@@ -16827,27 +17319,37 @@
       <c r="BP141" s="9"/>
       <c r="BQ141" s="9"/>
     </row>
-    <row r="142" spans="1:69" ht="16.5" thickBot="1">
+    <row r="142" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A142" s="3" t="s">
         <v>287</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C142" s="4"/>
+      <c r="C142" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D142" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E142" s="4"/>
-      <c r="F142" s="4"/>
-      <c r="G142" s="4"/>
+      <c r="E142" s="4">
+        <v>8407</v>
+      </c>
+      <c r="F142" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="G142" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I142" s="9"/>
       <c r="J142" s="9"/>
       <c r="K142" s="9"/>
       <c r="L142" s="9"/>
       <c r="M142" s="11"/>
       <c r="N142" s="9"/>
-      <c r="O142" s="9"/>
+      <c r="O142" s="9">
+        <v>1</v>
+      </c>
       <c r="P142" s="9"/>
       <c r="Q142" s="9"/>
       <c r="R142" s="9"/>
@@ -16858,22 +17360,34 @@
       <c r="W142" s="9"/>
       <c r="X142" s="9"/>
       <c r="Y142" s="11"/>
-      <c r="Z142" s="9"/>
-      <c r="AA142" s="9"/>
+      <c r="Z142" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA142" s="9">
+        <v>1</v>
+      </c>
       <c r="AB142" s="9"/>
       <c r="AC142" s="9"/>
-      <c r="AD142" s="9"/>
+      <c r="AD142" s="9">
+        <v>1</v>
+      </c>
       <c r="AE142" s="9"/>
       <c r="AF142" s="11"/>
       <c r="AG142" s="9"/>
-      <c r="AH142" s="9"/>
+      <c r="AH142" s="9">
+        <v>1</v>
+      </c>
       <c r="AI142" s="11"/>
       <c r="AJ142" s="9"/>
       <c r="AK142" s="9"/>
-      <c r="AL142" s="9"/>
+      <c r="AL142" s="9">
+        <v>1</v>
+      </c>
       <c r="AM142" s="9"/>
       <c r="AN142" s="11"/>
-      <c r="AO142" s="9"/>
+      <c r="AO142" s="9">
+        <v>1</v>
+      </c>
       <c r="AP142" s="9"/>
       <c r="AQ142" s="9"/>
       <c r="AR142" s="11"/>
@@ -16881,70 +17395,114 @@
       <c r="AT142" s="9"/>
       <c r="AU142" s="9"/>
       <c r="AV142" s="9"/>
-      <c r="AW142" s="9"/>
+      <c r="AW142" s="9">
+        <v>1</v>
+      </c>
       <c r="AX142" s="11"/>
       <c r="AY142" s="9"/>
-      <c r="AZ142" s="9"/>
+      <c r="AZ142" s="9">
+        <v>1</v>
+      </c>
       <c r="BA142" s="11"/>
       <c r="BB142" s="9"/>
-      <c r="BC142" s="9"/>
+      <c r="BC142" s="9">
+        <v>1</v>
+      </c>
       <c r="BD142" s="11"/>
-      <c r="BE142" s="9"/>
+      <c r="BE142" s="9">
+        <v>1</v>
+      </c>
       <c r="BF142" s="9"/>
       <c r="BG142" s="11"/>
       <c r="BH142" s="9"/>
-      <c r="BI142" s="9"/>
+      <c r="BI142" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ142" s="11"/>
-      <c r="BK142" s="9"/>
-      <c r="BL142" s="9"/>
+      <c r="BK142" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL142" s="9">
+        <v>1</v>
+      </c>
       <c r="BM142" s="11"/>
-      <c r="BN142" s="9"/>
+      <c r="BN142" s="9">
+        <v>1</v>
+      </c>
       <c r="BO142" s="9"/>
       <c r="BP142" s="9"/>
       <c r="BQ142" s="9"/>
     </row>
-    <row r="143" spans="1:69" ht="16.5" thickBot="1">
+    <row r="143" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A143" s="3" t="s">
         <v>289</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C143" s="4"/>
+      <c r="C143" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D143" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E143" s="4"/>
-      <c r="F143" s="4"/>
-      <c r="G143" s="4"/>
-      <c r="I143" s="9"/>
+      <c r="E143" s="4">
+        <v>190596</v>
+      </c>
+      <c r="F143" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G143" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I143" s="9">
+        <v>1</v>
+      </c>
       <c r="J143" s="9"/>
-      <c r="K143" s="9"/>
+      <c r="K143" s="9">
+        <v>1</v>
+      </c>
       <c r="L143" s="9"/>
       <c r="M143" s="11"/>
-      <c r="N143" s="9"/>
+      <c r="N143" s="9">
+        <v>1</v>
+      </c>
       <c r="O143" s="9"/>
       <c r="P143" s="9"/>
       <c r="Q143" s="9"/>
       <c r="R143" s="9"/>
-      <c r="S143" s="9"/>
+      <c r="S143" s="9">
+        <v>1</v>
+      </c>
       <c r="T143" s="11"/>
       <c r="U143" s="9"/>
       <c r="V143" s="9"/>
       <c r="W143" s="9"/>
-      <c r="X143" s="9"/>
+      <c r="X143" s="9">
+        <v>1</v>
+      </c>
       <c r="Y143" s="11"/>
-      <c r="Z143" s="9"/>
-      <c r="AA143" s="9"/>
+      <c r="Z143" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA143" s="9">
+        <v>1</v>
+      </c>
       <c r="AB143" s="9"/>
       <c r="AC143" s="9"/>
-      <c r="AD143" s="9"/>
+      <c r="AD143" s="9">
+        <v>1</v>
+      </c>
       <c r="AE143" s="9"/>
       <c r="AF143" s="11"/>
       <c r="AG143" s="9"/>
-      <c r="AH143" s="9"/>
+      <c r="AH143" s="9">
+        <v>1</v>
+      </c>
       <c r="AI143" s="11"/>
-      <c r="AJ143" s="9"/>
+      <c r="AJ143" s="9">
+        <v>1</v>
+      </c>
       <c r="AK143" s="9"/>
       <c r="AL143" s="9"/>
       <c r="AM143" s="9"/>
@@ -16954,24 +17512,36 @@
       <c r="AQ143" s="9"/>
       <c r="AR143" s="11"/>
       <c r="AS143" s="9"/>
-      <c r="AT143" s="9"/>
+      <c r="AT143" s="9">
+        <v>1</v>
+      </c>
       <c r="AU143" s="9"/>
       <c r="AV143" s="9"/>
       <c r="AW143" s="9"/>
       <c r="AX143" s="11"/>
       <c r="AY143" s="9"/>
-      <c r="AZ143" s="9"/>
+      <c r="AZ143" s="9">
+        <v>1</v>
+      </c>
       <c r="BA143" s="11"/>
-      <c r="BB143" s="9"/>
+      <c r="BB143" s="9">
+        <v>1</v>
+      </c>
       <c r="BC143" s="9"/>
       <c r="BD143" s="11"/>
-      <c r="BE143" s="9"/>
+      <c r="BE143" s="9">
+        <v>1</v>
+      </c>
       <c r="BF143" s="9"/>
       <c r="BG143" s="11"/>
-      <c r="BH143" s="9"/>
+      <c r="BH143" s="9">
+        <v>1</v>
+      </c>
       <c r="BI143" s="9"/>
       <c r="BJ143" s="11"/>
-      <c r="BK143" s="9"/>
+      <c r="BK143" s="9">
+        <v>1</v>
+      </c>
       <c r="BL143" s="9"/>
       <c r="BM143" s="11"/>
       <c r="BN143" s="9"/>
@@ -16979,53 +17549,79 @@
       <c r="BP143" s="9"/>
       <c r="BQ143" s="9"/>
     </row>
-    <row r="144" spans="1:69" ht="16.5" thickBot="1">
+    <row r="144" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A144" s="3" t="s">
         <v>291</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C144" s="4"/>
+      <c r="C144" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D144" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E144" s="4"/>
-      <c r="F144" s="4"/>
-      <c r="G144" s="4"/>
+      <c r="E144" s="4">
+        <v>54958</v>
+      </c>
+      <c r="F144" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G144" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="I144" s="9"/>
       <c r="J144" s="9"/>
       <c r="K144" s="9"/>
-      <c r="L144" s="9"/>
+      <c r="L144" s="9">
+        <v>1</v>
+      </c>
       <c r="M144" s="11"/>
       <c r="N144" s="9"/>
-      <c r="O144" s="9"/>
+      <c r="O144" s="9">
+        <v>1</v>
+      </c>
       <c r="P144" s="9"/>
       <c r="Q144" s="9"/>
       <c r="R144" s="9"/>
       <c r="S144" s="9"/>
       <c r="T144" s="11"/>
       <c r="U144" s="9"/>
-      <c r="V144" s="9"/>
+      <c r="V144" s="9">
+        <v>1</v>
+      </c>
       <c r="W144" s="9"/>
       <c r="X144" s="9"/>
       <c r="Y144" s="11"/>
-      <c r="Z144" s="9"/>
-      <c r="AA144" s="9"/>
-      <c r="AB144" s="9"/>
+      <c r="Z144" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA144" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB144" s="9">
+        <v>1</v>
+      </c>
       <c r="AC144" s="9"/>
       <c r="AD144" s="9"/>
       <c r="AE144" s="9"/>
       <c r="AF144" s="11"/>
       <c r="AG144" s="9"/>
-      <c r="AH144" s="9"/>
+      <c r="AH144" s="9">
+        <v>1</v>
+      </c>
       <c r="AI144" s="11"/>
       <c r="AJ144" s="9"/>
       <c r="AK144" s="9"/>
-      <c r="AL144" s="9"/>
+      <c r="AL144" s="9">
+        <v>1</v>
+      </c>
       <c r="AM144" s="9"/>
       <c r="AN144" s="11"/>
-      <c r="AO144" s="9"/>
+      <c r="AO144" s="9">
+        <v>1</v>
+      </c>
       <c r="AP144" s="9"/>
       <c r="AQ144" s="9"/>
       <c r="AR144" s="11"/>
@@ -17033,21 +17629,33 @@
       <c r="AT144" s="9"/>
       <c r="AU144" s="9"/>
       <c r="AV144" s="9"/>
-      <c r="AW144" s="9"/>
+      <c r="AW144" s="9">
+        <v>1</v>
+      </c>
       <c r="AX144" s="11"/>
       <c r="AY144" s="9"/>
-      <c r="AZ144" s="9"/>
+      <c r="AZ144" s="9">
+        <v>1</v>
+      </c>
       <c r="BA144" s="11"/>
       <c r="BB144" s="9"/>
-      <c r="BC144" s="9"/>
+      <c r="BC144" s="9">
+        <v>1</v>
+      </c>
       <c r="BD144" s="11"/>
-      <c r="BE144" s="9"/>
+      <c r="BE144" s="9">
+        <v>1</v>
+      </c>
       <c r="BF144" s="9"/>
       <c r="BG144" s="11"/>
-      <c r="BH144" s="9"/>
+      <c r="BH144" s="9">
+        <v>1</v>
+      </c>
       <c r="BI144" s="9"/>
       <c r="BJ144" s="11"/>
-      <c r="BK144" s="9"/>
+      <c r="BK144" s="9">
+        <v>1</v>
+      </c>
       <c r="BL144" s="9"/>
       <c r="BM144" s="11"/>
       <c r="BN144" s="9"/>
@@ -17055,48 +17663,80 @@
       <c r="BP144" s="9"/>
       <c r="BQ144" s="9"/>
     </row>
-    <row r="145" spans="1:69" ht="16.5" thickBot="1">
+    <row r="145" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A145" s="3" t="s">
         <v>293</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="C145" s="4"/>
+      <c r="C145" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D145" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E145" s="4"/>
-      <c r="F145" s="4"/>
-      <c r="G145" s="4"/>
-      <c r="I145" s="9"/>
-      <c r="J145" s="9"/>
+      <c r="E145" s="4">
+        <v>16054</v>
+      </c>
+      <c r="F145" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="G145" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I145" s="9">
+        <v>1</v>
+      </c>
+      <c r="J145" s="9">
+        <v>1</v>
+      </c>
       <c r="K145" s="9"/>
-      <c r="L145" s="9"/>
+      <c r="L145" s="9">
+        <v>1</v>
+      </c>
       <c r="M145" s="11"/>
       <c r="N145" s="9"/>
-      <c r="O145" s="9"/>
+      <c r="O145" s="9">
+        <v>1</v>
+      </c>
       <c r="P145" s="9"/>
       <c r="Q145" s="9"/>
       <c r="R145" s="9"/>
       <c r="S145" s="9"/>
       <c r="T145" s="11"/>
       <c r="U145" s="9"/>
-      <c r="V145" s="9"/>
+      <c r="V145" s="9">
+        <v>1</v>
+      </c>
       <c r="W145" s="9"/>
-      <c r="X145" s="9"/>
+      <c r="X145" s="9">
+        <v>1</v>
+      </c>
       <c r="Y145" s="11"/>
-      <c r="Z145" s="9"/>
-      <c r="AA145" s="9"/>
-      <c r="AB145" s="9"/>
-      <c r="AC145" s="9"/>
+      <c r="Z145" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA145" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB145" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC145" s="9">
+        <v>1</v>
+      </c>
       <c r="AD145" s="9"/>
       <c r="AE145" s="9"/>
       <c r="AF145" s="11"/>
-      <c r="AG145" s="9"/>
+      <c r="AG145" s="9">
+        <v>1</v>
+      </c>
       <c r="AH145" s="9"/>
       <c r="AI145" s="11"/>
-      <c r="AJ145" s="9"/>
+      <c r="AJ145" s="9">
+        <v>1</v>
+      </c>
       <c r="AK145" s="9"/>
       <c r="AL145" s="9"/>
       <c r="AM145" s="9"/>
@@ -17109,21 +17749,33 @@
       <c r="AT145" s="9"/>
       <c r="AU145" s="9"/>
       <c r="AV145" s="9"/>
-      <c r="AW145" s="9"/>
+      <c r="AW145" s="9">
+        <v>1</v>
+      </c>
       <c r="AX145" s="11"/>
-      <c r="AY145" s="9"/>
+      <c r="AY145" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ145" s="9"/>
       <c r="BA145" s="11"/>
       <c r="BB145" s="9"/>
-      <c r="BC145" s="9"/>
+      <c r="BC145" s="9">
+        <v>1</v>
+      </c>
       <c r="BD145" s="11"/>
-      <c r="BE145" s="9"/>
+      <c r="BE145" s="9">
+        <v>1</v>
+      </c>
       <c r="BF145" s="9"/>
       <c r="BG145" s="11"/>
-      <c r="BH145" s="9"/>
+      <c r="BH145" s="9">
+        <v>1</v>
+      </c>
       <c r="BI145" s="9"/>
       <c r="BJ145" s="11"/>
-      <c r="BK145" s="9"/>
+      <c r="BK145" s="9">
+        <v>1</v>
+      </c>
       <c r="BL145" s="9"/>
       <c r="BM145" s="11"/>
       <c r="BN145" s="9"/>
@@ -17131,26 +17783,40 @@
       <c r="BP145" s="9"/>
       <c r="BQ145" s="9"/>
     </row>
-    <row r="146" spans="1:69" ht="16.5" thickBot="1">
+    <row r="146" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A146" s="3" t="s">
         <v>295</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C146" s="4"/>
+      <c r="C146" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D146" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E146" s="4"/>
-      <c r="F146" s="4"/>
-      <c r="G146" s="4"/>
-      <c r="I146" s="9"/>
+      <c r="E146" s="4">
+        <v>387</v>
+      </c>
+      <c r="F146" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="G146" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="I146" s="9">
+        <v>1</v>
+      </c>
       <c r="J146" s="9"/>
       <c r="K146" s="9"/>
-      <c r="L146" s="9"/>
+      <c r="L146" s="9">
+        <v>1</v>
+      </c>
       <c r="M146" s="11"/>
-      <c r="N146" s="9"/>
+      <c r="N146" s="9">
+        <v>1</v>
+      </c>
       <c r="O146" s="9"/>
       <c r="P146" s="9"/>
       <c r="Q146" s="9"/>
@@ -17159,20 +17825,36 @@
       <c r="T146" s="11"/>
       <c r="U146" s="9"/>
       <c r="V146" s="9"/>
-      <c r="W146" s="9"/>
-      <c r="X146" s="9"/>
+      <c r="W146" s="9">
+        <v>1</v>
+      </c>
+      <c r="X146" s="9">
+        <v>1</v>
+      </c>
       <c r="Y146" s="11"/>
-      <c r="Z146" s="9"/>
-      <c r="AA146" s="9"/>
-      <c r="AB146" s="9"/>
+      <c r="Z146" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA146" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB146" s="9">
+        <v>1</v>
+      </c>
       <c r="AC146" s="9"/>
-      <c r="AD146" s="9"/>
+      <c r="AD146" s="9">
+        <v>1</v>
+      </c>
       <c r="AE146" s="9"/>
       <c r="AF146" s="11"/>
       <c r="AG146" s="9"/>
-      <c r="AH146" s="9"/>
+      <c r="AH146" s="9">
+        <v>1</v>
+      </c>
       <c r="AI146" s="11"/>
-      <c r="AJ146" s="9"/>
+      <c r="AJ146" s="9">
+        <v>1</v>
+      </c>
       <c r="AK146" s="9"/>
       <c r="AL146" s="9"/>
       <c r="AM146" s="9"/>
@@ -17185,21 +17867,33 @@
       <c r="AT146" s="9"/>
       <c r="AU146" s="9"/>
       <c r="AV146" s="9"/>
-      <c r="AW146" s="9"/>
+      <c r="AW146" s="9">
+        <v>1</v>
+      </c>
       <c r="AX146" s="11"/>
-      <c r="AY146" s="9"/>
+      <c r="AY146" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ146" s="9"/>
       <c r="BA146" s="11"/>
-      <c r="BB146" s="9"/>
+      <c r="BB146" s="9">
+        <v>1</v>
+      </c>
       <c r="BC146" s="9"/>
       <c r="BD146" s="11"/>
-      <c r="BE146" s="9"/>
+      <c r="BE146" s="9">
+        <v>1</v>
+      </c>
       <c r="BF146" s="9"/>
       <c r="BG146" s="11"/>
-      <c r="BH146" s="9"/>
+      <c r="BH146" s="9">
+        <v>1</v>
+      </c>
       <c r="BI146" s="9"/>
       <c r="BJ146" s="11"/>
-      <c r="BK146" s="9"/>
+      <c r="BK146" s="9">
+        <v>1</v>
+      </c>
       <c r="BL146" s="9"/>
       <c r="BM146" s="11"/>
       <c r="BN146" s="9"/>
@@ -17207,27 +17901,43 @@
       <c r="BP146" s="9"/>
       <c r="BQ146" s="9"/>
     </row>
-    <row r="147" spans="1:69" ht="16.5" thickBot="1">
+    <row r="147" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A147" s="3" t="s">
         <v>297</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="C147" s="4"/>
+      <c r="C147" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D147" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E147" s="4"/>
-      <c r="F147" s="4"/>
-      <c r="G147" s="4"/>
-      <c r="I147" s="9"/>
-      <c r="J147" s="9"/>
+      <c r="E147" s="4">
+        <v>273785</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G147" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="I147" s="9">
+        <v>1</v>
+      </c>
+      <c r="J147" s="9">
+        <v>1</v>
+      </c>
       <c r="K147" s="9"/>
-      <c r="L147" s="9"/>
+      <c r="L147" s="9">
+        <v>1</v>
+      </c>
       <c r="M147" s="11"/>
       <c r="N147" s="9"/>
-      <c r="O147" s="9"/>
+      <c r="O147" s="9">
+        <v>1</v>
+      </c>
       <c r="P147" s="9"/>
       <c r="Q147" s="9"/>
       <c r="R147" s="9"/>
@@ -17236,19 +17946,29 @@
       <c r="U147" s="9"/>
       <c r="V147" s="9"/>
       <c r="W147" s="9"/>
-      <c r="X147" s="9"/>
+      <c r="X147" s="9">
+        <v>1</v>
+      </c>
       <c r="Y147" s="11"/>
-      <c r="Z147" s="9"/>
-      <c r="AA147" s="9"/>
+      <c r="Z147" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA147" s="9">
+        <v>1</v>
+      </c>
       <c r="AB147" s="9"/>
       <c r="AC147" s="9"/>
       <c r="AD147" s="9"/>
       <c r="AE147" s="9"/>
       <c r="AF147" s="11"/>
-      <c r="AG147" s="9"/>
+      <c r="AG147" s="9">
+        <v>1</v>
+      </c>
       <c r="AH147" s="9"/>
       <c r="AI147" s="11"/>
-      <c r="AJ147" s="9"/>
+      <c r="AJ147" s="9">
+        <v>1</v>
+      </c>
       <c r="AK147" s="9"/>
       <c r="AL147" s="9"/>
       <c r="AM147" s="9"/>
@@ -17261,21 +17981,33 @@
       <c r="AT147" s="9"/>
       <c r="AU147" s="9"/>
       <c r="AV147" s="9"/>
-      <c r="AW147" s="9"/>
+      <c r="AW147" s="9">
+        <v>1</v>
+      </c>
       <c r="AX147" s="11"/>
       <c r="AY147" s="9"/>
-      <c r="AZ147" s="9"/>
+      <c r="AZ147" s="9">
+        <v>1</v>
+      </c>
       <c r="BA147" s="11"/>
       <c r="BB147" s="9"/>
-      <c r="BC147" s="9"/>
+      <c r="BC147" s="9">
+        <v>1</v>
+      </c>
       <c r="BD147" s="11"/>
-      <c r="BE147" s="9"/>
+      <c r="BE147" s="9">
+        <v>1</v>
+      </c>
       <c r="BF147" s="9"/>
       <c r="BG147" s="11"/>
-      <c r="BH147" s="9"/>
+      <c r="BH147" s="9">
+        <v>1</v>
+      </c>
       <c r="BI147" s="9"/>
       <c r="BJ147" s="11"/>
-      <c r="BK147" s="9"/>
+      <c r="BK147" s="9">
+        <v>1</v>
+      </c>
       <c r="BL147" s="9"/>
       <c r="BM147" s="11"/>
       <c r="BN147" s="9"/>
@@ -17283,27 +18015,43 @@
       <c r="BP147" s="9"/>
       <c r="BQ147" s="9"/>
     </row>
-    <row r="148" spans="1:69" ht="16.5" thickBot="1">
+    <row r="148" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A148" s="3" t="s">
         <v>299</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="C148" s="4"/>
+      <c r="C148" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D148" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E148" s="4"/>
-      <c r="F148" s="4"/>
-      <c r="G148" s="4"/>
-      <c r="I148" s="9"/>
-      <c r="J148" s="9"/>
+      <c r="E148" s="4">
+        <v>296667</v>
+      </c>
+      <c r="F148" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G148" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="I148" s="9">
+        <v>1</v>
+      </c>
+      <c r="J148" s="9">
+        <v>1</v>
+      </c>
       <c r="K148" s="9"/>
-      <c r="L148" s="9"/>
+      <c r="L148" s="9">
+        <v>1</v>
+      </c>
       <c r="M148" s="11"/>
       <c r="N148" s="9"/>
-      <c r="O148" s="9"/>
+      <c r="O148" s="9">
+        <v>1</v>
+      </c>
       <c r="P148" s="9"/>
       <c r="Q148" s="9"/>
       <c r="R148" s="9"/>
@@ -17312,24 +18060,36 @@
       <c r="U148" s="9"/>
       <c r="V148" s="9"/>
       <c r="W148" s="9"/>
-      <c r="X148" s="9"/>
+      <c r="X148" s="9">
+        <v>1</v>
+      </c>
       <c r="Y148" s="11"/>
-      <c r="Z148" s="9"/>
-      <c r="AA148" s="9"/>
+      <c r="Z148" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA148" s="9">
+        <v>1</v>
+      </c>
       <c r="AB148" s="9"/>
       <c r="AC148" s="9"/>
       <c r="AD148" s="9"/>
       <c r="AE148" s="9"/>
       <c r="AF148" s="11"/>
       <c r="AG148" s="9"/>
-      <c r="AH148" s="9"/>
+      <c r="AH148" s="9">
+        <v>1</v>
+      </c>
       <c r="AI148" s="11"/>
       <c r="AJ148" s="9"/>
       <c r="AK148" s="9"/>
-      <c r="AL148" s="9"/>
+      <c r="AL148" s="9">
+        <v>1</v>
+      </c>
       <c r="AM148" s="9"/>
       <c r="AN148" s="11"/>
-      <c r="AO148" s="9"/>
+      <c r="AO148" s="9">
+        <v>1</v>
+      </c>
       <c r="AP148" s="9"/>
       <c r="AQ148" s="9"/>
       <c r="AR148" s="11"/>
@@ -17337,21 +18097,33 @@
       <c r="AT148" s="9"/>
       <c r="AU148" s="9"/>
       <c r="AV148" s="9"/>
-      <c r="AW148" s="9"/>
+      <c r="AW148" s="9">
+        <v>1</v>
+      </c>
       <c r="AX148" s="11"/>
-      <c r="AY148" s="9"/>
+      <c r="AY148" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ148" s="9"/>
       <c r="BA148" s="11"/>
-      <c r="BB148" s="9"/>
+      <c r="BB148" s="9">
+        <v>1</v>
+      </c>
       <c r="BC148" s="9"/>
       <c r="BD148" s="11"/>
-      <c r="BE148" s="9"/>
+      <c r="BE148" s="9">
+        <v>1</v>
+      </c>
       <c r="BF148" s="9"/>
       <c r="BG148" s="11"/>
       <c r="BH148" s="9"/>
-      <c r="BI148" s="9"/>
+      <c r="BI148" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ148" s="11"/>
-      <c r="BK148" s="9"/>
+      <c r="BK148" s="9">
+        <v>1</v>
+      </c>
       <c r="BL148" s="9"/>
       <c r="BM148" s="11"/>
       <c r="BN148" s="9"/>
@@ -17359,48 +18131,74 @@
       <c r="BP148" s="9"/>
       <c r="BQ148" s="9"/>
     </row>
-    <row r="149" spans="1:69" ht="16.5" thickBot="1">
+    <row r="149" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A149" s="3" t="s">
         <v>301</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C149" s="4"/>
+      <c r="C149" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D149" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E149" s="4"/>
-      <c r="F149" s="4"/>
-      <c r="G149" s="4"/>
+      <c r="E149" s="4">
+        <v>291443</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G149" s="4" t="s">
+        <v>548</v>
+      </c>
       <c r="I149" s="9"/>
       <c r="J149" s="9"/>
-      <c r="K149" s="9"/>
-      <c r="L149" s="9"/>
+      <c r="K149" s="9">
+        <v>1</v>
+      </c>
+      <c r="L149" s="9">
+        <v>1</v>
+      </c>
       <c r="M149" s="11"/>
-      <c r="N149" s="9"/>
+      <c r="N149" s="9">
+        <v>1</v>
+      </c>
       <c r="O149" s="9"/>
       <c r="P149" s="9"/>
       <c r="Q149" s="9"/>
       <c r="R149" s="9"/>
-      <c r="S149" s="9"/>
+      <c r="S149" s="9">
+        <v>1</v>
+      </c>
       <c r="T149" s="11"/>
       <c r="U149" s="9"/>
       <c r="V149" s="9"/>
       <c r="W149" s="9"/>
-      <c r="X149" s="9"/>
+      <c r="X149" s="9">
+        <v>1</v>
+      </c>
       <c r="Y149" s="11"/>
-      <c r="Z149" s="9"/>
-      <c r="AA149" s="9"/>
+      <c r="Z149" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA149" s="9">
+        <v>1</v>
+      </c>
       <c r="AB149" s="9"/>
       <c r="AC149" s="9"/>
       <c r="AD149" s="9"/>
       <c r="AE149" s="9"/>
       <c r="AF149" s="11"/>
-      <c r="AG149" s="9"/>
+      <c r="AG149" s="9">
+        <v>1</v>
+      </c>
       <c r="AH149" s="9"/>
       <c r="AI149" s="11"/>
-      <c r="AJ149" s="9"/>
+      <c r="AJ149" s="9">
+        <v>1</v>
+      </c>
       <c r="AK149" s="9"/>
       <c r="AL149" s="9"/>
       <c r="AM149" s="9"/>
@@ -17413,48 +18211,78 @@
       <c r="AT149" s="9"/>
       <c r="AU149" s="9"/>
       <c r="AV149" s="9"/>
-      <c r="AW149" s="9"/>
+      <c r="AW149" s="9">
+        <v>1</v>
+      </c>
       <c r="AX149" s="11"/>
       <c r="AY149" s="9"/>
-      <c r="AZ149" s="9"/>
+      <c r="AZ149" s="9">
+        <v>1</v>
+      </c>
       <c r="BA149" s="11"/>
       <c r="BB149" s="9"/>
-      <c r="BC149" s="9"/>
+      <c r="BC149" s="9">
+        <v>1</v>
+      </c>
       <c r="BD149" s="11"/>
-      <c r="BE149" s="9"/>
+      <c r="BE149" s="9">
+        <v>1</v>
+      </c>
       <c r="BF149" s="9"/>
       <c r="BG149" s="11"/>
-      <c r="BH149" s="9"/>
+      <c r="BH149" s="9">
+        <v>1</v>
+      </c>
       <c r="BI149" s="9"/>
       <c r="BJ149" s="11"/>
-      <c r="BK149" s="9"/>
-      <c r="BL149" s="9"/>
+      <c r="BK149" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL149" s="9">
+        <v>1</v>
+      </c>
       <c r="BM149" s="11"/>
-      <c r="BN149" s="9"/>
-      <c r="BO149" s="9"/>
+      <c r="BN149" s="9">
+        <v>1</v>
+      </c>
+      <c r="BO149" s="9">
+        <v>1</v>
+      </c>
       <c r="BP149" s="9"/>
       <c r="BQ149" s="9"/>
     </row>
-    <row r="150" spans="1:69" ht="16.5" thickBot="1">
+    <row r="150" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A150" s="3" t="s">
         <v>303</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C150" s="4"/>
+      <c r="C150" s="4" t="s">
+        <v>563</v>
+      </c>
       <c r="D150" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E150" s="4"/>
-      <c r="F150" s="4"/>
-      <c r="G150" s="4"/>
-      <c r="I150" s="9"/>
+      <c r="E150" s="4">
+        <v>773</v>
+      </c>
+      <c r="F150" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G150" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="I150" s="9">
+        <v>1</v>
+      </c>
       <c r="J150" s="9"/>
       <c r="K150" s="9"/>
       <c r="L150" s="9"/>
       <c r="M150" s="11"/>
-      <c r="N150" s="9"/>
+      <c r="N150" s="9">
+        <v>1</v>
+      </c>
       <c r="O150" s="9"/>
       <c r="P150" s="9"/>
       <c r="Q150" s="9"/>
@@ -17464,9 +18292,13 @@
       <c r="U150" s="9"/>
       <c r="V150" s="9"/>
       <c r="W150" s="9"/>
-      <c r="X150" s="9"/>
+      <c r="X150" s="9">
+        <v>1</v>
+      </c>
       <c r="Y150" s="11"/>
-      <c r="Z150" s="9"/>
+      <c r="Z150" s="9">
+        <v>1</v>
+      </c>
       <c r="AA150" s="9"/>
       <c r="AB150" s="9"/>
       <c r="AC150" s="9"/>
@@ -17474,9 +18306,13 @@
       <c r="AE150" s="9"/>
       <c r="AF150" s="11"/>
       <c r="AG150" s="9"/>
-      <c r="AH150" s="9"/>
+      <c r="AH150" s="9">
+        <v>1</v>
+      </c>
       <c r="AI150" s="11"/>
-      <c r="AJ150" s="9"/>
+      <c r="AJ150" s="9">
+        <v>1</v>
+      </c>
       <c r="AK150" s="9"/>
       <c r="AL150" s="9"/>
       <c r="AM150" s="9"/>
@@ -17489,21 +18325,33 @@
       <c r="AT150" s="9"/>
       <c r="AU150" s="9"/>
       <c r="AV150" s="9"/>
-      <c r="AW150" s="9"/>
+      <c r="AW150" s="9">
+        <v>1</v>
+      </c>
       <c r="AX150" s="11"/>
       <c r="AY150" s="9"/>
-      <c r="AZ150" s="9"/>
+      <c r="AZ150" s="9">
+        <v>1</v>
+      </c>
       <c r="BA150" s="11"/>
-      <c r="BB150" s="9"/>
+      <c r="BB150" s="9">
+        <v>1</v>
+      </c>
       <c r="BC150" s="9"/>
       <c r="BD150" s="11"/>
       <c r="BE150" s="9"/>
-      <c r="BF150" s="9"/>
+      <c r="BF150" s="9">
+        <v>1</v>
+      </c>
       <c r="BG150" s="11"/>
-      <c r="BH150" s="9"/>
+      <c r="BH150" s="9">
+        <v>1</v>
+      </c>
       <c r="BI150" s="9"/>
       <c r="BJ150" s="11"/>
-      <c r="BK150" s="9"/>
+      <c r="BK150" s="9">
+        <v>1</v>
+      </c>
       <c r="BL150" s="9"/>
       <c r="BM150" s="11"/>
       <c r="BN150" s="9"/>
@@ -20855,7 +21703,7 @@
       <c r="BP194" s="9"/>
       <c r="BQ194" s="9"/>
     </row>
-    <row r="195" spans="1:69" ht="16.5" thickBot="1">
+    <row r="195" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A195" s="3" t="s">
         <v>395</v>
       </c>
@@ -20931,7 +21779,7 @@
       <c r="BP195" s="9"/>
       <c r="BQ195" s="9"/>
     </row>
-    <row r="196" spans="1:69" ht="16.5" thickBot="1">
+    <row r="196" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A196" s="3" t="s">
         <v>398</v>
       </c>
@@ -21007,7 +21855,7 @@
       <c r="BP196" s="9"/>
       <c r="BQ196" s="9"/>
     </row>
-    <row r="197" spans="1:69" ht="16.5" thickBot="1">
+    <row r="197" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A197" s="3" t="s">
         <v>400</v>
       </c>
@@ -21083,7 +21931,7 @@
       <c r="BP197" s="9"/>
       <c r="BQ197" s="9"/>
     </row>
-    <row r="198" spans="1:69" ht="16.5" thickBot="1">
+    <row r="198" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A198" s="3" t="s">
         <v>402</v>
       </c>
@@ -21159,7 +22007,7 @@
       <c r="BP198" s="9"/>
       <c r="BQ198" s="9"/>
     </row>
-    <row r="199" spans="1:69" ht="16.5" thickBot="1">
+    <row r="199" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A199" s="3" t="s">
         <v>404</v>
       </c>
@@ -21235,7 +22083,7 @@
       <c r="BP199" s="9"/>
       <c r="BQ199" s="9"/>
     </row>
-    <row r="200" spans="1:69" ht="16.5" thickBot="1">
+    <row r="200" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A200" s="3" t="s">
         <v>406</v>
       </c>
@@ -21311,7 +22159,7 @@
       <c r="BP200" s="9"/>
       <c r="BQ200" s="9"/>
     </row>
-    <row r="201" spans="1:69" ht="16.5" thickBot="1">
+    <row r="201" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A201" s="3" t="s">
         <v>408</v>
       </c>
@@ -21387,7 +22235,7 @@
       <c r="BP201" s="9"/>
       <c r="BQ201" s="9"/>
     </row>
-    <row r="202" spans="1:69" ht="16.5" thickBot="1">
+    <row r="202" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A202" s="3" t="s">
         <v>410</v>
       </c>
@@ -21463,7 +22311,7 @@
       <c r="BP202" s="9"/>
       <c r="BQ202" s="9"/>
     </row>
-    <row r="203" spans="1:69" ht="32.25" thickBot="1">
+    <row r="203" spans="1:69" ht="32.25" hidden="1" thickBot="1">
       <c r="A203" s="3" t="s">
         <v>412</v>
       </c>
@@ -21539,7 +22387,7 @@
       <c r="BP203" s="9"/>
       <c r="BQ203" s="9"/>
     </row>
-    <row r="204" spans="1:69" ht="17.25" thickBot="1">
+    <row r="204" spans="1:69" ht="17.25" hidden="1" thickBot="1">
       <c r="A204" s="3" t="s">
         <v>414</v>
       </c>
@@ -21615,7 +22463,7 @@
       <c r="BP204" s="9"/>
       <c r="BQ204" s="9"/>
     </row>
-    <row r="205" spans="1:69" ht="16.5" thickBot="1">
+    <row r="205" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A205" s="3" t="s">
         <v>416</v>
       </c>
@@ -21691,7 +22539,7 @@
       <c r="BP205" s="9"/>
       <c r="BQ205" s="9"/>
     </row>
-    <row r="206" spans="1:69" ht="16.5" thickBot="1">
+    <row r="206" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A206" s="3" t="s">
         <v>418</v>
       </c>
@@ -21767,7 +22615,7 @@
       <c r="BP206" s="9"/>
       <c r="BQ206" s="9"/>
     </row>
-    <row r="207" spans="1:69" ht="16.5" thickBot="1">
+    <row r="207" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A207" s="3" t="s">
         <v>420</v>
       </c>
@@ -21843,7 +22691,7 @@
       <c r="BP207" s="9"/>
       <c r="BQ207" s="9"/>
     </row>
-    <row r="208" spans="1:69" ht="16.5" thickBot="1">
+    <row r="208" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A208" s="3" t="s">
         <v>422</v>
       </c>
@@ -21919,7 +22767,7 @@
       <c r="BP208" s="9"/>
       <c r="BQ208" s="9"/>
     </row>
-    <row r="209" spans="1:69" ht="16.5" thickBot="1">
+    <row r="209" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A209" s="3" t="s">
         <v>424</v>
       </c>
@@ -21995,7 +22843,7 @@
       <c r="BP209" s="9"/>
       <c r="BQ209" s="9"/>
     </row>
-    <row r="210" spans="1:69" ht="16.5" thickBot="1">
+    <row r="210" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A210" s="3" t="s">
         <v>426</v>
       </c>
@@ -22071,7 +22919,7 @@
       <c r="BP210" s="9"/>
       <c r="BQ210" s="9"/>
     </row>
-    <row r="211" spans="1:69" ht="16.5" thickBot="1">
+    <row r="211" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A211" s="3" t="s">
         <v>428</v>
       </c>
@@ -22147,7 +22995,7 @@
       <c r="BP211" s="9"/>
       <c r="BQ211" s="9"/>
     </row>
-    <row r="212" spans="1:69" ht="32.25" thickBot="1">
+    <row r="212" spans="1:69" ht="32.25" hidden="1" thickBot="1">
       <c r="A212" s="3" t="s">
         <v>430</v>
       </c>
@@ -22223,7 +23071,7 @@
       <c r="BP212" s="9"/>
       <c r="BQ212" s="9"/>
     </row>
-    <row r="213" spans="1:69" ht="16.5" thickBot="1">
+    <row r="213" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A213" s="3" t="s">
         <v>432</v>
       </c>
@@ -22299,7 +23147,7 @@
       <c r="BP213" s="9"/>
       <c r="BQ213" s="9"/>
     </row>
-    <row r="214" spans="1:69" ht="16.5" thickBot="1">
+    <row r="214" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A214" s="3" t="s">
         <v>434</v>
       </c>
@@ -22375,7 +23223,7 @@
       <c r="BP214" s="9"/>
       <c r="BQ214" s="9"/>
     </row>
-    <row r="215" spans="1:69" ht="16.5" thickBot="1">
+    <row r="215" spans="1:69" ht="16.5" hidden="1" thickBot="1">
       <c r="A215" s="3" t="s">
         <v>436</v>
       </c>
@@ -22451,7 +23299,7 @@
       <c r="BP215" s="9"/>
       <c r="BQ215" s="9"/>
     </row>
-    <row r="216" spans="1:69" ht="201.75">
+    <row r="216" spans="1:69" ht="202.5">
       <c r="I216" s="6" t="s">
         <v>485</v>
       </c>
@@ -22616,31 +23464,31 @@
       </c>
       <c r="I217">
         <f>SUM(I3:I215)</f>
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="J217">
         <f t="shared" ref="J217:BQ217" si="0">SUM(J3:J215)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K217">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L217">
         <f>SUM(L3:L215)</f>
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="N217">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="O217">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="P217">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q217">
         <f t="shared" si="0"/>
@@ -22648,63 +23496,63 @@
       </c>
       <c r="R217">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S217">
         <f>SUM(S3:S215)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="U217">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V217">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="W217">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="X217">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="Z217">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AA217">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="AB217">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="AC217">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD217">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="AE217">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AG217">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AH217">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="AJ217">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="AK217">
         <f t="shared" si="0"/>
@@ -22712,7 +23560,7 @@
       </c>
       <c r="AL217">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="AM217">
         <f t="shared" si="0"/>
@@ -22720,7 +23568,7 @@
       </c>
       <c r="AO217">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="AP217">
         <f t="shared" si="0"/>
@@ -22736,11 +23584,11 @@
       </c>
       <c r="AS217">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AT217">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AU217">
         <f t="shared" si="0"/>
@@ -22748,23 +23596,23 @@
       </c>
       <c r="AV217">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AW217">
         <f>SUM(AW3:AW215)</f>
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="AY217">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="AZ217">
         <f>SUM(AZ3:AZ215)</f>
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="BB217">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="BD217" s="12">
         <f t="shared" si="0"/>
@@ -22772,38 +23620,38 @@
       </c>
       <c r="BE217">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="BF217">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="BG217" s="12" t="s">
         <v>482</v>
       </c>
       <c r="BH217">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="BI217">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="BK217">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="BL217">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BN217">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BO217">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP217">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Task 2 - dodano  coś
</commit_message>
<xml_diff>
--- a/dane_aplikacji-zygol.xlsx
+++ b/dane_aplikacji-zygol.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="568">
   <si>
     <t>Id</t>
   </si>
@@ -1735,6 +1735,18 @@
   </si>
   <si>
     <t>3.3</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1844,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1888,11 +1900,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1970,6 +1993,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2068,13 +2092,17 @@
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$AH$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:multiLvlStrRef>
+                  <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
@@ -2082,7 +2110,14 @@
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:multiLvlStrRef>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
@@ -2098,11 +2133,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-622771744"/>
-        <c:axId val="-622760864"/>
+        <c:axId val="517880688"/>
+        <c:axId val="517868720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-622771744"/>
+        <c:axId val="517880688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,7 +2180,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-622760864"/>
+        <c:crossAx val="517868720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2153,7 +2188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-622760864"/>
+        <c:axId val="517868720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,7 +2239,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-622771744"/>
+        <c:crossAx val="517880688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3119,17 +3154,17 @@
   <dimension ref="A1:BQ217"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N175" sqref="N175"/>
+      <selection activeCell="AK167" sqref="AK167:AK169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="41.125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="15.75" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="14.75" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.25" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="5" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="15.25" customWidth="1"/>
     <col min="8" max="8" width="1.375" customWidth="1"/>
     <col min="9" max="12" width="3.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="1.125" style="12" customWidth="1"/>
@@ -3138,11 +3173,13 @@
     <col min="21" max="23" width="3.875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3.375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="1.25" style="12" customWidth="1"/>
-    <col min="26" max="27" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.875" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="3.375" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="3.875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="0.75" style="12" customWidth="1"/>
-    <col min="33" max="34" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="0.875" style="12" customWidth="1"/>
     <col min="36" max="39" width="3.875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="1.125" style="12" customWidth="1"/>
@@ -3154,11 +3191,13 @@
     <col min="51" max="51" width="3.875" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="3.875" customWidth="1"/>
     <col min="53" max="53" width="1.125" style="12" customWidth="1"/>
-    <col min="54" max="55" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.75" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="0.75" style="12" customWidth="1"/>
     <col min="57" max="58" width="3.875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="1" style="12" customWidth="1"/>
-    <col min="60" max="61" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="3.875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="1" style="12" customWidth="1"/>
     <col min="63" max="64" width="3.875" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="1.125" style="12" customWidth="1"/>
@@ -3272,7 +3311,7 @@
       <c r="BM1" s="10"/>
       <c r="BN1" s="7"/>
     </row>
-    <row r="2" spans="1:69" ht="143.25" thickBot="1">
+    <row r="2" spans="1:69" ht="141.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3449,7 +3488,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="3" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="3" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
@@ -3555,7 +3594,7 @@
       <c r="BP3" s="19"/>
       <c r="BQ3" s="19"/>
     </row>
-    <row r="4" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="4" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
@@ -3665,7 +3704,7 @@
       <c r="BP4" s="19"/>
       <c r="BQ4" s="19"/>
     </row>
-    <row r="5" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="5" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
@@ -3741,7 +3780,7 @@
       <c r="BP5" s="19"/>
       <c r="BQ5" s="19"/>
     </row>
-    <row r="6" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="6" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A6" s="22" t="s">
         <v>10</v>
       </c>
@@ -3817,7 +3856,7 @@
       <c r="BP6" s="19"/>
       <c r="BQ6" s="19"/>
     </row>
-    <row r="7" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="7" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
@@ -3925,7 +3964,7 @@
       <c r="BP7" s="19"/>
       <c r="BQ7" s="19"/>
     </row>
-    <row r="8" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="8" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -4031,7 +4070,7 @@
       <c r="BP8" s="19"/>
       <c r="BQ8" s="19"/>
     </row>
-    <row r="9" spans="1:69" s="18" customFormat="1" ht="17.25" hidden="1" customHeight="1" thickBot="1">
+    <row r="9" spans="1:69" s="18" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
@@ -4149,7 +4188,7 @@
       <c r="BP9" s="19"/>
       <c r="BQ9" s="19"/>
     </row>
-    <row r="10" spans="1:69" s="18" customFormat="1" ht="15" hidden="1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:69" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="16" t="s">
         <v>18</v>
       </c>
@@ -4263,7 +4302,7 @@
       <c r="BP10" s="19"/>
       <c r="BQ10" s="19"/>
     </row>
-    <row r="11" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="11" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
@@ -4369,7 +4408,7 @@
       <c r="BP11" s="19"/>
       <c r="BQ11" s="19"/>
     </row>
-    <row r="12" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="12" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
@@ -4485,7 +4524,7 @@
       <c r="BP12" s="19"/>
       <c r="BQ12" s="19"/>
     </row>
-    <row r="13" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="13" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A13" s="16" t="s">
         <v>24</v>
       </c>
@@ -4603,7 +4642,7 @@
       <c r="BP13" s="19"/>
       <c r="BQ13" s="19"/>
     </row>
-    <row r="14" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="14" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A14" s="16" t="s">
         <v>26</v>
       </c>
@@ -4715,7 +4754,7 @@
       <c r="BP14" s="19"/>
       <c r="BQ14" s="19"/>
     </row>
-    <row r="15" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="15" spans="1:69" ht="16.5" thickBot="1">
       <c r="A15" s="14" t="s">
         <v>28</v>
       </c>
@@ -4791,7 +4830,7 @@
       <c r="BP15" s="9"/>
       <c r="BQ15" s="9"/>
     </row>
-    <row r="16" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="16" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A16" s="16" t="s">
         <v>30</v>
       </c>
@@ -4897,7 +4936,7 @@
       <c r="BP16" s="19"/>
       <c r="BQ16" s="19"/>
     </row>
-    <row r="17" spans="1:69" s="18" customFormat="1" ht="15" hidden="1" customHeight="1" thickBot="1">
+    <row r="17" spans="1:69" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A17" s="16" t="s">
         <v>32</v>
       </c>
@@ -5005,7 +5044,7 @@
       <c r="BP17" s="19"/>
       <c r="BQ17" s="19"/>
     </row>
-    <row r="18" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="18" spans="1:69" s="18" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
       <c r="A18" s="16" t="s">
         <v>34</v>
       </c>
@@ -5109,7 +5148,7 @@
       <c r="BP18" s="19"/>
       <c r="BQ18" s="19"/>
     </row>
-    <row r="19" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="19" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
@@ -5229,7 +5268,7 @@
       <c r="BP19" s="19"/>
       <c r="BQ19" s="19"/>
     </row>
-    <row r="20" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="20" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>38</v>
       </c>
@@ -5341,7 +5380,7 @@
       <c r="BP20" s="19"/>
       <c r="BQ20" s="19"/>
     </row>
-    <row r="21" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="21" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
@@ -5457,7 +5496,7 @@
       <c r="BP21" s="19"/>
       <c r="BQ21" s="19"/>
     </row>
-    <row r="22" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="22" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A22" s="16" t="s">
         <v>42</v>
       </c>
@@ -5571,7 +5610,7 @@
       <c r="BP22" s="19"/>
       <c r="BQ22" s="19"/>
     </row>
-    <row r="23" spans="1:69" s="18" customFormat="1" ht="16.5" hidden="1" thickBot="1">
+    <row r="23" spans="1:69" s="18" customFormat="1" ht="16.5" thickBot="1">
       <c r="A23" s="16" t="s">
         <v>44</v>
       </c>
@@ -5693,7 +5732,7 @@
       <c r="BP23" s="19"/>
       <c r="BQ23" s="19"/>
     </row>
-    <row r="24" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="24" spans="1:69" ht="16.5" thickBot="1">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -5769,7 +5808,7 @@
       <c r="BP24" s="9"/>
       <c r="BQ24" s="9"/>
     </row>
-    <row r="25" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="25" spans="1:69" ht="16.5" thickBot="1">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -5845,7 +5884,7 @@
       <c r="BP25" s="9"/>
       <c r="BQ25" s="9"/>
     </row>
-    <row r="26" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="26" spans="1:69" ht="16.5" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
@@ -5921,7 +5960,7 @@
       <c r="BP26" s="9"/>
       <c r="BQ26" s="9"/>
     </row>
-    <row r="27" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="27" spans="1:69" ht="16.5" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>53</v>
       </c>
@@ -5997,7 +6036,7 @@
       <c r="BP27" s="9"/>
       <c r="BQ27" s="9"/>
     </row>
-    <row r="28" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="28" spans="1:69" ht="16.5" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
@@ -6073,7 +6112,7 @@
       <c r="BP28" s="9"/>
       <c r="BQ28" s="9"/>
     </row>
-    <row r="29" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="29" spans="1:69" ht="16.5" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>57</v>
       </c>
@@ -6149,7 +6188,7 @@
       <c r="BP29" s="9"/>
       <c r="BQ29" s="9"/>
     </row>
-    <row r="30" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="30" spans="1:69" ht="16.5" thickBot="1">
       <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
@@ -6225,7 +6264,7 @@
       <c r="BP30" s="9"/>
       <c r="BQ30" s="9"/>
     </row>
-    <row r="31" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="31" spans="1:69" ht="16.5" thickBot="1">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
@@ -6301,7 +6340,7 @@
       <c r="BP31" s="9"/>
       <c r="BQ31" s="9"/>
     </row>
-    <row r="32" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="32" spans="1:69" ht="16.5" thickBot="1">
       <c r="A32" s="3" t="s">
         <v>63</v>
       </c>
@@ -6377,7 +6416,7 @@
       <c r="BP32" s="9"/>
       <c r="BQ32" s="9"/>
     </row>
-    <row r="33" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="33" spans="1:69" ht="16.5" thickBot="1">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -6453,7 +6492,7 @@
       <c r="BP33" s="9"/>
       <c r="BQ33" s="9"/>
     </row>
-    <row r="34" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="34" spans="1:69" ht="16.5" thickBot="1">
       <c r="A34" s="3" t="s">
         <v>67</v>
       </c>
@@ -6529,7 +6568,7 @@
       <c r="BP34" s="9"/>
       <c r="BQ34" s="9"/>
     </row>
-    <row r="35" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="35" spans="1:69" ht="16.5" thickBot="1">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -6605,7 +6644,7 @@
       <c r="BP35" s="9"/>
       <c r="BQ35" s="9"/>
     </row>
-    <row r="36" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="36" spans="1:69" ht="16.5" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>71</v>
       </c>
@@ -6681,7 +6720,7 @@
       <c r="BP36" s="9"/>
       <c r="BQ36" s="9"/>
     </row>
-    <row r="37" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="37" spans="1:69" ht="16.5" thickBot="1">
       <c r="A37" s="3" t="s">
         <v>73</v>
       </c>
@@ -6757,7 +6796,7 @@
       <c r="BP37" s="9"/>
       <c r="BQ37" s="9"/>
     </row>
-    <row r="38" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="38" spans="1:69" ht="16.5" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>75</v>
       </c>
@@ -6833,7 +6872,7 @@
       <c r="BP38" s="9"/>
       <c r="BQ38" s="9"/>
     </row>
-    <row r="39" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="39" spans="1:69" ht="16.5" thickBot="1">
       <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
@@ -6909,7 +6948,7 @@
       <c r="BP39" s="9"/>
       <c r="BQ39" s="9"/>
     </row>
-    <row r="40" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="40" spans="1:69" ht="16.5" thickBot="1">
       <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
@@ -6985,7 +7024,7 @@
       <c r="BP40" s="9"/>
       <c r="BQ40" s="9"/>
     </row>
-    <row r="41" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="41" spans="1:69" ht="16.5" thickBot="1">
       <c r="A41" s="3" t="s">
         <v>81</v>
       </c>
@@ -7061,7 +7100,7 @@
       <c r="BP41" s="9"/>
       <c r="BQ41" s="9"/>
     </row>
-    <row r="42" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="42" spans="1:69" ht="16.5" thickBot="1">
       <c r="A42" s="3" t="s">
         <v>83</v>
       </c>
@@ -7137,7 +7176,7 @@
       <c r="BP42" s="9"/>
       <c r="BQ42" s="9"/>
     </row>
-    <row r="43" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="43" spans="1:69" ht="16.5" thickBot="1">
       <c r="A43" s="3" t="s">
         <v>85</v>
       </c>
@@ -7213,7 +7252,7 @@
       <c r="BP43" s="9"/>
       <c r="BQ43" s="9"/>
     </row>
-    <row r="44" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="44" spans="1:69" ht="16.5" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>87</v>
       </c>
@@ -7289,7 +7328,7 @@
       <c r="BP44" s="9"/>
       <c r="BQ44" s="9"/>
     </row>
-    <row r="45" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="45" spans="1:69" ht="16.5" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>89</v>
       </c>
@@ -7365,7 +7404,7 @@
       <c r="BP45" s="9"/>
       <c r="BQ45" s="9"/>
     </row>
-    <row r="46" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="46" spans="1:69" ht="16.5" thickBot="1">
       <c r="A46" s="3" t="s">
         <v>91</v>
       </c>
@@ -7473,7 +7512,7 @@
       <c r="BP46" s="9"/>
       <c r="BQ46" s="9"/>
     </row>
-    <row r="47" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="47" spans="1:69" ht="16.5" thickBot="1">
       <c r="A47" s="3" t="s">
         <v>94</v>
       </c>
@@ -7599,7 +7638,7 @@
       <c r="BP47" s="9"/>
       <c r="BQ47" s="9"/>
     </row>
-    <row r="48" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="48" spans="1:69" ht="16.5" thickBot="1">
       <c r="A48" s="3" t="s">
         <v>96</v>
       </c>
@@ -7715,7 +7754,7 @@
       <c r="BP48" s="9"/>
       <c r="BQ48" s="9"/>
     </row>
-    <row r="49" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="49" spans="1:69" ht="16.5" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>98</v>
       </c>
@@ -7835,7 +7874,7 @@
       <c r="BP49" s="9"/>
       <c r="BQ49" s="9"/>
     </row>
-    <row r="50" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="50" spans="1:69" ht="16.5" thickBot="1">
       <c r="A50" s="24" t="s">
         <v>100</v>
       </c>
@@ -7911,7 +7950,7 @@
       <c r="BP50" s="9"/>
       <c r="BQ50" s="9"/>
     </row>
-    <row r="51" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="51" spans="1:69" ht="16.5" thickBot="1">
       <c r="A51" s="3" t="s">
         <v>102</v>
       </c>
@@ -8025,7 +8064,7 @@
       <c r="BP51" s="9"/>
       <c r="BQ51" s="9"/>
     </row>
-    <row r="52" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="52" spans="1:69" ht="16.5" thickBot="1">
       <c r="A52" s="3" t="s">
         <v>104</v>
       </c>
@@ -8133,7 +8172,7 @@
       <c r="BP52" s="9"/>
       <c r="BQ52" s="9"/>
     </row>
-    <row r="53" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="53" spans="1:69" ht="16.5" thickBot="1">
       <c r="A53" s="3" t="s">
         <v>106</v>
       </c>
@@ -8245,7 +8284,7 @@
       <c r="BP53" s="9"/>
       <c r="BQ53" s="9"/>
     </row>
-    <row r="54" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="54" spans="1:69" ht="16.5" thickBot="1">
       <c r="A54" s="3" t="s">
         <v>108</v>
       </c>
@@ -8359,7 +8398,7 @@
       <c r="BP54" s="9"/>
       <c r="BQ54" s="9"/>
     </row>
-    <row r="55" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="55" spans="1:69" ht="16.5" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
@@ -8471,7 +8510,7 @@
       <c r="BP55" s="9"/>
       <c r="BQ55" s="9"/>
     </row>
-    <row r="56" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="56" spans="1:69" ht="16.5" thickBot="1">
       <c r="A56" s="24" t="s">
         <v>112</v>
       </c>
@@ -8547,7 +8586,7 @@
       <c r="BP56" s="9"/>
       <c r="BQ56" s="9"/>
     </row>
-    <row r="57" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="57" spans="1:69" ht="16.5" thickBot="1">
       <c r="A57" s="3" t="s">
         <v>114</v>
       </c>
@@ -8661,7 +8700,7 @@
       <c r="BP57" s="9"/>
       <c r="BQ57" s="9"/>
     </row>
-    <row r="58" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="58" spans="1:69" ht="16.5" thickBot="1">
       <c r="A58" s="3" t="s">
         <v>116</v>
       </c>
@@ -8771,7 +8810,7 @@
       <c r="BP58" s="9"/>
       <c r="BQ58" s="9"/>
     </row>
-    <row r="59" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="59" spans="1:69" ht="16.5" thickBot="1">
       <c r="A59" s="3" t="s">
         <v>118</v>
       </c>
@@ -8879,7 +8918,7 @@
       <c r="BP59" s="9"/>
       <c r="BQ59" s="9"/>
     </row>
-    <row r="60" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="60" spans="1:69" ht="16.5" thickBot="1">
       <c r="A60" s="3" t="s">
         <v>120</v>
       </c>
@@ -8995,7 +9034,7 @@
       <c r="BP60" s="9"/>
       <c r="BQ60" s="9"/>
     </row>
-    <row r="61" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="61" spans="1:69" ht="16.5" thickBot="1">
       <c r="A61" s="3" t="s">
         <v>122</v>
       </c>
@@ -9113,7 +9152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="62" spans="1:69" ht="16.5" thickBot="1">
       <c r="A62" s="3" t="s">
         <v>124</v>
       </c>
@@ -9231,7 +9270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:69" ht="15.75" hidden="1" customHeight="1" thickBot="1">
+    <row r="63" spans="1:69" ht="15.75" customHeight="1" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>126</v>
       </c>
@@ -9341,7 +9380,7 @@
       <c r="BP63" s="9"/>
       <c r="BQ63" s="9"/>
     </row>
-    <row r="64" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="64" spans="1:69" ht="16.5" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>128</v>
       </c>
@@ -9457,7 +9496,7 @@
       <c r="BP64" s="9"/>
       <c r="BQ64" s="9"/>
     </row>
-    <row r="65" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="65" spans="1:69" ht="16.5" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>130</v>
       </c>
@@ -9581,7 +9620,7 @@
       <c r="BP65" s="9"/>
       <c r="BQ65" s="9"/>
     </row>
-    <row r="66" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="66" spans="1:69" ht="16.5" thickBot="1">
       <c r="A66" s="3" t="s">
         <v>132</v>
       </c>
@@ -9701,7 +9740,7 @@
       <c r="BP66" s="9"/>
       <c r="BQ66" s="9"/>
     </row>
-    <row r="67" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="67" spans="1:69" ht="16.5" thickBot="1">
       <c r="A67" s="3" t="s">
         <v>134</v>
       </c>
@@ -9817,7 +9856,7 @@
       <c r="BP67" s="9"/>
       <c r="BQ67" s="9"/>
     </row>
-    <row r="68" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="68" spans="1:69" ht="16.5" thickBot="1">
       <c r="A68" s="3" t="s">
         <v>137</v>
       </c>
@@ -9923,7 +9962,7 @@
       <c r="BP68" s="9"/>
       <c r="BQ68" s="9"/>
     </row>
-    <row r="69" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="69" spans="1:69" ht="16.5" thickBot="1">
       <c r="A69" s="24" t="s">
         <v>139</v>
       </c>
@@ -9999,7 +10038,7 @@
       <c r="BP69" s="9"/>
       <c r="BQ69" s="9"/>
     </row>
-    <row r="70" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="70" spans="1:69" ht="16.5" thickBot="1">
       <c r="A70" s="3" t="s">
         <v>141</v>
       </c>
@@ -10107,7 +10146,7 @@
       <c r="BP70" s="9"/>
       <c r="BQ70" s="9"/>
     </row>
-    <row r="71" spans="1:69" ht="32.25" hidden="1" thickBot="1">
+    <row r="71" spans="1:69" ht="32.25" thickBot="1">
       <c r="A71" s="3" t="s">
         <v>143</v>
       </c>
@@ -10219,7 +10258,7 @@
       <c r="BP71" s="9"/>
       <c r="BQ71" s="9"/>
     </row>
-    <row r="72" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="72" spans="1:69" ht="16.5" thickBot="1">
       <c r="A72" s="3" t="s">
         <v>145</v>
       </c>
@@ -10327,7 +10366,7 @@
       <c r="BP72" s="9"/>
       <c r="BQ72" s="9"/>
     </row>
-    <row r="73" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="73" spans="1:69" ht="16.5" thickBot="1">
       <c r="A73" s="3" t="s">
         <v>147</v>
       </c>
@@ -10439,7 +10478,7 @@
       <c r="BP73" s="9"/>
       <c r="BQ73" s="9"/>
     </row>
-    <row r="74" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="74" spans="1:69" ht="16.5" thickBot="1">
       <c r="A74" s="3" t="s">
         <v>149</v>
       </c>
@@ -10553,7 +10592,7 @@
       <c r="BP74" s="9"/>
       <c r="BQ74" s="9"/>
     </row>
-    <row r="75" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="75" spans="1:69" ht="16.5" thickBot="1">
       <c r="A75" s="3" t="s">
         <v>151</v>
       </c>
@@ -10671,7 +10710,7 @@
       <c r="BP75" s="9"/>
       <c r="BQ75" s="9"/>
     </row>
-    <row r="76" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="76" spans="1:69" ht="16.5" thickBot="1">
       <c r="A76" s="3" t="s">
         <v>153</v>
       </c>
@@ -10781,7 +10820,7 @@
       <c r="BP76" s="9"/>
       <c r="BQ76" s="9"/>
     </row>
-    <row r="77" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="77" spans="1:69" ht="16.5" thickBot="1">
       <c r="A77" s="3" t="s">
         <v>155</v>
       </c>
@@ -10891,7 +10930,7 @@
       <c r="BP77" s="9"/>
       <c r="BQ77" s="9"/>
     </row>
-    <row r="78" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="78" spans="1:69" ht="16.5" thickBot="1">
       <c r="A78" s="3" t="s">
         <v>157</v>
       </c>
@@ -11001,7 +11040,7 @@
       <c r="BP78" s="9"/>
       <c r="BQ78" s="9"/>
     </row>
-    <row r="79" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="79" spans="1:69" ht="16.5" thickBot="1">
       <c r="A79" s="3" t="s">
         <v>159</v>
       </c>
@@ -11125,7 +11164,7 @@
       <c r="BP79" s="9"/>
       <c r="BQ79" s="9"/>
     </row>
-    <row r="80" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="80" spans="1:69" ht="16.5" thickBot="1">
       <c r="A80" s="3" t="s">
         <v>161</v>
       </c>
@@ -11233,7 +11272,7 @@
       <c r="BP80" s="9"/>
       <c r="BQ80" s="9"/>
     </row>
-    <row r="81" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="81" spans="1:69" ht="16.5" thickBot="1">
       <c r="A81" s="24" t="s">
         <v>163</v>
       </c>
@@ -11309,7 +11348,7 @@
       <c r="BP81" s="9"/>
       <c r="BQ81" s="9"/>
     </row>
-    <row r="82" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="82" spans="1:69" ht="16.5" thickBot="1">
       <c r="A82" s="3" t="s">
         <v>165</v>
       </c>
@@ -11425,7 +11464,7 @@
       <c r="BP82" s="9"/>
       <c r="BQ82" s="9"/>
     </row>
-    <row r="83" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="83" spans="1:69" ht="16.5" thickBot="1">
       <c r="A83" s="3" t="s">
         <v>167</v>
       </c>
@@ -11539,7 +11578,7 @@
       <c r="BP83" s="9"/>
       <c r="BQ83" s="9"/>
     </row>
-    <row r="84" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="84" spans="1:69" ht="16.5" thickBot="1">
       <c r="A84" s="3" t="s">
         <v>169</v>
       </c>
@@ -11651,7 +11690,7 @@
       <c r="BP84" s="9"/>
       <c r="BQ84" s="9"/>
     </row>
-    <row r="85" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="85" spans="1:69" ht="16.5" thickBot="1">
       <c r="A85" s="3" t="s">
         <v>171</v>
       </c>
@@ -11763,7 +11802,7 @@
       <c r="BP85" s="9"/>
       <c r="BQ85" s="9"/>
     </row>
-    <row r="86" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="86" spans="1:69" ht="16.5" thickBot="1">
       <c r="A86" s="3" t="s">
         <v>173</v>
       </c>
@@ -11881,7 +11920,7 @@
       <c r="BP86" s="9"/>
       <c r="BQ86" s="9"/>
     </row>
-    <row r="87" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="87" spans="1:69" ht="16.5" thickBot="1">
       <c r="A87" s="3" t="s">
         <v>175</v>
       </c>
@@ -11995,7 +12034,7 @@
       <c r="BP87" s="9"/>
       <c r="BQ87" s="9"/>
     </row>
-    <row r="88" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="88" spans="1:69" ht="16.5" thickBot="1">
       <c r="A88" s="3" t="s">
         <v>177</v>
       </c>
@@ -12105,7 +12144,7 @@
       <c r="BP88" s="9"/>
       <c r="BQ88" s="9"/>
     </row>
-    <row r="89" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="89" spans="1:69" ht="16.5" thickBot="1">
       <c r="A89" s="3" t="s">
         <v>180</v>
       </c>
@@ -12231,7 +12270,7 @@
       <c r="BP89" s="9"/>
       <c r="BQ89" s="9"/>
     </row>
-    <row r="90" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="90" spans="1:69" ht="16.5" thickBot="1">
       <c r="A90" s="3" t="s">
         <v>182</v>
       </c>
@@ -12347,7 +12386,7 @@
       <c r="BP90" s="9"/>
       <c r="BQ90" s="9"/>
     </row>
-    <row r="91" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="91" spans="1:69" ht="16.5" thickBot="1">
       <c r="A91" s="14" t="s">
         <v>184</v>
       </c>
@@ -12424,7 +12463,7 @@
       <c r="BP91" s="9"/>
       <c r="BQ91" s="9"/>
     </row>
-    <row r="92" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="92" spans="1:69" ht="16.5" thickBot="1">
       <c r="A92" s="3" t="s">
         <v>187</v>
       </c>
@@ -12542,7 +12581,7 @@
       <c r="BP92" s="9"/>
       <c r="BQ92" s="9"/>
     </row>
-    <row r="93" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="93" spans="1:69" ht="16.5" thickBot="1">
       <c r="A93" s="3" t="s">
         <v>189</v>
       </c>
@@ -12660,7 +12699,7 @@
       <c r="BP93" s="9"/>
       <c r="BQ93" s="9"/>
     </row>
-    <row r="94" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="94" spans="1:69" ht="16.5" thickBot="1">
       <c r="A94" s="3" t="s">
         <v>191</v>
       </c>
@@ -12778,7 +12817,7 @@
       <c r="BP94" s="9"/>
       <c r="BQ94" s="9"/>
     </row>
-    <row r="95" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="95" spans="1:69" ht="16.5" thickBot="1">
       <c r="A95" s="3" t="s">
         <v>193</v>
       </c>
@@ -12892,7 +12931,7 @@
       <c r="BP95" s="9"/>
       <c r="BQ95" s="9"/>
     </row>
-    <row r="96" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="96" spans="1:69" ht="16.5" thickBot="1">
       <c r="A96" s="3" t="s">
         <v>195</v>
       </c>
@@ -13012,7 +13051,7 @@
       <c r="BP96" s="9"/>
       <c r="BQ96" s="9"/>
     </row>
-    <row r="97" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="97" spans="1:69" ht="16.5" thickBot="1">
       <c r="A97" s="3" t="s">
         <v>197</v>
       </c>
@@ -13130,7 +13169,7 @@
       <c r="BP97" s="9"/>
       <c r="BQ97" s="9"/>
     </row>
-    <row r="98" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="98" spans="1:69" ht="16.5" thickBot="1">
       <c r="A98" s="3" t="s">
         <v>199</v>
       </c>
@@ -13246,7 +13285,7 @@
       <c r="BP98" s="9"/>
       <c r="BQ98" s="9"/>
     </row>
-    <row r="99" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="99" spans="1:69" ht="16.5" thickBot="1">
       <c r="A99" s="3" t="s">
         <v>201</v>
       </c>
@@ -13358,7 +13397,7 @@
       <c r="BP99" s="9"/>
       <c r="BQ99" s="9"/>
     </row>
-    <row r="100" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="100" spans="1:69" ht="16.5" thickBot="1">
       <c r="A100" s="3" t="s">
         <v>203</v>
       </c>
@@ -13472,7 +13511,7 @@
       <c r="BP100" s="9"/>
       <c r="BQ100" s="9"/>
     </row>
-    <row r="101" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="101" spans="1:69" ht="16.5" thickBot="1">
       <c r="A101" s="3" t="s">
         <v>205</v>
       </c>
@@ -13588,7 +13627,7 @@
       <c r="BP101" s="9"/>
       <c r="BQ101" s="9"/>
     </row>
-    <row r="102" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="102" spans="1:69" ht="16.5" thickBot="1">
       <c r="A102" s="14" t="s">
         <v>207</v>
       </c>
@@ -13664,7 +13703,7 @@
       <c r="BP102" s="9"/>
       <c r="BQ102" s="9"/>
     </row>
-    <row r="103" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="103" spans="1:69" ht="16.5" thickBot="1">
       <c r="A103" s="14" t="s">
         <v>209</v>
       </c>
@@ -13740,7 +13779,7 @@
       <c r="BP103" s="9"/>
       <c r="BQ103" s="9"/>
     </row>
-    <row r="104" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="104" spans="1:69" ht="16.5" thickBot="1">
       <c r="A104" s="3" t="s">
         <v>211</v>
       </c>
@@ -13854,7 +13893,7 @@
       <c r="BP104" s="9"/>
       <c r="BQ104" s="9"/>
     </row>
-    <row r="105" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="105" spans="1:69" ht="16.5" thickBot="1">
       <c r="A105" s="3" t="s">
         <v>213</v>
       </c>
@@ -13972,7 +14011,7 @@
       <c r="BP105" s="9"/>
       <c r="BQ105" s="9"/>
     </row>
-    <row r="106" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="106" spans="1:69" ht="16.5" thickBot="1">
       <c r="A106" s="3" t="s">
         <v>215</v>
       </c>
@@ -14084,7 +14123,7 @@
       <c r="BP106" s="9"/>
       <c r="BQ106" s="9"/>
     </row>
-    <row r="107" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="107" spans="1:69" ht="16.5" thickBot="1">
       <c r="A107" s="3" t="s">
         <v>217</v>
       </c>
@@ -14198,7 +14237,7 @@
       <c r="BP107" s="9"/>
       <c r="BQ107" s="9"/>
     </row>
-    <row r="108" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="108" spans="1:69" ht="16.5" thickBot="1">
       <c r="A108" s="3" t="s">
         <v>219</v>
       </c>
@@ -14322,7 +14361,7 @@
       <c r="BP108" s="9"/>
       <c r="BQ108" s="9"/>
     </row>
-    <row r="109" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="109" spans="1:69" ht="16.5" thickBot="1">
       <c r="A109" s="29" t="s">
         <v>221</v>
       </c>
@@ -14398,7 +14437,7 @@
       <c r="BP109" s="9"/>
       <c r="BQ109" s="9"/>
     </row>
-    <row r="110" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="110" spans="1:69" ht="16.5" thickBot="1">
       <c r="A110" s="3" t="s">
         <v>224</v>
       </c>
@@ -14474,7 +14513,7 @@
       <c r="BP110" s="9"/>
       <c r="BQ110" s="9"/>
     </row>
-    <row r="111" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="111" spans="1:69" ht="16.5" thickBot="1">
       <c r="A111" s="3" t="s">
         <v>226</v>
       </c>
@@ -14550,7 +14589,7 @@
       <c r="BP111" s="9"/>
       <c r="BQ111" s="9"/>
     </row>
-    <row r="112" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="112" spans="1:69" ht="16.5" thickBot="1">
       <c r="A112" s="3" t="s">
         <v>228</v>
       </c>
@@ -14626,7 +14665,7 @@
       <c r="BP112" s="9"/>
       <c r="BQ112" s="9"/>
     </row>
-    <row r="113" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="113" spans="1:69" ht="16.5" thickBot="1">
       <c r="A113" s="3" t="s">
         <v>230</v>
       </c>
@@ -14702,7 +14741,7 @@
       <c r="BP113" s="9"/>
       <c r="BQ113" s="9"/>
     </row>
-    <row r="114" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="114" spans="1:69" ht="16.5" thickBot="1">
       <c r="A114" s="3" t="s">
         <v>232</v>
       </c>
@@ -14778,7 +14817,7 @@
       <c r="BP114" s="9"/>
       <c r="BQ114" s="9"/>
     </row>
-    <row r="115" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="115" spans="1:69" ht="16.5" thickBot="1">
       <c r="A115" s="3" t="s">
         <v>234</v>
       </c>
@@ -14854,7 +14893,7 @@
       <c r="BP115" s="9"/>
       <c r="BQ115" s="9"/>
     </row>
-    <row r="116" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="116" spans="1:69" ht="16.5" thickBot="1">
       <c r="A116" s="3" t="s">
         <v>235</v>
       </c>
@@ -14930,7 +14969,7 @@
       <c r="BP116" s="9"/>
       <c r="BQ116" s="9"/>
     </row>
-    <row r="117" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="117" spans="1:69" ht="16.5" thickBot="1">
       <c r="A117" s="3" t="s">
         <v>236</v>
       </c>
@@ -15006,7 +15045,7 @@
       <c r="BP117" s="9"/>
       <c r="BQ117" s="9"/>
     </row>
-    <row r="118" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="118" spans="1:69" ht="16.5" thickBot="1">
       <c r="A118" s="3" t="s">
         <v>238</v>
       </c>
@@ -15082,7 +15121,7 @@
       <c r="BP118" s="9"/>
       <c r="BQ118" s="9"/>
     </row>
-    <row r="119" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="119" spans="1:69" ht="16.5" thickBot="1">
       <c r="A119" s="3" t="s">
         <v>240</v>
       </c>
@@ -15158,7 +15197,7 @@
       <c r="BP119" s="9"/>
       <c r="BQ119" s="9"/>
     </row>
-    <row r="120" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="120" spans="1:69" ht="16.5" thickBot="1">
       <c r="A120" s="3" t="s">
         <v>242</v>
       </c>
@@ -15234,7 +15273,7 @@
       <c r="BP120" s="9"/>
       <c r="BQ120" s="9"/>
     </row>
-    <row r="121" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="121" spans="1:69" ht="16.5" thickBot="1">
       <c r="A121" s="3" t="s">
         <v>244</v>
       </c>
@@ -15310,7 +15349,7 @@
       <c r="BP121" s="9"/>
       <c r="BQ121" s="9"/>
     </row>
-    <row r="122" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="122" spans="1:69" ht="16.5" thickBot="1">
       <c r="A122" s="3" t="s">
         <v>246</v>
       </c>
@@ -15386,7 +15425,7 @@
       <c r="BP122" s="9"/>
       <c r="BQ122" s="9"/>
     </row>
-    <row r="123" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="123" spans="1:69" ht="16.5" thickBot="1">
       <c r="A123" s="3" t="s">
         <v>248</v>
       </c>
@@ -15462,7 +15501,7 @@
       <c r="BP123" s="9"/>
       <c r="BQ123" s="9"/>
     </row>
-    <row r="124" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="124" spans="1:69" ht="16.5" thickBot="1">
       <c r="A124" s="3" t="s">
         <v>250</v>
       </c>
@@ -15538,7 +15577,7 @@
       <c r="BP124" s="9"/>
       <c r="BQ124" s="9"/>
     </row>
-    <row r="125" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="125" spans="1:69" ht="16.5" thickBot="1">
       <c r="A125" s="3" t="s">
         <v>252</v>
       </c>
@@ -15614,7 +15653,7 @@
       <c r="BP125" s="9"/>
       <c r="BQ125" s="9"/>
     </row>
-    <row r="126" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="126" spans="1:69" ht="16.5" thickBot="1">
       <c r="A126" s="3" t="s">
         <v>254</v>
       </c>
@@ -15690,7 +15729,7 @@
       <c r="BP126" s="9"/>
       <c r="BQ126" s="9"/>
     </row>
-    <row r="127" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="127" spans="1:69" ht="16.5" thickBot="1">
       <c r="A127" s="3" t="s">
         <v>256</v>
       </c>
@@ -15766,7 +15805,7 @@
       <c r="BP127" s="9"/>
       <c r="BQ127" s="9"/>
     </row>
-    <row r="128" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="128" spans="1:69" ht="16.5" thickBot="1">
       <c r="A128" s="3" t="s">
         <v>258</v>
       </c>
@@ -15842,7 +15881,7 @@
       <c r="BP128" s="9"/>
       <c r="BQ128" s="9"/>
     </row>
-    <row r="129" spans="1:69" ht="32.25" hidden="1" thickBot="1">
+    <row r="129" spans="1:69" ht="32.25" thickBot="1">
       <c r="A129" s="3" t="s">
         <v>260</v>
       </c>
@@ -15918,7 +15957,7 @@
       <c r="BP129" s="9"/>
       <c r="BQ129" s="9"/>
     </row>
-    <row r="130" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="130" spans="1:69" ht="16.5" thickBot="1">
       <c r="A130" s="3" t="s">
         <v>262</v>
       </c>
@@ -16036,7 +16075,7 @@
       <c r="BP130" s="9"/>
       <c r="BQ130" s="9"/>
     </row>
-    <row r="131" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="131" spans="1:69" ht="16.5" thickBot="1">
       <c r="A131" s="3" t="s">
         <v>265</v>
       </c>
@@ -16156,7 +16195,7 @@
       <c r="BP131" s="9"/>
       <c r="BQ131" s="9"/>
     </row>
-    <row r="132" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="132" spans="1:69" ht="16.5" thickBot="1">
       <c r="A132" s="3" t="s">
         <v>267</v>
       </c>
@@ -16272,7 +16311,7 @@
       <c r="BP132" s="9"/>
       <c r="BQ132" s="9"/>
     </row>
-    <row r="133" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="133" spans="1:69" ht="16.5" thickBot="1">
       <c r="A133" s="3" t="s">
         <v>269</v>
       </c>
@@ -16390,7 +16429,7 @@
       <c r="BP133" s="9"/>
       <c r="BQ133" s="9"/>
     </row>
-    <row r="134" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="134" spans="1:69" ht="16.5" thickBot="1">
       <c r="A134" s="3" t="s">
         <v>271</v>
       </c>
@@ -16506,7 +16545,7 @@
       <c r="BP134" s="9"/>
       <c r="BQ134" s="9"/>
     </row>
-    <row r="135" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="135" spans="1:69" ht="16.5" thickBot="1">
       <c r="A135" s="3" t="s">
         <v>273</v>
       </c>
@@ -16618,7 +16657,7 @@
       <c r="BP135" s="9"/>
       <c r="BQ135" s="9"/>
     </row>
-    <row r="136" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="136" spans="1:69" ht="16.5" thickBot="1">
       <c r="A136" s="3" t="s">
         <v>275</v>
       </c>
@@ -16738,7 +16777,7 @@
       <c r="BP136" s="9"/>
       <c r="BQ136" s="9"/>
     </row>
-    <row r="137" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="137" spans="1:69" ht="16.5" thickBot="1">
       <c r="A137" s="3" t="s">
         <v>277</v>
       </c>
@@ -16854,7 +16893,7 @@
       <c r="BP137" s="9"/>
       <c r="BQ137" s="9"/>
     </row>
-    <row r="138" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="138" spans="1:69" ht="16.5" thickBot="1">
       <c r="A138" s="3" t="s">
         <v>279</v>
       </c>
@@ -16972,7 +17011,7 @@
       <c r="BP138" s="9"/>
       <c r="BQ138" s="9"/>
     </row>
-    <row r="139" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="139" spans="1:69" ht="16.5" thickBot="1">
       <c r="A139" s="3" t="s">
         <v>281</v>
       </c>
@@ -17086,7 +17125,7 @@
       <c r="BP139" s="9"/>
       <c r="BQ139" s="9"/>
     </row>
-    <row r="140" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="140" spans="1:69" ht="16.5" thickBot="1">
       <c r="A140" s="3" t="s">
         <v>283</v>
       </c>
@@ -17204,7 +17243,7 @@
       <c r="BP140" s="9"/>
       <c r="BQ140" s="9"/>
     </row>
-    <row r="141" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="141" spans="1:69" ht="16.5" thickBot="1">
       <c r="A141" s="3" t="s">
         <v>285</v>
       </c>
@@ -17314,7 +17353,7 @@
       <c r="BP141" s="9"/>
       <c r="BQ141" s="9"/>
     </row>
-    <row r="142" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="142" spans="1:69" ht="16.5" thickBot="1">
       <c r="A142" s="3" t="s">
         <v>287</v>
       </c>
@@ -17428,7 +17467,7 @@
       <c r="BP142" s="9"/>
       <c r="BQ142" s="9"/>
     </row>
-    <row r="143" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="143" spans="1:69" ht="16.5" thickBot="1">
       <c r="A143" s="3" t="s">
         <v>289</v>
       </c>
@@ -17544,7 +17583,7 @@
       <c r="BP143" s="9"/>
       <c r="BQ143" s="9"/>
     </row>
-    <row r="144" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="144" spans="1:69" ht="16.5" thickBot="1">
       <c r="A144" s="3" t="s">
         <v>291</v>
       </c>
@@ -17658,7 +17697,7 @@
       <c r="BP144" s="9"/>
       <c r="BQ144" s="9"/>
     </row>
-    <row r="145" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="145" spans="1:69" ht="16.5" thickBot="1">
       <c r="A145" s="3" t="s">
         <v>293</v>
       </c>
@@ -17778,7 +17817,7 @@
       <c r="BP145" s="9"/>
       <c r="BQ145" s="9"/>
     </row>
-    <row r="146" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="146" spans="1:69" ht="16.5" thickBot="1">
       <c r="A146" s="3" t="s">
         <v>295</v>
       </c>
@@ -17896,7 +17935,7 @@
       <c r="BP146" s="9"/>
       <c r="BQ146" s="9"/>
     </row>
-    <row r="147" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="147" spans="1:69" ht="16.5" thickBot="1">
       <c r="A147" s="3" t="s">
         <v>297</v>
       </c>
@@ -18010,7 +18049,7 @@
       <c r="BP147" s="9"/>
       <c r="BQ147" s="9"/>
     </row>
-    <row r="148" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="148" spans="1:69" ht="16.5" thickBot="1">
       <c r="A148" s="3" t="s">
         <v>299</v>
       </c>
@@ -18126,7 +18165,7 @@
       <c r="BP148" s="9"/>
       <c r="BQ148" s="9"/>
     </row>
-    <row r="149" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="149" spans="1:69" ht="16.5" thickBot="1">
       <c r="A149" s="3" t="s">
         <v>301</v>
       </c>
@@ -18246,7 +18285,7 @@
       <c r="BP149" s="9"/>
       <c r="BQ149" s="9"/>
     </row>
-    <row r="150" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="150" spans="1:69" ht="16.5" thickBot="1">
       <c r="A150" s="3" t="s">
         <v>303</v>
       </c>
@@ -18354,7 +18393,7 @@
       <c r="BP150" s="9"/>
       <c r="BQ150" s="9"/>
     </row>
-    <row r="151" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="151" spans="1:69" ht="16.5" thickBot="1">
       <c r="A151" s="3" t="s">
         <v>305</v>
       </c>
@@ -18464,7 +18503,7 @@
       <c r="BP151" s="9"/>
       <c r="BQ151" s="9"/>
     </row>
-    <row r="152" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="152" spans="1:69" ht="16.5" thickBot="1">
       <c r="A152" s="3" t="s">
         <v>308</v>
       </c>
@@ -18584,7 +18623,7 @@
       <c r="BP152" s="9"/>
       <c r="BQ152" s="9"/>
     </row>
-    <row r="153" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="153" spans="1:69" ht="16.5" thickBot="1">
       <c r="A153" s="3" t="s">
         <v>310</v>
       </c>
@@ -18694,7 +18733,7 @@
       <c r="BP153" s="9"/>
       <c r="BQ153" s="9"/>
     </row>
-    <row r="154" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="154" spans="1:69" ht="16.5" thickBot="1">
       <c r="A154" s="3" t="s">
         <v>312</v>
       </c>
@@ -18814,7 +18853,7 @@
       <c r="BP154" s="9"/>
       <c r="BQ154" s="9"/>
     </row>
-    <row r="155" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="155" spans="1:69" ht="16.5" thickBot="1">
       <c r="A155" s="3" t="s">
         <v>314</v>
       </c>
@@ -18934,7 +18973,7 @@
       <c r="BP155" s="9"/>
       <c r="BQ155" s="9"/>
     </row>
-    <row r="156" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="156" spans="1:69" ht="16.5" thickBot="1">
       <c r="A156" s="3" t="s">
         <v>316</v>
       </c>
@@ -19044,7 +19083,7 @@
       <c r="BP156" s="9"/>
       <c r="BQ156" s="9"/>
     </row>
-    <row r="157" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="157" spans="1:69" ht="16.5" thickBot="1">
       <c r="A157" s="3" t="s">
         <v>318</v>
       </c>
@@ -19166,7 +19205,7 @@
       <c r="BP157" s="9"/>
       <c r="BQ157" s="9"/>
     </row>
-    <row r="158" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="158" spans="1:69" ht="16.5" thickBot="1">
       <c r="A158" s="3" t="s">
         <v>320</v>
       </c>
@@ -19290,7 +19329,7 @@
       <c r="BP158" s="9"/>
       <c r="BQ158" s="9"/>
     </row>
-    <row r="159" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="159" spans="1:69" ht="16.5" thickBot="1">
       <c r="A159" s="24" t="s">
         <v>322</v>
       </c>
@@ -19366,7 +19405,7 @@
       <c r="BP159" s="9"/>
       <c r="BQ159" s="9"/>
     </row>
-    <row r="160" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="160" spans="1:69" ht="16.5" thickBot="1">
       <c r="A160" s="3" t="s">
         <v>324</v>
       </c>
@@ -19482,7 +19521,7 @@
       <c r="BP160" s="9"/>
       <c r="BQ160" s="9"/>
     </row>
-    <row r="161" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="161" spans="1:69" ht="16.5" thickBot="1">
       <c r="A161" s="3" t="s">
         <v>326</v>
       </c>
@@ -19598,7 +19637,7 @@
       <c r="BP161" s="9"/>
       <c r="BQ161" s="9"/>
     </row>
-    <row r="162" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="162" spans="1:69" ht="16.5" thickBot="1">
       <c r="A162" s="3" t="s">
         <v>328</v>
       </c>
@@ -19700,7 +19739,7 @@
       <c r="BP162" s="9"/>
       <c r="BQ162" s="9"/>
     </row>
-    <row r="163" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="163" spans="1:69" ht="16.5" thickBot="1">
       <c r="A163" s="3" t="s">
         <v>330</v>
       </c>
@@ -19816,7 +19855,7 @@
       <c r="BP163" s="9"/>
       <c r="BQ163" s="9"/>
     </row>
-    <row r="164" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="164" spans="1:69" ht="16.5" thickBot="1">
       <c r="A164" s="3" t="s">
         <v>332</v>
       </c>
@@ -19932,7 +19971,7 @@
       <c r="BP164" s="9"/>
       <c r="BQ164" s="9"/>
     </row>
-    <row r="165" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="165" spans="1:69" ht="16.5" thickBot="1">
       <c r="A165" s="3" t="s">
         <v>334</v>
       </c>
@@ -20036,7 +20075,7 @@
       <c r="BP165" s="9"/>
       <c r="BQ165" s="9"/>
     </row>
-    <row r="166" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="166" spans="1:69" ht="16.5" thickBot="1">
       <c r="A166" s="3" t="s">
         <v>336</v>
       </c>
@@ -20158,7 +20197,7 @@
       <c r="BP166" s="9"/>
       <c r="BQ166" s="9"/>
     </row>
-    <row r="167" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="167" spans="1:69" ht="16.5" thickBot="1">
       <c r="A167" s="14" t="s">
         <v>338</v>
       </c>
@@ -20234,7 +20273,7 @@
       <c r="BP167" s="9"/>
       <c r="BQ167" s="9"/>
     </row>
-    <row r="168" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="168" spans="1:69" ht="16.5" thickBot="1">
       <c r="A168" s="3" t="s">
         <v>340</v>
       </c>
@@ -20354,7 +20393,7 @@
       <c r="BP168" s="9"/>
       <c r="BQ168" s="9"/>
     </row>
-    <row r="169" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="169" spans="1:69" ht="16.5" thickBot="1">
       <c r="A169" s="3" t="s">
         <v>342</v>
       </c>
@@ -20468,7 +20507,7 @@
       <c r="BP169" s="9"/>
       <c r="BQ169" s="9"/>
     </row>
-    <row r="170" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="170" spans="1:69" ht="16.5" thickBot="1">
       <c r="A170" s="24" t="s">
         <v>344</v>
       </c>
@@ -20551,20 +20590,34 @@
       <c r="B171" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="C171" s="4"/>
+      <c r="C171" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D171" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E171" s="4"/>
-      <c r="F171" s="4"/>
-      <c r="G171" s="4"/>
-      <c r="I171" s="9"/>
+      <c r="E171" s="4">
+        <v>5344</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G171" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="I171" s="9">
+        <v>1</v>
+      </c>
       <c r="J171" s="9"/>
       <c r="K171" s="9"/>
-      <c r="L171" s="9"/>
+      <c r="L171" s="9">
+        <v>1</v>
+      </c>
       <c r="M171" s="11"/>
       <c r="N171" s="9"/>
-      <c r="O171" s="9"/>
+      <c r="O171" s="9">
+        <v>1</v>
+      </c>
       <c r="P171" s="9"/>
       <c r="Q171" s="9"/>
       <c r="R171" s="9"/>
@@ -20572,20 +20625,34 @@
       <c r="T171" s="11"/>
       <c r="U171" s="9"/>
       <c r="V171" s="9"/>
-      <c r="W171" s="9"/>
-      <c r="X171" s="9"/>
+      <c r="W171" s="9">
+        <v>1</v>
+      </c>
+      <c r="X171" s="9">
+        <v>1</v>
+      </c>
       <c r="Y171" s="11"/>
-      <c r="Z171" s="9"/>
-      <c r="AA171" s="9"/>
+      <c r="Z171" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA171" s="9">
+        <v>1</v>
+      </c>
       <c r="AB171" s="9"/>
       <c r="AC171" s="9"/>
-      <c r="AD171" s="9"/>
+      <c r="AD171" s="9">
+        <v>1</v>
+      </c>
       <c r="AE171" s="9"/>
       <c r="AF171" s="11"/>
       <c r="AG171" s="9"/>
-      <c r="AH171" s="9"/>
+      <c r="AH171" s="9">
+        <v>1</v>
+      </c>
       <c r="AI171" s="11"/>
-      <c r="AJ171" s="9"/>
+      <c r="AJ171" s="9">
+        <v>1</v>
+      </c>
       <c r="AK171" s="9"/>
       <c r="AL171" s="9"/>
       <c r="AM171" s="9"/>
@@ -20598,21 +20665,33 @@
       <c r="AT171" s="9"/>
       <c r="AU171" s="9"/>
       <c r="AV171" s="9"/>
-      <c r="AW171" s="9"/>
+      <c r="AW171" s="9">
+        <v>1</v>
+      </c>
       <c r="AX171" s="11"/>
       <c r="AY171" s="9"/>
-      <c r="AZ171" s="9"/>
+      <c r="AZ171" s="9">
+        <v>1</v>
+      </c>
       <c r="BA171" s="11"/>
-      <c r="BB171" s="9"/>
+      <c r="BB171" s="9">
+        <v>1</v>
+      </c>
       <c r="BC171" s="9"/>
       <c r="BD171" s="11"/>
-      <c r="BE171" s="9"/>
+      <c r="BE171" s="9">
+        <v>1</v>
+      </c>
       <c r="BF171" s="9"/>
       <c r="BG171" s="11"/>
-      <c r="BH171" s="9"/>
+      <c r="BH171" s="9">
+        <v>1</v>
+      </c>
       <c r="BI171" s="9"/>
       <c r="BJ171" s="11"/>
-      <c r="BK171" s="9"/>
+      <c r="BK171" s="9">
+        <v>1</v>
+      </c>
       <c r="BL171" s="9"/>
       <c r="BM171" s="11"/>
       <c r="BN171" s="9"/>
@@ -20627,41 +20706,69 @@
       <c r="B172" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="C172" s="4"/>
+      <c r="C172" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D172" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E172" s="4"/>
-      <c r="F172" s="4"/>
-      <c r="G172" s="4"/>
+      <c r="E172" s="4">
+        <v>7933</v>
+      </c>
+      <c r="F172" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="G172" s="4" t="s">
+        <v>534</v>
+      </c>
       <c r="I172" s="9"/>
-      <c r="J172" s="9"/>
+      <c r="J172" s="9">
+        <v>1</v>
+      </c>
       <c r="K172" s="9"/>
-      <c r="L172" s="9"/>
+      <c r="L172" s="9">
+        <v>1</v>
+      </c>
       <c r="M172" s="11"/>
-      <c r="N172" s="9"/>
+      <c r="N172" s="9">
+        <v>1</v>
+      </c>
       <c r="O172" s="9"/>
       <c r="P172" s="9"/>
       <c r="Q172" s="9"/>
       <c r="R172" s="9"/>
-      <c r="S172" s="9"/>
+      <c r="S172" s="9">
+        <v>1</v>
+      </c>
       <c r="T172" s="11"/>
       <c r="U172" s="9"/>
-      <c r="V172" s="9"/>
+      <c r="V172" s="9">
+        <v>1</v>
+      </c>
       <c r="W172" s="9"/>
-      <c r="X172" s="9"/>
+      <c r="X172" s="9">
+        <v>1</v>
+      </c>
       <c r="Y172" s="11"/>
-      <c r="Z172" s="9"/>
+      <c r="Z172" s="9">
+        <v>1</v>
+      </c>
       <c r="AA172" s="9"/>
       <c r="AB172" s="9"/>
-      <c r="AC172" s="9"/>
+      <c r="AC172" s="9">
+        <v>1</v>
+      </c>
       <c r="AD172" s="9"/>
       <c r="AE172" s="9"/>
       <c r="AF172" s="11"/>
-      <c r="AG172" s="9"/>
+      <c r="AG172" s="9">
+        <v>1</v>
+      </c>
       <c r="AH172" s="9"/>
       <c r="AI172" s="11"/>
-      <c r="AJ172" s="9"/>
+      <c r="AJ172" s="9">
+        <v>1</v>
+      </c>
       <c r="AK172" s="9"/>
       <c r="AL172" s="9"/>
       <c r="AM172" s="9"/>
@@ -20670,25 +20777,37 @@
       <c r="AP172" s="9"/>
       <c r="AQ172" s="9"/>
       <c r="AR172" s="11"/>
-      <c r="AS172" s="9"/>
+      <c r="AS172" s="9">
+        <v>1</v>
+      </c>
       <c r="AT172" s="9"/>
       <c r="AU172" s="9"/>
       <c r="AV172" s="9"/>
       <c r="AW172" s="9"/>
       <c r="AX172" s="11"/>
       <c r="AY172" s="9"/>
-      <c r="AZ172" s="9"/>
+      <c r="AZ172" s="9">
+        <v>1</v>
+      </c>
       <c r="BA172" s="11"/>
       <c r="BB172" s="9"/>
-      <c r="BC172" s="9"/>
+      <c r="BC172" s="9">
+        <v>1</v>
+      </c>
       <c r="BD172" s="11"/>
-      <c r="BE172" s="9"/>
+      <c r="BE172" s="9">
+        <v>1</v>
+      </c>
       <c r="BF172" s="9"/>
       <c r="BG172" s="11"/>
-      <c r="BH172" s="9"/>
+      <c r="BH172" s="9">
+        <v>1</v>
+      </c>
       <c r="BI172" s="9"/>
       <c r="BJ172" s="11"/>
-      <c r="BK172" s="9"/>
+      <c r="BK172" s="9">
+        <v>1</v>
+      </c>
       <c r="BL172" s="9"/>
       <c r="BM172" s="11"/>
       <c r="BN172" s="9"/>
@@ -20703,66 +20822,106 @@
       <c r="B173" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="C173" s="4"/>
+      <c r="C173" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D173" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E173" s="4"/>
-      <c r="F173" s="4"/>
-      <c r="G173" s="4"/>
-      <c r="I173" s="9"/>
-      <c r="J173" s="9"/>
+      <c r="E173" s="4">
+        <v>135</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="G173" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I173" s="9">
+        <v>1</v>
+      </c>
+      <c r="J173" s="9">
+        <v>1</v>
+      </c>
       <c r="K173" s="9"/>
       <c r="L173" s="9"/>
       <c r="M173" s="11"/>
       <c r="N173" s="9"/>
-      <c r="O173" s="9"/>
+      <c r="O173" s="9">
+        <v>1</v>
+      </c>
       <c r="P173" s="9"/>
       <c r="Q173" s="9"/>
       <c r="R173" s="9"/>
       <c r="S173" s="9"/>
       <c r="T173" s="11"/>
-      <c r="U173" s="9"/>
-      <c r="V173" s="9"/>
+      <c r="U173" s="9">
+        <v>1</v>
+      </c>
+      <c r="V173" s="9">
+        <v>1</v>
+      </c>
       <c r="W173" s="9"/>
       <c r="X173" s="9"/>
       <c r="Y173" s="11"/>
-      <c r="Z173" s="9"/>
-      <c r="AA173" s="9"/>
+      <c r="Z173" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA173" s="9">
+        <v>1</v>
+      </c>
       <c r="AB173" s="9"/>
       <c r="AC173" s="9"/>
       <c r="AD173" s="9"/>
       <c r="AE173" s="9"/>
       <c r="AF173" s="11"/>
       <c r="AG173" s="9"/>
-      <c r="AH173" s="9"/>
+      <c r="AH173" s="9">
+        <v>1</v>
+      </c>
       <c r="AI173" s="11"/>
       <c r="AJ173" s="9"/>
       <c r="AK173" s="9"/>
-      <c r="AL173" s="9"/>
-      <c r="AM173" s="9"/>
+      <c r="AL173" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM173" s="9">
+        <v>1</v>
+      </c>
       <c r="AN173" s="11"/>
       <c r="AO173" s="9"/>
       <c r="AP173" s="9"/>
-      <c r="AQ173" s="9"/>
+      <c r="AQ173" s="9">
+        <v>1</v>
+      </c>
       <c r="AR173" s="11"/>
       <c r="AS173" s="9"/>
       <c r="AT173" s="9"/>
       <c r="AU173" s="9"/>
       <c r="AV173" s="9"/>
-      <c r="AW173" s="9"/>
+      <c r="AW173" s="9">
+        <v>1</v>
+      </c>
       <c r="AX173" s="11"/>
       <c r="AY173" s="9"/>
-      <c r="AZ173" s="9"/>
+      <c r="AZ173" s="9">
+        <v>1</v>
+      </c>
       <c r="BA173" s="11"/>
       <c r="BB173" s="9"/>
-      <c r="BC173" s="9"/>
+      <c r="BC173" s="9">
+        <v>1</v>
+      </c>
       <c r="BD173" s="11"/>
-      <c r="BE173" s="9"/>
+      <c r="BE173" s="9">
+        <v>1</v>
+      </c>
       <c r="BF173" s="9"/>
       <c r="BG173" s="11"/>
       <c r="BH173" s="9"/>
-      <c r="BI173" s="9"/>
+      <c r="BI173" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ173" s="11"/>
       <c r="BK173" s="9"/>
       <c r="BL173" s="9"/>
@@ -20779,20 +20938,34 @@
       <c r="B174" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="C174" s="4"/>
+      <c r="C174" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D174" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E174" s="4"/>
-      <c r="F174" s="4"/>
-      <c r="G174" s="4"/>
-      <c r="I174" s="9"/>
+      <c r="E174" s="4">
+        <v>1958</v>
+      </c>
+      <c r="F174" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G174" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="I174" s="9">
+        <v>1</v>
+      </c>
       <c r="J174" s="9"/>
       <c r="K174" s="9"/>
-      <c r="L174" s="9"/>
+      <c r="L174" s="9">
+        <v>1</v>
+      </c>
       <c r="M174" s="11"/>
       <c r="N174" s="9"/>
-      <c r="O174" s="9"/>
+      <c r="O174" s="9">
+        <v>1</v>
+      </c>
       <c r="P174" s="9"/>
       <c r="Q174" s="9"/>
       <c r="R174" s="9"/>
@@ -20800,14 +20973,20 @@
       <c r="T174" s="11"/>
       <c r="U174" s="9"/>
       <c r="V174" s="9"/>
-      <c r="W174" s="9"/>
+      <c r="W174" s="9">
+        <v>1</v>
+      </c>
       <c r="X174" s="9"/>
       <c r="Y174" s="11"/>
-      <c r="Z174" s="9"/>
+      <c r="Z174" s="9">
+        <v>1</v>
+      </c>
       <c r="AA174" s="9"/>
       <c r="AB174" s="9"/>
       <c r="AC174" s="9"/>
-      <c r="AD174" s="9"/>
+      <c r="AD174" s="9">
+        <v>1</v>
+      </c>
       <c r="AE174" s="9"/>
       <c r="AF174" s="11"/>
       <c r="AG174" s="9"/>
@@ -20815,10 +20994,14 @@
       <c r="AI174" s="11"/>
       <c r="AJ174" s="9"/>
       <c r="AK174" s="9"/>
-      <c r="AL174" s="9"/>
+      <c r="AL174" s="9">
+        <v>1</v>
+      </c>
       <c r="AM174" s="9"/>
       <c r="AN174" s="11"/>
-      <c r="AO174" s="9"/>
+      <c r="AO174" s="9">
+        <v>1</v>
+      </c>
       <c r="AP174" s="9"/>
       <c r="AQ174" s="9"/>
       <c r="AR174" s="11"/>
@@ -20826,18 +21009,28 @@
       <c r="AT174" s="9"/>
       <c r="AU174" s="9"/>
       <c r="AV174" s="9"/>
-      <c r="AW174" s="9"/>
+      <c r="AW174" s="9">
+        <v>1</v>
+      </c>
       <c r="AX174" s="11"/>
       <c r="AY174" s="9"/>
-      <c r="AZ174" s="9"/>
+      <c r="AZ174" s="9">
+        <v>1</v>
+      </c>
       <c r="BA174" s="11"/>
       <c r="BB174" s="9"/>
-      <c r="BC174" s="9"/>
+      <c r="BC174" s="9">
+        <v>1</v>
+      </c>
       <c r="BD174" s="11"/>
       <c r="BE174" s="9"/>
-      <c r="BF174" s="9"/>
+      <c r="BF174" s="9">
+        <v>1</v>
+      </c>
       <c r="BG174" s="11"/>
-      <c r="BH174" s="9"/>
+      <c r="BH174" s="9">
+        <v>1</v>
+      </c>
       <c r="BI174" s="9"/>
       <c r="BJ174" s="11"/>
       <c r="BK174" s="9"/>
@@ -20855,46 +21048,82 @@
       <c r="B175" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C175" s="4"/>
+      <c r="C175" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D175" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E175" s="4"/>
-      <c r="F175" s="4"/>
-      <c r="G175" s="4"/>
-      <c r="I175" s="9"/>
-      <c r="J175" s="9"/>
-      <c r="K175" s="9"/>
-      <c r="L175" s="9"/>
+      <c r="E175" s="4">
+        <v>19758</v>
+      </c>
+      <c r="F175" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="G175" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="I175" s="9">
+        <v>1</v>
+      </c>
+      <c r="J175" s="9">
+        <v>1</v>
+      </c>
+      <c r="K175" s="9">
+        <v>1</v>
+      </c>
+      <c r="L175" s="9">
+        <v>1</v>
+      </c>
       <c r="M175" s="11"/>
-      <c r="N175" s="9"/>
+      <c r="N175" s="9">
+        <v>1</v>
+      </c>
       <c r="O175" s="9"/>
       <c r="P175" s="9"/>
       <c r="Q175" s="9"/>
       <c r="R175" s="9"/>
-      <c r="S175" s="9"/>
+      <c r="S175" s="9">
+        <v>1</v>
+      </c>
       <c r="T175" s="11"/>
       <c r="U175" s="9"/>
       <c r="V175" s="9"/>
       <c r="W175" s="9"/>
-      <c r="X175" s="9"/>
+      <c r="X175" s="9">
+        <v>1</v>
+      </c>
       <c r="Y175" s="11"/>
-      <c r="Z175" s="9"/>
-      <c r="AA175" s="9"/>
+      <c r="Z175" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA175" s="9">
+        <v>1</v>
+      </c>
       <c r="AB175" s="9"/>
       <c r="AC175" s="9"/>
-      <c r="AD175" s="9"/>
-      <c r="AE175" s="9"/>
+      <c r="AD175" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE175" s="9">
+        <v>1</v>
+      </c>
       <c r="AF175" s="11"/>
       <c r="AG175" s="9"/>
-      <c r="AH175" s="9"/>
+      <c r="AH175" s="9">
+        <v>1</v>
+      </c>
       <c r="AI175" s="11"/>
       <c r="AJ175" s="9"/>
       <c r="AK175" s="9"/>
-      <c r="AL175" s="9"/>
+      <c r="AL175" s="9">
+        <v>1</v>
+      </c>
       <c r="AM175" s="9"/>
       <c r="AN175" s="11"/>
-      <c r="AO175" s="9"/>
+      <c r="AO175" s="9">
+        <v>1</v>
+      </c>
       <c r="AP175" s="9"/>
       <c r="AQ175" s="9"/>
       <c r="AR175" s="11"/>
@@ -20902,21 +21131,33 @@
       <c r="AT175" s="9"/>
       <c r="AU175" s="9"/>
       <c r="AV175" s="9"/>
-      <c r="AW175" s="9"/>
+      <c r="AW175" s="9">
+        <v>1</v>
+      </c>
       <c r="AX175" s="11"/>
-      <c r="AY175" s="9"/>
+      <c r="AY175" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ175" s="9"/>
       <c r="BA175" s="11"/>
-      <c r="BB175" s="9"/>
+      <c r="BB175" s="9">
+        <v>1</v>
+      </c>
       <c r="BC175" s="9"/>
       <c r="BD175" s="11"/>
       <c r="BE175" s="9"/>
-      <c r="BF175" s="9"/>
+      <c r="BF175" s="9">
+        <v>1</v>
+      </c>
       <c r="BG175" s="11"/>
       <c r="BH175" s="9"/>
-      <c r="BI175" s="9"/>
+      <c r="BI175" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ175" s="11"/>
-      <c r="BK175" s="9"/>
+      <c r="BK175" s="9">
+        <v>1</v>
+      </c>
       <c r="BL175" s="9"/>
       <c r="BM175" s="11"/>
       <c r="BN175" s="9"/>
@@ -20931,31 +21172,49 @@
       <c r="B176" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="C176" s="4"/>
+      <c r="C176" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D176" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E176" s="4"/>
-      <c r="F176" s="4"/>
-      <c r="G176" s="4"/>
+      <c r="E176" s="4">
+        <v>498</v>
+      </c>
+      <c r="F176" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G176" s="4" t="s">
+        <v>543</v>
+      </c>
       <c r="I176" s="9"/>
       <c r="J176" s="9"/>
       <c r="K176" s="9"/>
-      <c r="L176" s="9"/>
+      <c r="L176" s="9">
+        <v>1</v>
+      </c>
       <c r="M176" s="11"/>
-      <c r="N176" s="9"/>
+      <c r="N176" s="9">
+        <v>1</v>
+      </c>
       <c r="O176" s="9"/>
       <c r="P176" s="9"/>
       <c r="Q176" s="9"/>
       <c r="R176" s="9"/>
-      <c r="S176" s="9"/>
+      <c r="S176" s="9">
+        <v>1</v>
+      </c>
       <c r="T176" s="11"/>
       <c r="U176" s="9"/>
       <c r="V176" s="9"/>
       <c r="W176" s="9"/>
-      <c r="X176" s="9"/>
+      <c r="X176" s="9">
+        <v>1</v>
+      </c>
       <c r="Y176" s="11"/>
-      <c r="Z176" s="9"/>
+      <c r="Z176" s="9">
+        <v>1</v>
+      </c>
       <c r="AA176" s="9"/>
       <c r="AB176" s="9"/>
       <c r="AC176" s="9"/>
@@ -20963,9 +21222,13 @@
       <c r="AE176" s="9"/>
       <c r="AF176" s="11"/>
       <c r="AG176" s="9"/>
-      <c r="AH176" s="9"/>
+      <c r="AH176" s="9">
+        <v>1</v>
+      </c>
       <c r="AI176" s="11"/>
-      <c r="AJ176" s="9"/>
+      <c r="AJ176" s="9">
+        <v>1</v>
+      </c>
       <c r="AK176" s="9"/>
       <c r="AL176" s="9"/>
       <c r="AM176" s="9"/>
@@ -20976,26 +21239,40 @@
       <c r="AR176" s="11"/>
       <c r="AS176" s="9"/>
       <c r="AT176" s="9"/>
-      <c r="AU176" s="9"/>
+      <c r="AU176" s="9">
+        <v>1</v>
+      </c>
       <c r="AV176" s="9"/>
       <c r="AW176" s="9"/>
       <c r="AX176" s="11"/>
       <c r="AY176" s="9"/>
-      <c r="AZ176" s="9"/>
+      <c r="AZ176" s="9">
+        <v>1</v>
+      </c>
       <c r="BA176" s="11"/>
       <c r="BB176" s="9"/>
-      <c r="BC176" s="9"/>
+      <c r="BC176" s="9">
+        <v>1</v>
+      </c>
       <c r="BD176" s="11"/>
       <c r="BE176" s="9"/>
-      <c r="BF176" s="9"/>
+      <c r="BF176" s="9">
+        <v>1</v>
+      </c>
       <c r="BG176" s="11"/>
-      <c r="BH176" s="9"/>
+      <c r="BH176" s="9">
+        <v>1</v>
+      </c>
       <c r="BI176" s="9"/>
       <c r="BJ176" s="11"/>
-      <c r="BK176" s="9"/>
+      <c r="BK176" s="9">
+        <v>1</v>
+      </c>
       <c r="BL176" s="9"/>
       <c r="BM176" s="11"/>
-      <c r="BN176" s="9"/>
+      <c r="BN176" s="9">
+        <v>1</v>
+      </c>
       <c r="BO176" s="9"/>
       <c r="BP176" s="9"/>
       <c r="BQ176" s="9"/>
@@ -21007,20 +21284,34 @@
       <c r="B177" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C177" s="4"/>
+      <c r="C177" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D177" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E177" s="4"/>
-      <c r="F177" s="4"/>
-      <c r="G177" s="4"/>
-      <c r="I177" s="9"/>
+      <c r="E177" s="4">
+        <v>20196</v>
+      </c>
+      <c r="F177" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G177" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="I177" s="9">
+        <v>1</v>
+      </c>
       <c r="J177" s="9"/>
       <c r="K177" s="9"/>
-      <c r="L177" s="9"/>
+      <c r="L177" s="9">
+        <v>1</v>
+      </c>
       <c r="M177" s="11"/>
       <c r="N177" s="9"/>
-      <c r="O177" s="9"/>
+      <c r="O177" s="9">
+        <v>1</v>
+      </c>
       <c r="P177" s="9"/>
       <c r="Q177" s="9"/>
       <c r="R177" s="9"/>
@@ -21028,47 +21319,70 @@
       <c r="T177" s="11"/>
       <c r="U177" s="9"/>
       <c r="V177" s="9"/>
-      <c r="W177" s="9"/>
+      <c r="W177" s="9">
+        <v>1</v>
+      </c>
       <c r="X177" s="9"/>
       <c r="Y177" s="11"/>
-      <c r="Z177" s="9"/>
+      <c r="Z177" s="9">
+        <v>1</v>
+      </c>
       <c r="AA177" s="9"/>
       <c r="AB177" s="9"/>
       <c r="AC177" s="9"/>
-      <c r="AD177" s="9"/>
+      <c r="AD177" s="9">
+        <v>1</v>
+      </c>
       <c r="AE177" s="9"/>
       <c r="AF177" s="11"/>
-      <c r="AG177" s="9"/>
+      <c r="AG177" s="9">
+        <v>1</v>
+      </c>
       <c r="AH177" s="9"/>
       <c r="AI177" s="11"/>
       <c r="AJ177" s="9"/>
       <c r="AK177" s="9"/>
-      <c r="AL177" s="9"/>
+      <c r="AL177" s="9">
+        <v>1</v>
+      </c>
       <c r="AM177" s="9"/>
       <c r="AN177" s="11"/>
-      <c r="AO177" s="9"/>
+      <c r="AO177" s="9">
+        <v>1</v>
+      </c>
       <c r="AP177" s="9"/>
       <c r="AQ177" s="9"/>
       <c r="AR177" s="11"/>
       <c r="AS177" s="9"/>
       <c r="AT177" s="9"/>
       <c r="AU177" s="9"/>
-      <c r="AV177" s="9"/>
-      <c r="AW177" s="9"/>
+      <c r="AW177" s="9">
+        <v>1</v>
+      </c>
       <c r="AX177" s="11"/>
       <c r="AY177" s="9"/>
-      <c r="AZ177" s="9"/>
+      <c r="AZ177" s="9">
+        <v>1</v>
+      </c>
       <c r="BA177" s="11"/>
-      <c r="BB177" s="9"/>
+      <c r="BB177" s="9">
+        <v>1</v>
+      </c>
       <c r="BC177" s="9"/>
       <c r="BD177" s="11"/>
-      <c r="BE177" s="9"/>
+      <c r="BE177" s="9">
+        <v>1</v>
+      </c>
       <c r="BF177" s="9"/>
       <c r="BG177" s="11"/>
-      <c r="BH177" s="9"/>
+      <c r="BH177" s="9">
+        <v>1</v>
+      </c>
       <c r="BI177" s="9"/>
       <c r="BJ177" s="11"/>
-      <c r="BK177" s="9"/>
+      <c r="BK177" s="9">
+        <v>1</v>
+      </c>
       <c r="BL177" s="9"/>
       <c r="BM177" s="11"/>
       <c r="BN177" s="9"/>
@@ -21083,27 +21397,43 @@
       <c r="B178" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C178" s="4"/>
+      <c r="C178" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D178" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E178" s="4"/>
-      <c r="F178" s="4"/>
-      <c r="G178" s="4"/>
+      <c r="E178" s="4">
+        <v>36</v>
+      </c>
+      <c r="F178" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="G178" s="4" t="s">
+        <v>552</v>
+      </c>
       <c r="I178" s="9"/>
       <c r="J178" s="9"/>
       <c r="K178" s="9"/>
-      <c r="L178" s="9"/>
+      <c r="L178" s="9">
+        <v>1</v>
+      </c>
       <c r="M178" s="11"/>
       <c r="N178" s="9"/>
-      <c r="O178" s="9"/>
+      <c r="O178" s="9">
+        <v>1</v>
+      </c>
       <c r="P178" s="9"/>
       <c r="Q178" s="9"/>
       <c r="R178" s="9"/>
       <c r="S178" s="9"/>
       <c r="T178" s="11"/>
-      <c r="U178" s="9"/>
-      <c r="V178" s="9"/>
+      <c r="U178" s="9">
+        <v>1</v>
+      </c>
+      <c r="V178" s="9">
+        <v>1</v>
+      </c>
       <c r="W178" s="9"/>
       <c r="X178" s="9"/>
       <c r="Y178" s="11"/>
@@ -21115,9 +21445,13 @@
       <c r="AE178" s="9"/>
       <c r="AF178" s="11"/>
       <c r="AG178" s="9"/>
-      <c r="AH178" s="9"/>
+      <c r="AH178" s="9">
+        <v>1</v>
+      </c>
       <c r="AI178" s="11"/>
-      <c r="AJ178" s="9"/>
+      <c r="AJ178" s="9">
+        <v>1</v>
+      </c>
       <c r="AK178" s="9"/>
       <c r="AL178" s="9"/>
       <c r="AM178" s="9"/>
@@ -21130,19 +21464,29 @@
       <c r="AT178" s="9"/>
       <c r="AU178" s="9"/>
       <c r="AV178" s="9"/>
-      <c r="AW178" s="9"/>
+      <c r="AW178" s="31">
+        <v>1</v>
+      </c>
       <c r="AX178" s="11"/>
       <c r="AY178" s="9"/>
-      <c r="AZ178" s="9"/>
+      <c r="AZ178" s="9">
+        <v>1</v>
+      </c>
       <c r="BA178" s="11"/>
       <c r="BB178" s="9"/>
-      <c r="BC178" s="9"/>
+      <c r="BC178" s="9">
+        <v>1</v>
+      </c>
       <c r="BD178" s="11"/>
       <c r="BE178" s="9"/>
-      <c r="BF178" s="9"/>
+      <c r="BF178" s="9">
+        <v>1</v>
+      </c>
       <c r="BG178" s="11"/>
       <c r="BH178" s="9"/>
-      <c r="BI178" s="9"/>
+      <c r="BI178" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ178" s="11"/>
       <c r="BK178" s="9"/>
       <c r="BL178" s="9"/>
@@ -21159,19 +21503,33 @@
       <c r="B179" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C179" s="4"/>
+      <c r="C179" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D179" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E179" s="4"/>
-      <c r="F179" s="4"/>
-      <c r="G179" s="4"/>
+      <c r="E179" s="4">
+        <v>1003</v>
+      </c>
+      <c r="F179" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="G179" s="4" t="s">
+        <v>533</v>
+      </c>
       <c r="I179" s="9"/>
-      <c r="J179" s="9"/>
+      <c r="J179" s="9">
+        <v>1</v>
+      </c>
       <c r="K179" s="9"/>
-      <c r="L179" s="9"/>
+      <c r="L179" s="9">
+        <v>1</v>
+      </c>
       <c r="M179" s="11"/>
-      <c r="N179" s="9"/>
+      <c r="N179" s="9">
+        <v>1</v>
+      </c>
       <c r="O179" s="9"/>
       <c r="P179" s="9"/>
       <c r="Q179" s="9"/>
@@ -21180,10 +21538,14 @@
       <c r="T179" s="11"/>
       <c r="U179" s="9"/>
       <c r="V179" s="9"/>
-      <c r="W179" s="9"/>
+      <c r="W179" s="9">
+        <v>1</v>
+      </c>
       <c r="X179" s="9"/>
       <c r="Y179" s="11"/>
-      <c r="Z179" s="9"/>
+      <c r="Z179" s="9">
+        <v>1</v>
+      </c>
       <c r="AA179" s="9"/>
       <c r="AB179" s="9"/>
       <c r="AC179" s="9"/>
@@ -21191,9 +21553,13 @@
       <c r="AE179" s="9"/>
       <c r="AF179" s="11"/>
       <c r="AG179" s="9"/>
-      <c r="AH179" s="9"/>
+      <c r="AH179" s="9">
+        <v>1</v>
+      </c>
       <c r="AI179" s="11"/>
-      <c r="AJ179" s="9"/>
+      <c r="AJ179" s="9">
+        <v>1</v>
+      </c>
       <c r="AK179" s="9"/>
       <c r="AL179" s="9"/>
       <c r="AM179" s="9"/>
@@ -21202,25 +21568,37 @@
       <c r="AP179" s="9"/>
       <c r="AQ179" s="9"/>
       <c r="AR179" s="11"/>
-      <c r="AS179" s="9"/>
+      <c r="AS179" s="9">
+        <v>1</v>
+      </c>
       <c r="AT179" s="9"/>
       <c r="AU179" s="9"/>
       <c r="AV179" s="9"/>
       <c r="AW179" s="9"/>
       <c r="AX179" s="11"/>
       <c r="AY179" s="9"/>
-      <c r="AZ179" s="9"/>
+      <c r="AZ179" s="9">
+        <v>1</v>
+      </c>
       <c r="BA179" s="11"/>
-      <c r="BB179" s="9"/>
+      <c r="BB179" s="9">
+        <v>1</v>
+      </c>
       <c r="BC179" s="9"/>
       <c r="BD179" s="11"/>
       <c r="BE179" s="9"/>
-      <c r="BF179" s="9"/>
+      <c r="BF179" s="9">
+        <v>1</v>
+      </c>
       <c r="BG179" s="11"/>
-      <c r="BH179" s="9"/>
+      <c r="BH179" s="9">
+        <v>1</v>
+      </c>
       <c r="BI179" s="9"/>
       <c r="BJ179" s="11"/>
-      <c r="BK179" s="9"/>
+      <c r="BK179" s="9">
+        <v>1</v>
+      </c>
       <c r="BL179" s="9"/>
       <c r="BM179" s="11"/>
       <c r="BN179" s="9"/>
@@ -21235,20 +21613,32 @@
       <c r="B180" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C180" s="4"/>
+      <c r="C180" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D180" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E180" s="4"/>
-      <c r="F180" s="4"/>
-      <c r="G180" s="4"/>
+      <c r="E180" s="4">
+        <v>920</v>
+      </c>
+      <c r="F180" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G180" s="4" t="s">
+        <v>534</v>
+      </c>
       <c r="I180" s="9"/>
       <c r="J180" s="9"/>
       <c r="K180" s="9"/>
-      <c r="L180" s="9"/>
+      <c r="L180" s="9">
+        <v>1</v>
+      </c>
       <c r="M180" s="11"/>
       <c r="N180" s="9"/>
-      <c r="O180" s="9"/>
+      <c r="O180" s="9">
+        <v>1</v>
+      </c>
       <c r="P180" s="9"/>
       <c r="Q180" s="9"/>
       <c r="R180" s="9"/>
@@ -21257,24 +21647,36 @@
       <c r="U180" s="9"/>
       <c r="V180" s="9"/>
       <c r="W180" s="9"/>
-      <c r="X180" s="9"/>
+      <c r="X180" s="9">
+        <v>1</v>
+      </c>
       <c r="Y180" s="11"/>
-      <c r="Z180" s="9"/>
+      <c r="Z180" s="9">
+        <v>1</v>
+      </c>
       <c r="AA180" s="9"/>
       <c r="AB180" s="9"/>
       <c r="AC180" s="9"/>
-      <c r="AD180" s="9"/>
+      <c r="AD180" s="9">
+        <v>1</v>
+      </c>
       <c r="AE180" s="9"/>
       <c r="AF180" s="11"/>
       <c r="AG180" s="9"/>
-      <c r="AH180" s="9"/>
+      <c r="AH180" s="9">
+        <v>1</v>
+      </c>
       <c r="AI180" s="11"/>
       <c r="AJ180" s="9"/>
       <c r="AK180" s="9"/>
-      <c r="AL180" s="9"/>
+      <c r="AL180" s="9">
+        <v>1</v>
+      </c>
       <c r="AM180" s="9"/>
       <c r="AN180" s="11"/>
-      <c r="AO180" s="9"/>
+      <c r="AO180" s="9">
+        <v>1</v>
+      </c>
       <c r="AP180" s="9"/>
       <c r="AQ180" s="9"/>
       <c r="AR180" s="11"/>
@@ -21282,18 +21684,28 @@
       <c r="AT180" s="9"/>
       <c r="AU180" s="9"/>
       <c r="AV180" s="9"/>
-      <c r="AW180" s="9"/>
+      <c r="AW180" s="9">
+        <v>1</v>
+      </c>
       <c r="AX180" s="11"/>
       <c r="AY180" s="9"/>
-      <c r="AZ180" s="9"/>
+      <c r="AZ180" s="9">
+        <v>1</v>
+      </c>
       <c r="BA180" s="11"/>
       <c r="BB180" s="9"/>
-      <c r="BC180" s="9"/>
+      <c r="BC180" s="9">
+        <v>1</v>
+      </c>
       <c r="BD180" s="11"/>
-      <c r="BE180" s="9"/>
+      <c r="BE180" s="9">
+        <v>1</v>
+      </c>
       <c r="BF180" s="9"/>
       <c r="BG180" s="11"/>
-      <c r="BH180" s="9"/>
+      <c r="BH180" s="9">
+        <v>1</v>
+      </c>
       <c r="BI180" s="9"/>
       <c r="BJ180" s="11"/>
       <c r="BK180" s="9"/>
@@ -21311,31 +21723,51 @@
       <c r="B181" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C181" s="4"/>
+      <c r="C181" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D181" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E181" s="4"/>
-      <c r="F181" s="4"/>
-      <c r="G181" s="4"/>
-      <c r="I181" s="9"/>
+      <c r="E181" s="4">
+        <v>142</v>
+      </c>
+      <c r="F181" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G181" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="I181" s="9">
+        <v>1</v>
+      </c>
       <c r="J181" s="9"/>
       <c r="K181" s="9"/>
-      <c r="L181" s="9"/>
+      <c r="L181" s="9">
+        <v>1</v>
+      </c>
       <c r="M181" s="11"/>
-      <c r="N181" s="9"/>
+      <c r="N181" s="9">
+        <v>1</v>
+      </c>
       <c r="O181" s="9"/>
       <c r="P181" s="9"/>
       <c r="Q181" s="9"/>
       <c r="R181" s="9"/>
-      <c r="S181" s="9"/>
+      <c r="S181" s="9">
+        <v>1</v>
+      </c>
       <c r="T181" s="11"/>
       <c r="U181" s="9"/>
       <c r="V181" s="9"/>
       <c r="W181" s="9"/>
-      <c r="X181" s="9"/>
+      <c r="X181" s="9">
+        <v>1</v>
+      </c>
       <c r="Y181" s="11"/>
-      <c r="Z181" s="9"/>
+      <c r="Z181" s="9">
+        <v>1</v>
+      </c>
       <c r="AA181" s="9"/>
       <c r="AB181" s="9"/>
       <c r="AC181" s="9"/>
@@ -21343,9 +21775,13 @@
       <c r="AE181" s="9"/>
       <c r="AF181" s="11"/>
       <c r="AG181" s="9"/>
-      <c r="AH181" s="9"/>
+      <c r="AH181" s="9">
+        <v>1</v>
+      </c>
       <c r="AI181" s="11"/>
-      <c r="AJ181" s="9"/>
+      <c r="AJ181" s="9">
+        <v>1</v>
+      </c>
       <c r="AK181" s="9"/>
       <c r="AL181" s="9"/>
       <c r="AM181" s="9"/>
@@ -21354,25 +21790,37 @@
       <c r="AP181" s="9"/>
       <c r="AQ181" s="9"/>
       <c r="AR181" s="11"/>
-      <c r="AS181" s="9"/>
+      <c r="AS181" s="9">
+        <v>1</v>
+      </c>
       <c r="AT181" s="9"/>
       <c r="AU181" s="9"/>
       <c r="AV181" s="9"/>
       <c r="AW181" s="9"/>
       <c r="AX181" s="11"/>
       <c r="AY181" s="9"/>
-      <c r="AZ181" s="9"/>
+      <c r="AZ181" s="9">
+        <v>1</v>
+      </c>
       <c r="BA181" s="11"/>
-      <c r="BB181" s="9"/>
+      <c r="BB181" s="9">
+        <v>1</v>
+      </c>
       <c r="BC181" s="9"/>
       <c r="BD181" s="11"/>
-      <c r="BE181" s="9"/>
+      <c r="BE181" s="9">
+        <v>1</v>
+      </c>
       <c r="BF181" s="9"/>
       <c r="BG181" s="11"/>
-      <c r="BH181" s="9"/>
+      <c r="BH181" s="9">
+        <v>1</v>
+      </c>
       <c r="BI181" s="9"/>
       <c r="BJ181" s="11"/>
-      <c r="BK181" s="9"/>
+      <c r="BK181" s="9">
+        <v>1</v>
+      </c>
       <c r="BL181" s="9"/>
       <c r="BM181" s="11"/>
       <c r="BN181" s="9"/>
@@ -21387,13 +21835,21 @@
       <c r="B182" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C182" s="4"/>
+      <c r="C182" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D182" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E182" s="4"/>
-      <c r="F182" s="4"/>
-      <c r="G182" s="4"/>
+      <c r="E182" s="4">
+        <v>515</v>
+      </c>
+      <c r="F182" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G182" s="4" t="s">
+        <v>533</v>
+      </c>
       <c r="I182" s="9"/>
       <c r="J182" s="9"/>
       <c r="K182" s="9"/>
@@ -21463,41 +21919,69 @@
       <c r="B183" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="C183" s="4"/>
+      <c r="C183" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D183" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E183" s="4"/>
-      <c r="F183" s="4"/>
-      <c r="G183" s="4"/>
-      <c r="I183" s="9"/>
+      <c r="E183" s="4">
+        <v>205</v>
+      </c>
+      <c r="F183" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="G183" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="I183" s="9">
+        <v>1</v>
+      </c>
       <c r="J183" s="9"/>
       <c r="K183" s="9"/>
-      <c r="L183" s="9"/>
+      <c r="L183" s="9">
+        <v>1</v>
+      </c>
       <c r="M183" s="11"/>
-      <c r="N183" s="9"/>
+      <c r="N183" s="9">
+        <v>1</v>
+      </c>
       <c r="O183" s="9"/>
       <c r="P183" s="9"/>
       <c r="Q183" s="9"/>
       <c r="R183" s="9"/>
-      <c r="S183" s="9"/>
+      <c r="S183" s="9">
+        <v>1</v>
+      </c>
       <c r="T183" s="11"/>
       <c r="U183" s="9"/>
       <c r="V183" s="9"/>
       <c r="W183" s="9"/>
-      <c r="X183" s="9"/>
+      <c r="X183" s="9">
+        <v>1</v>
+      </c>
       <c r="Y183" s="11"/>
       <c r="Z183" s="9"/>
-      <c r="AA183" s="9"/>
-      <c r="AB183" s="9"/>
+      <c r="AA183" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB183" s="9">
+        <v>1</v>
+      </c>
       <c r="AC183" s="9"/>
       <c r="AD183" s="9"/>
-      <c r="AE183" s="9"/>
+      <c r="AE183" s="9" t="s">
+        <v>567</v>
+      </c>
       <c r="AF183" s="11"/>
       <c r="AG183" s="9"/>
-      <c r="AH183" s="9"/>
+      <c r="AH183" s="9">
+        <v>1</v>
+      </c>
       <c r="AI183" s="11"/>
-      <c r="AJ183" s="9"/>
+      <c r="AJ183" s="9">
+        <v>1</v>
+      </c>
       <c r="AK183" s="9"/>
       <c r="AL183" s="9"/>
       <c r="AM183" s="9"/>
@@ -21506,25 +21990,37 @@
       <c r="AP183" s="9"/>
       <c r="AQ183" s="9"/>
       <c r="AR183" s="11"/>
-      <c r="AS183" s="9"/>
+      <c r="AS183" s="9">
+        <v>1</v>
+      </c>
       <c r="AT183" s="9"/>
       <c r="AU183" s="9"/>
       <c r="AV183" s="9"/>
       <c r="AW183" s="9"/>
       <c r="AX183" s="11"/>
       <c r="AY183" s="9"/>
-      <c r="AZ183" s="9"/>
+      <c r="AZ183" s="9">
+        <v>1</v>
+      </c>
       <c r="BA183" s="11"/>
       <c r="BB183" s="9"/>
-      <c r="BC183" s="9"/>
+      <c r="BC183" s="9">
+        <v>1</v>
+      </c>
       <c r="BD183" s="11"/>
-      <c r="BE183" s="9"/>
+      <c r="BE183" s="9">
+        <v>1</v>
+      </c>
       <c r="BF183" s="9"/>
       <c r="BG183" s="11"/>
       <c r="BH183" s="9"/>
-      <c r="BI183" s="9"/>
+      <c r="BI183" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ183" s="11"/>
-      <c r="BK183" s="9"/>
+      <c r="BK183" s="9">
+        <v>1</v>
+      </c>
       <c r="BL183" s="9"/>
       <c r="BM183" s="11"/>
       <c r="BN183" s="9"/>
@@ -21539,41 +22035,63 @@
       <c r="B184" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="C184" s="4"/>
+      <c r="C184" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D184" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E184" s="4"/>
-      <c r="F184" s="4"/>
-      <c r="G184" s="4"/>
+      <c r="E184" s="4">
+        <v>1993</v>
+      </c>
+      <c r="F184" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="G184" s="4" t="s">
+        <v>534</v>
+      </c>
       <c r="I184" s="9"/>
-      <c r="J184" s="9"/>
+      <c r="J184" s="9">
+        <v>1</v>
+      </c>
       <c r="K184" s="9"/>
       <c r="L184" s="9"/>
       <c r="M184" s="11"/>
       <c r="N184" s="9"/>
-      <c r="O184" s="9"/>
+      <c r="O184" s="9">
+        <v>1</v>
+      </c>
       <c r="P184" s="9"/>
       <c r="Q184" s="9"/>
       <c r="R184" s="9"/>
       <c r="S184" s="9"/>
       <c r="T184" s="11"/>
       <c r="U184" s="9"/>
-      <c r="V184" s="9"/>
+      <c r="V184" s="9">
+        <v>1</v>
+      </c>
       <c r="W184" s="9"/>
       <c r="X184" s="9"/>
       <c r="Y184" s="11"/>
       <c r="Z184" s="9"/>
-      <c r="AA184" s="9"/>
+      <c r="AA184" s="9">
+        <v>1</v>
+      </c>
       <c r="AB184" s="9"/>
       <c r="AC184" s="9"/>
-      <c r="AD184" s="9"/>
+      <c r="AD184" s="9">
+        <v>1</v>
+      </c>
       <c r="AE184" s="9"/>
       <c r="AF184" s="11"/>
       <c r="AG184" s="9"/>
-      <c r="AH184" s="9"/>
+      <c r="AH184" s="9">
+        <v>1</v>
+      </c>
       <c r="AI184" s="11"/>
-      <c r="AJ184" s="9"/>
+      <c r="AJ184" s="9">
+        <v>1</v>
+      </c>
       <c r="AK184" s="9"/>
       <c r="AL184" s="9"/>
       <c r="AM184" s="9"/>
@@ -21586,18 +22104,28 @@
       <c r="AT184" s="9"/>
       <c r="AU184" s="9"/>
       <c r="AV184" s="9"/>
-      <c r="AW184" s="9"/>
+      <c r="AW184" s="9">
+        <v>1</v>
+      </c>
       <c r="AX184" s="11"/>
       <c r="AY184" s="9"/>
-      <c r="AZ184" s="9"/>
+      <c r="AZ184" s="9">
+        <v>1</v>
+      </c>
       <c r="BA184" s="11"/>
       <c r="BB184" s="9"/>
-      <c r="BC184" s="9"/>
+      <c r="BC184" s="9">
+        <v>1</v>
+      </c>
       <c r="BD184" s="11"/>
       <c r="BE184" s="9"/>
-      <c r="BF184" s="9"/>
+      <c r="BF184" s="9">
+        <v>1</v>
+      </c>
       <c r="BG184" s="11"/>
-      <c r="BH184" s="9"/>
+      <c r="BH184" s="9">
+        <v>1</v>
+      </c>
       <c r="BI184" s="9"/>
       <c r="BJ184" s="11"/>
       <c r="BK184" s="9"/>
@@ -21615,41 +22143,71 @@
       <c r="B185" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="C185" s="4"/>
+      <c r="C185" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D185" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E185" s="4"/>
-      <c r="F185" s="4"/>
-      <c r="G185" s="4"/>
-      <c r="I185" s="9"/>
+      <c r="E185" s="4">
+        <v>8835</v>
+      </c>
+      <c r="F185" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G185" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="I185" s="9">
+        <v>1</v>
+      </c>
       <c r="J185" s="9"/>
       <c r="K185" s="9"/>
-      <c r="L185" s="9"/>
+      <c r="L185" s="9">
+        <v>1</v>
+      </c>
       <c r="M185" s="11"/>
       <c r="N185" s="9"/>
-      <c r="O185" s="9"/>
+      <c r="O185" s="9">
+        <v>1</v>
+      </c>
       <c r="P185" s="9"/>
       <c r="Q185" s="9"/>
       <c r="R185" s="9"/>
       <c r="S185" s="9"/>
       <c r="T185" s="11"/>
       <c r="U185" s="9"/>
-      <c r="V185" s="9"/>
+      <c r="V185" s="9">
+        <v>1</v>
+      </c>
       <c r="W185" s="9"/>
-      <c r="X185" s="9"/>
+      <c r="X185" s="9">
+        <v>1</v>
+      </c>
       <c r="Y185" s="11"/>
-      <c r="Z185" s="9"/>
-      <c r="AA185" s="9"/>
-      <c r="AB185" s="9"/>
+      <c r="Z185" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA185" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB185" s="9">
+        <v>1</v>
+      </c>
       <c r="AC185" s="9"/>
-      <c r="AD185" s="9"/>
+      <c r="AD185" s="9">
+        <v>1</v>
+      </c>
       <c r="AE185" s="9"/>
       <c r="AF185" s="11"/>
       <c r="AG185" s="9"/>
-      <c r="AH185" s="9"/>
+      <c r="AH185" s="9">
+        <v>1</v>
+      </c>
       <c r="AI185" s="11"/>
-      <c r="AJ185" s="9"/>
+      <c r="AJ185" s="9">
+        <v>1</v>
+      </c>
       <c r="AK185" s="9"/>
       <c r="AL185" s="9"/>
       <c r="AM185" s="9"/>
@@ -21662,21 +22220,33 @@
       <c r="AT185" s="9"/>
       <c r="AU185" s="9"/>
       <c r="AV185" s="9"/>
-      <c r="AW185" s="9"/>
+      <c r="AW185" s="9">
+        <v>1</v>
+      </c>
       <c r="AX185" s="11"/>
-      <c r="AY185" s="9"/>
+      <c r="AY185" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ185" s="9"/>
       <c r="BA185" s="11"/>
       <c r="BB185" s="9"/>
-      <c r="BC185" s="9"/>
+      <c r="BC185" s="9">
+        <v>1</v>
+      </c>
       <c r="BD185" s="11"/>
-      <c r="BE185" s="9"/>
+      <c r="BE185" s="9">
+        <v>1</v>
+      </c>
       <c r="BF185" s="9"/>
       <c r="BG185" s="11"/>
-      <c r="BH185" s="9"/>
+      <c r="BH185" s="9">
+        <v>1</v>
+      </c>
       <c r="BI185" s="9"/>
       <c r="BJ185" s="11"/>
-      <c r="BK185" s="9"/>
+      <c r="BK185" s="9">
+        <v>1</v>
+      </c>
       <c r="BL185" s="9"/>
       <c r="BM185" s="11"/>
       <c r="BN185" s="9"/>
@@ -21691,41 +22261,65 @@
       <c r="B186" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="C186" s="4"/>
+      <c r="C186" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D186" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E186" s="4"/>
-      <c r="F186" s="4"/>
-      <c r="G186" s="4"/>
+      <c r="E186" s="4">
+        <v>5084</v>
+      </c>
+      <c r="F186" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G186" s="4" t="s">
+        <v>538</v>
+      </c>
       <c r="I186" s="9"/>
-      <c r="J186" s="9"/>
+      <c r="J186" s="9">
+        <v>1</v>
+      </c>
       <c r="K186" s="9"/>
       <c r="L186" s="9"/>
       <c r="M186" s="11"/>
       <c r="N186" s="9"/>
-      <c r="O186" s="9"/>
+      <c r="O186" s="9">
+        <v>1</v>
+      </c>
       <c r="P186" s="9"/>
       <c r="Q186" s="9"/>
       <c r="R186" s="9"/>
       <c r="S186" s="9"/>
       <c r="T186" s="11"/>
       <c r="U186" s="9"/>
-      <c r="V186" s="9"/>
+      <c r="V186" s="9">
+        <v>1</v>
+      </c>
       <c r="W186" s="9"/>
-      <c r="X186" s="9"/>
+      <c r="X186" s="9">
+        <v>1</v>
+      </c>
       <c r="Y186" s="11"/>
-      <c r="Z186" s="9"/>
+      <c r="Z186" s="9">
+        <v>1</v>
+      </c>
       <c r="AA186" s="9"/>
-      <c r="AB186" s="9"/>
+      <c r="AB186" s="9">
+        <v>1</v>
+      </c>
       <c r="AC186" s="9"/>
       <c r="AD186" s="9"/>
       <c r="AE186" s="9"/>
       <c r="AF186" s="11"/>
       <c r="AG186" s="9"/>
-      <c r="AH186" s="9"/>
+      <c r="AH186" s="9">
+        <v>1</v>
+      </c>
       <c r="AI186" s="11"/>
-      <c r="AJ186" s="9"/>
+      <c r="AJ186" s="9">
+        <v>1</v>
+      </c>
       <c r="AK186" s="9"/>
       <c r="AL186" s="9"/>
       <c r="AM186" s="9"/>
@@ -21738,21 +22332,33 @@
       <c r="AT186" s="9"/>
       <c r="AU186" s="9"/>
       <c r="AV186" s="9"/>
-      <c r="AW186" s="9"/>
+      <c r="AW186" s="9">
+        <v>1</v>
+      </c>
       <c r="AX186" s="11"/>
-      <c r="AY186" s="9"/>
+      <c r="AY186" s="9">
+        <v>1</v>
+      </c>
       <c r="AZ186" s="9"/>
       <c r="BA186" s="11"/>
-      <c r="BB186" s="9"/>
+      <c r="BB186" s="9">
+        <v>1</v>
+      </c>
       <c r="BC186" s="9"/>
       <c r="BD186" s="11"/>
       <c r="BE186" s="9"/>
-      <c r="BF186" s="9"/>
+      <c r="BF186" s="9">
+        <v>1</v>
+      </c>
       <c r="BG186" s="11"/>
-      <c r="BH186" s="9"/>
+      <c r="BH186" s="9">
+        <v>1</v>
+      </c>
       <c r="BI186" s="9"/>
       <c r="BJ186" s="11"/>
-      <c r="BK186" s="9"/>
+      <c r="BK186" s="9">
+        <v>1</v>
+      </c>
       <c r="BL186" s="9"/>
       <c r="BM186" s="11"/>
       <c r="BN186" s="9"/>
@@ -21767,46 +22373,72 @@
       <c r="B187" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="C187" s="4"/>
+      <c r="C187" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D187" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E187" s="4"/>
-      <c r="F187" s="4"/>
-      <c r="G187" s="4"/>
+      <c r="E187" s="4">
+        <v>9131</v>
+      </c>
+      <c r="F187" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="G187" s="4" t="s">
+        <v>538</v>
+      </c>
       <c r="I187" s="9"/>
       <c r="J187" s="9"/>
       <c r="K187" s="9"/>
-      <c r="L187" s="9"/>
+      <c r="L187" s="9">
+        <v>1</v>
+      </c>
       <c r="M187" s="11"/>
       <c r="N187" s="9"/>
-      <c r="O187" s="9"/>
+      <c r="O187" s="9">
+        <v>1</v>
+      </c>
       <c r="P187" s="9"/>
       <c r="Q187" s="9"/>
       <c r="R187" s="9"/>
       <c r="S187" s="9"/>
       <c r="T187" s="11"/>
       <c r="U187" s="9"/>
-      <c r="V187" s="9"/>
+      <c r="V187" s="9">
+        <v>1</v>
+      </c>
       <c r="W187" s="9"/>
       <c r="X187" s="9"/>
       <c r="Y187" s="11"/>
-      <c r="Z187" s="9"/>
+      <c r="Z187" s="9">
+        <v>1</v>
+      </c>
       <c r="AA187" s="9"/>
       <c r="AB187" s="9"/>
       <c r="AC187" s="9"/>
-      <c r="AD187" s="9"/>
+      <c r="AD187" s="9">
+        <v>1</v>
+      </c>
       <c r="AE187" s="9"/>
       <c r="AF187" s="11"/>
       <c r="AG187" s="9"/>
-      <c r="AH187" s="9"/>
+      <c r="AH187" s="9">
+        <v>1</v>
+      </c>
       <c r="AI187" s="11"/>
       <c r="AJ187" s="9"/>
       <c r="AK187" s="9"/>
-      <c r="AL187" s="9"/>
-      <c r="AM187" s="9"/>
+      <c r="AL187" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM187" s="9">
+        <v>1</v>
+      </c>
       <c r="AN187" s="11"/>
-      <c r="AO187" s="9"/>
+      <c r="AO187" s="9">
+        <v>1</v>
+      </c>
       <c r="AP187" s="9"/>
       <c r="AQ187" s="9"/>
       <c r="AR187" s="11"/>
@@ -21814,21 +22446,33 @@
       <c r="AT187" s="9"/>
       <c r="AU187" s="9"/>
       <c r="AV187" s="9"/>
-      <c r="AW187" s="9"/>
+      <c r="AW187" s="9">
+        <v>1</v>
+      </c>
       <c r="AX187" s="11"/>
       <c r="AY187" s="9"/>
-      <c r="AZ187" s="9"/>
+      <c r="AZ187" s="9">
+        <v>1</v>
+      </c>
       <c r="BA187" s="11"/>
       <c r="BB187" s="9"/>
-      <c r="BC187" s="9"/>
+      <c r="BC187" s="9">
+        <v>1</v>
+      </c>
       <c r="BD187" s="11"/>
       <c r="BE187" s="9"/>
-      <c r="BF187" s="9"/>
+      <c r="BF187" s="9">
+        <v>1</v>
+      </c>
       <c r="BG187" s="11"/>
-      <c r="BH187" s="9"/>
+      <c r="BH187" s="9">
+        <v>1</v>
+      </c>
       <c r="BI187" s="9"/>
       <c r="BJ187" s="11"/>
-      <c r="BK187" s="9"/>
+      <c r="BK187" s="9">
+        <v>1</v>
+      </c>
       <c r="BL187" s="9"/>
       <c r="BM187" s="11"/>
       <c r="BN187" s="9"/>
@@ -21843,46 +22487,66 @@
       <c r="B188" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C188" s="4"/>
+      <c r="C188" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D188" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E188" s="4"/>
-      <c r="F188" s="4"/>
-      <c r="G188" s="4"/>
+      <c r="E188" s="4">
+        <v>5885</v>
+      </c>
+      <c r="F188" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G188" s="4" t="s">
+        <v>541</v>
+      </c>
       <c r="I188" s="9"/>
       <c r="J188" s="9"/>
       <c r="K188" s="9"/>
       <c r="L188" s="9"/>
       <c r="M188" s="11"/>
       <c r="N188" s="9"/>
-      <c r="O188" s="9"/>
+      <c r="O188" s="9">
+        <v>1</v>
+      </c>
       <c r="P188" s="9"/>
       <c r="Q188" s="9"/>
       <c r="R188" s="9"/>
       <c r="S188" s="9"/>
       <c r="T188" s="11"/>
       <c r="U188" s="9"/>
-      <c r="V188" s="9"/>
+      <c r="V188" s="9">
+        <v>1</v>
+      </c>
       <c r="W188" s="9"/>
       <c r="X188" s="9"/>
       <c r="Y188" s="11"/>
       <c r="Z188" s="9"/>
-      <c r="AA188" s="9"/>
+      <c r="AA188" s="9">
+        <v>1</v>
+      </c>
       <c r="AB188" s="9"/>
       <c r="AC188" s="9"/>
       <c r="AD188" s="9"/>
       <c r="AE188" s="9"/>
       <c r="AF188" s="11"/>
       <c r="AG188" s="9"/>
-      <c r="AH188" s="9"/>
+      <c r="AH188" s="9">
+        <v>1</v>
+      </c>
       <c r="AI188" s="11"/>
       <c r="AJ188" s="9"/>
       <c r="AK188" s="9"/>
-      <c r="AL188" s="9"/>
+      <c r="AL188" s="9">
+        <v>1</v>
+      </c>
       <c r="AM188" s="9"/>
       <c r="AN188" s="11"/>
-      <c r="AO188" s="9"/>
+      <c r="AO188" s="9">
+        <v>1</v>
+      </c>
       <c r="AP188" s="9"/>
       <c r="AQ188" s="9"/>
       <c r="AR188" s="11"/>
@@ -21890,21 +22554,33 @@
       <c r="AT188" s="9"/>
       <c r="AU188" s="9"/>
       <c r="AV188" s="9"/>
-      <c r="AW188" s="9"/>
+      <c r="AW188" s="9">
+        <v>1</v>
+      </c>
       <c r="AX188" s="11"/>
       <c r="AY188" s="9"/>
-      <c r="AZ188" s="9"/>
+      <c r="AZ188" s="9">
+        <v>1</v>
+      </c>
       <c r="BA188" s="11"/>
-      <c r="BB188" s="9"/>
+      <c r="BB188" s="9">
+        <v>1</v>
+      </c>
       <c r="BC188" s="9"/>
       <c r="BD188" s="11"/>
       <c r="BE188" s="9"/>
-      <c r="BF188" s="9"/>
+      <c r="BF188" s="9">
+        <v>1</v>
+      </c>
       <c r="BG188" s="11"/>
-      <c r="BH188" s="9"/>
+      <c r="BH188" s="9">
+        <v>1</v>
+      </c>
       <c r="BI188" s="9"/>
       <c r="BJ188" s="11"/>
-      <c r="BK188" s="9"/>
+      <c r="BK188" s="9">
+        <v>1</v>
+      </c>
       <c r="BL188" s="9"/>
       <c r="BM188" s="11"/>
       <c r="BN188" s="9"/>
@@ -21919,31 +22595,47 @@
       <c r="B189" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C189" s="4"/>
+      <c r="C189" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D189" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E189" s="4"/>
-      <c r="F189" s="4"/>
-      <c r="G189" s="4"/>
+      <c r="E189" s="4">
+        <v>164</v>
+      </c>
+      <c r="F189" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G189" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="I189" s="9"/>
       <c r="J189" s="9"/>
       <c r="K189" s="9"/>
-      <c r="L189" s="9"/>
+      <c r="L189" s="9">
+        <v>1</v>
+      </c>
       <c r="M189" s="11"/>
       <c r="N189" s="9"/>
-      <c r="O189" s="9"/>
+      <c r="O189" s="9">
+        <v>1</v>
+      </c>
       <c r="P189" s="9"/>
       <c r="Q189" s="9"/>
       <c r="R189" s="9"/>
       <c r="S189" s="9"/>
       <c r="T189" s="11"/>
       <c r="U189" s="9"/>
-      <c r="V189" s="9"/>
+      <c r="V189" s="9">
+        <v>1</v>
+      </c>
       <c r="W189" s="9"/>
       <c r="X189" s="9"/>
       <c r="Y189" s="11"/>
-      <c r="Z189" s="9"/>
+      <c r="Z189" s="9">
+        <v>1</v>
+      </c>
       <c r="AA189" s="9"/>
       <c r="AB189" s="9"/>
       <c r="AC189" s="9"/>
@@ -21951,9 +22643,13 @@
       <c r="AE189" s="9"/>
       <c r="AF189" s="11"/>
       <c r="AG189" s="9"/>
-      <c r="AH189" s="9"/>
+      <c r="AH189" s="9">
+        <v>1</v>
+      </c>
       <c r="AI189" s="11"/>
-      <c r="AJ189" s="9"/>
+      <c r="AJ189" s="9">
+        <v>1</v>
+      </c>
       <c r="AK189" s="9"/>
       <c r="AL189" s="9"/>
       <c r="AM189" s="9"/>
@@ -21966,21 +22662,33 @@
       <c r="AT189" s="9"/>
       <c r="AU189" s="9"/>
       <c r="AV189" s="9"/>
-      <c r="AW189" s="9"/>
+      <c r="AW189" s="9">
+        <v>1</v>
+      </c>
       <c r="AX189" s="11"/>
       <c r="AY189" s="9"/>
-      <c r="AZ189" s="9"/>
+      <c r="AZ189" s="9">
+        <v>1</v>
+      </c>
       <c r="BA189" s="11"/>
       <c r="BB189" s="9"/>
-      <c r="BC189" s="9"/>
+      <c r="BC189" s="9">
+        <v>1</v>
+      </c>
       <c r="BD189" s="11"/>
       <c r="BE189" s="9"/>
-      <c r="BF189" s="9"/>
+      <c r="BF189" s="9">
+        <v>1</v>
+      </c>
       <c r="BG189" s="11"/>
-      <c r="BH189" s="9"/>
+      <c r="BH189" s="9">
+        <v>1</v>
+      </c>
       <c r="BI189" s="9"/>
       <c r="BJ189" s="11"/>
-      <c r="BK189" s="9"/>
+      <c r="BK189" s="9">
+        <v>1</v>
+      </c>
       <c r="BL189" s="9"/>
       <c r="BM189" s="11"/>
       <c r="BN189" s="9"/>
@@ -21995,41 +22703,63 @@
       <c r="B190" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="C190" s="4"/>
+      <c r="C190" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D190" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E190" s="4"/>
-      <c r="F190" s="4"/>
-      <c r="G190" s="4"/>
+      <c r="E190" s="4">
+        <v>52</v>
+      </c>
+      <c r="F190" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="G190" s="4" t="s">
+        <v>552</v>
+      </c>
       <c r="I190" s="9"/>
       <c r="J190" s="9"/>
       <c r="K190" s="9"/>
       <c r="L190" s="9"/>
       <c r="M190" s="11"/>
       <c r="N190" s="9"/>
-      <c r="O190" s="9"/>
+      <c r="O190" s="9">
+        <v>1</v>
+      </c>
       <c r="P190" s="9"/>
       <c r="Q190" s="9"/>
       <c r="R190" s="9"/>
       <c r="S190" s="9"/>
       <c r="T190" s="11"/>
-      <c r="U190" s="9"/>
+      <c r="U190" s="9">
+        <v>1</v>
+      </c>
       <c r="V190" s="9"/>
-      <c r="W190" s="9"/>
+      <c r="W190" s="9">
+        <v>1</v>
+      </c>
       <c r="X190" s="9"/>
       <c r="Y190" s="11"/>
       <c r="Z190" s="9"/>
-      <c r="AA190" s="9"/>
+      <c r="AA190" s="9">
+        <v>1</v>
+      </c>
       <c r="AB190" s="9"/>
       <c r="AC190" s="9"/>
-      <c r="AD190" s="9"/>
+      <c r="AD190" s="9">
+        <v>1</v>
+      </c>
       <c r="AE190" s="9"/>
       <c r="AF190" s="11"/>
       <c r="AG190" s="9"/>
-      <c r="AH190" s="9"/>
+      <c r="AH190" s="9">
+        <v>1</v>
+      </c>
       <c r="AI190" s="11"/>
-      <c r="AJ190" s="9"/>
+      <c r="AJ190" s="9">
+        <v>1</v>
+      </c>
       <c r="AK190" s="9"/>
       <c r="AL190" s="9"/>
       <c r="AM190" s="9"/>
@@ -22042,18 +22772,28 @@
       <c r="AT190" s="9"/>
       <c r="AU190" s="9"/>
       <c r="AV190" s="9"/>
-      <c r="AW190" s="9"/>
+      <c r="AW190" s="9">
+        <v>1</v>
+      </c>
       <c r="AX190" s="11"/>
       <c r="AY190" s="9"/>
-      <c r="AZ190" s="9"/>
+      <c r="AZ190" s="9">
+        <v>1</v>
+      </c>
       <c r="BA190" s="11"/>
-      <c r="BB190" s="9"/>
+      <c r="BB190" s="9">
+        <v>1</v>
+      </c>
       <c r="BC190" s="9"/>
       <c r="BD190" s="11"/>
       <c r="BE190" s="9"/>
-      <c r="BF190" s="9"/>
+      <c r="BF190" s="9">
+        <v>1</v>
+      </c>
       <c r="BG190" s="11"/>
-      <c r="BH190" s="9"/>
+      <c r="BH190" s="9">
+        <v>1</v>
+      </c>
       <c r="BI190" s="9"/>
       <c r="BJ190" s="11"/>
       <c r="BK190" s="9"/>
@@ -22071,27 +22811,39 @@
       <c r="B191" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="C191" s="4"/>
+      <c r="C191" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D191" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E191" s="4"/>
-      <c r="F191" s="4"/>
-      <c r="G191" s="4"/>
+      <c r="E191" s="4">
+        <v>559</v>
+      </c>
+      <c r="F191" s="4">
+        <v>36</v>
+      </c>
+      <c r="G191" s="4" t="s">
+        <v>533</v>
+      </c>
       <c r="I191" s="9"/>
       <c r="J191" s="9"/>
       <c r="K191" s="9"/>
       <c r="L191" s="9"/>
       <c r="M191" s="11"/>
       <c r="N191" s="9"/>
-      <c r="O191" s="9"/>
+      <c r="O191" s="9">
+        <v>1</v>
+      </c>
       <c r="P191" s="9"/>
       <c r="Q191" s="9"/>
       <c r="R191" s="9"/>
       <c r="S191" s="9"/>
       <c r="T191" s="11"/>
       <c r="U191" s="9"/>
-      <c r="V191" s="9"/>
+      <c r="V191" s="9">
+        <v>1</v>
+      </c>
       <c r="W191" s="9"/>
       <c r="X191" s="9"/>
       <c r="Y191" s="11"/>
@@ -22103,9 +22855,13 @@
       <c r="AE191" s="9"/>
       <c r="AF191" s="11"/>
       <c r="AG191" s="9"/>
-      <c r="AH191" s="9"/>
+      <c r="AH191" s="9">
+        <v>1</v>
+      </c>
       <c r="AI191" s="11"/>
-      <c r="AJ191" s="9"/>
+      <c r="AJ191" s="9">
+        <v>1</v>
+      </c>
       <c r="AK191" s="9"/>
       <c r="AL191" s="9"/>
       <c r="AM191" s="9"/>
@@ -22118,19 +22874,29 @@
       <c r="AT191" s="9"/>
       <c r="AU191" s="9"/>
       <c r="AV191" s="9"/>
-      <c r="AW191" s="9"/>
+      <c r="AW191" s="9">
+        <v>1</v>
+      </c>
       <c r="AX191" s="11"/>
       <c r="AY191" s="9"/>
-      <c r="AZ191" s="9"/>
+      <c r="AZ191" s="9">
+        <v>1</v>
+      </c>
       <c r="BA191" s="11"/>
       <c r="BB191" s="9"/>
-      <c r="BC191" s="9"/>
+      <c r="BC191" s="9">
+        <v>1</v>
+      </c>
       <c r="BD191" s="11"/>
       <c r="BE191" s="9"/>
-      <c r="BF191" s="9"/>
+      <c r="BF191" s="9">
+        <v>1</v>
+      </c>
       <c r="BG191" s="11"/>
       <c r="BH191" s="9"/>
-      <c r="BI191" s="9"/>
+      <c r="BI191" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ191" s="11"/>
       <c r="BK191" s="9"/>
       <c r="BL191" s="9"/>
@@ -22141,19 +22907,21 @@
       <c r="BQ191" s="9"/>
     </row>
     <row r="192" spans="1:69" ht="16.5" thickBot="1">
-      <c r="A192" s="3" t="s">
+      <c r="A192" s="24" t="s">
         <v>389</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="B192" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="C192" s="4"/>
-      <c r="D192" s="4" t="s">
+      <c r="C192" s="25" t="s">
+        <v>561</v>
+      </c>
+      <c r="D192" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="E192" s="4"/>
-      <c r="F192" s="4"/>
-      <c r="G192" s="4"/>
+      <c r="E192" s="25"/>
+      <c r="F192" s="25"/>
+      <c r="G192" s="25"/>
       <c r="I192" s="9"/>
       <c r="J192" s="9"/>
       <c r="K192" s="9"/>
@@ -22223,46 +22991,70 @@
       <c r="B193" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="C193" s="4"/>
+      <c r="C193" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D193" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E193" s="4"/>
-      <c r="F193" s="4"/>
-      <c r="G193" s="4"/>
+      <c r="E193" s="4">
+        <v>23</v>
+      </c>
+      <c r="F193" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="G193" s="4" t="s">
+        <v>552</v>
+      </c>
       <c r="I193" s="9"/>
       <c r="J193" s="9"/>
       <c r="K193" s="9"/>
       <c r="L193" s="9"/>
       <c r="M193" s="11"/>
       <c r="N193" s="9"/>
-      <c r="O193" s="9"/>
+      <c r="O193" s="9">
+        <v>1</v>
+      </c>
       <c r="P193" s="9"/>
       <c r="Q193" s="9"/>
       <c r="R193" s="9"/>
       <c r="S193" s="9"/>
       <c r="T193" s="11"/>
       <c r="U193" s="9"/>
-      <c r="V193" s="9"/>
+      <c r="V193" s="9">
+        <v>1</v>
+      </c>
       <c r="W193" s="9"/>
-      <c r="X193" s="9"/>
+      <c r="X193" s="9">
+        <v>1</v>
+      </c>
       <c r="Y193" s="11"/>
-      <c r="Z193" s="9"/>
+      <c r="Z193" s="9">
+        <v>1</v>
+      </c>
       <c r="AA193" s="9"/>
       <c r="AB193" s="9"/>
       <c r="AC193" s="9"/>
       <c r="AD193" s="9"/>
-      <c r="AE193" s="9"/>
+      <c r="AE193" s="9">
+        <v>1</v>
+      </c>
       <c r="AF193" s="11"/>
       <c r="AG193" s="9"/>
-      <c r="AH193" s="9"/>
+      <c r="AH193" s="9">
+        <v>1</v>
+      </c>
       <c r="AI193" s="11"/>
       <c r="AJ193" s="9"/>
       <c r="AK193" s="9"/>
-      <c r="AL193" s="9"/>
+      <c r="AL193" s="9">
+        <v>1</v>
+      </c>
       <c r="AM193" s="9"/>
       <c r="AN193" s="11"/>
-      <c r="AO193" s="9"/>
+      <c r="AO193" s="9">
+        <v>1</v>
+      </c>
       <c r="AP193" s="9"/>
       <c r="AQ193" s="9"/>
       <c r="AR193" s="11"/>
@@ -22270,21 +23062,33 @@
       <c r="AT193" s="9"/>
       <c r="AU193" s="9"/>
       <c r="AV193" s="9"/>
-      <c r="AW193" s="9"/>
+      <c r="AW193" s="9">
+        <v>1</v>
+      </c>
       <c r="AX193" s="11"/>
       <c r="AY193" s="9"/>
-      <c r="AZ193" s="9"/>
+      <c r="AZ193" s="9">
+        <v>1</v>
+      </c>
       <c r="BA193" s="11"/>
       <c r="BB193" s="9"/>
-      <c r="BC193" s="9"/>
+      <c r="BC193" s="9">
+        <v>1</v>
+      </c>
       <c r="BD193" s="11"/>
       <c r="BE193" s="9"/>
-      <c r="BF193" s="9"/>
+      <c r="BF193" s="9">
+        <v>1</v>
+      </c>
       <c r="BG193" s="11"/>
       <c r="BH193" s="9"/>
-      <c r="BI193" s="9"/>
+      <c r="BI193" s="9">
+        <v>1</v>
+      </c>
       <c r="BJ193" s="11"/>
-      <c r="BK193" s="9"/>
+      <c r="BK193" s="9">
+        <v>1</v>
+      </c>
       <c r="BL193" s="9"/>
       <c r="BM193" s="11"/>
       <c r="BN193" s="9"/>
@@ -22292,14 +23096,16 @@
       <c r="BP193" s="9"/>
       <c r="BQ193" s="9"/>
     </row>
-    <row r="194" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="194" spans="1:69" ht="16.5" thickBot="1">
       <c r="A194" s="3" t="s">
         <v>393</v>
       </c>
       <c r="B194" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C194" s="4"/>
+      <c r="C194" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D194" s="4" t="s">
         <v>395</v>
       </c>
@@ -22368,14 +23174,16 @@
       <c r="BP194" s="9"/>
       <c r="BQ194" s="9"/>
     </row>
-    <row r="195" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="195" spans="1:69" ht="16.5" thickBot="1">
       <c r="A195" s="3" t="s">
         <v>396</v>
       </c>
       <c r="B195" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="C195" s="4"/>
+      <c r="C195" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D195" s="4" t="s">
         <v>395</v>
       </c>
@@ -22444,14 +23252,16 @@
       <c r="BP195" s="9"/>
       <c r="BQ195" s="9"/>
     </row>
-    <row r="196" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="196" spans="1:69" ht="16.5" thickBot="1">
       <c r="A196" s="3" t="s">
         <v>398</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="C196" s="4"/>
+      <c r="C196" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D196" s="4" t="s">
         <v>395</v>
       </c>
@@ -22520,14 +23330,16 @@
       <c r="BP196" s="9"/>
       <c r="BQ196" s="9"/>
     </row>
-    <row r="197" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="197" spans="1:69" ht="16.5" thickBot="1">
       <c r="A197" s="3" t="s">
         <v>400</v>
       </c>
       <c r="B197" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="C197" s="4"/>
+      <c r="C197" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D197" s="4" t="s">
         <v>395</v>
       </c>
@@ -22596,14 +23408,16 @@
       <c r="BP197" s="9"/>
       <c r="BQ197" s="9"/>
     </row>
-    <row r="198" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="198" spans="1:69" ht="16.5" thickBot="1">
       <c r="A198" s="3" t="s">
         <v>402</v>
       </c>
       <c r="B198" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="C198" s="4"/>
+      <c r="C198" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D198" s="4" t="s">
         <v>395</v>
       </c>
@@ -22672,14 +23486,16 @@
       <c r="BP198" s="9"/>
       <c r="BQ198" s="9"/>
     </row>
-    <row r="199" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="199" spans="1:69" ht="16.5" thickBot="1">
       <c r="A199" s="3" t="s">
         <v>404</v>
       </c>
       <c r="B199" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="C199" s="4"/>
+      <c r="C199" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D199" s="4" t="s">
         <v>395</v>
       </c>
@@ -22748,14 +23564,16 @@
       <c r="BP199" s="9"/>
       <c r="BQ199" s="9"/>
     </row>
-    <row r="200" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="200" spans="1:69" ht="16.5" thickBot="1">
       <c r="A200" s="3" t="s">
         <v>406</v>
       </c>
       <c r="B200" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="C200" s="4"/>
+      <c r="C200" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D200" s="4" t="s">
         <v>395</v>
       </c>
@@ -22824,14 +23642,16 @@
       <c r="BP200" s="9"/>
       <c r="BQ200" s="9"/>
     </row>
-    <row r="201" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="201" spans="1:69" ht="16.5" thickBot="1">
       <c r="A201" s="3" t="s">
         <v>408</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="C201" s="4"/>
+      <c r="C201" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D201" s="4" t="s">
         <v>395</v>
       </c>
@@ -22900,14 +23720,16 @@
       <c r="BP201" s="9"/>
       <c r="BQ201" s="9"/>
     </row>
-    <row r="202" spans="1:69" ht="32.25" hidden="1" thickBot="1">
+    <row r="202" spans="1:69" ht="32.25" thickBot="1">
       <c r="A202" s="3" t="s">
         <v>410</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C202" s="4"/>
+      <c r="C202" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D202" s="4" t="s">
         <v>395</v>
       </c>
@@ -22976,14 +23798,16 @@
       <c r="BP202" s="9"/>
       <c r="BQ202" s="9"/>
     </row>
-    <row r="203" spans="1:69" ht="17.25" hidden="1" thickBot="1">
+    <row r="203" spans="1:69" ht="17.25" thickBot="1">
       <c r="A203" s="3" t="s">
         <v>412</v>
       </c>
       <c r="B203" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="C203" s="4"/>
+      <c r="C203" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D203" s="4" t="s">
         <v>395</v>
       </c>
@@ -23052,14 +23876,16 @@
       <c r="BP203" s="9"/>
       <c r="BQ203" s="9"/>
     </row>
-    <row r="204" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="204" spans="1:69" ht="16.5" thickBot="1">
       <c r="A204" s="3" t="s">
         <v>414</v>
       </c>
       <c r="B204" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="C204" s="4"/>
+      <c r="C204" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D204" s="4" t="s">
         <v>395</v>
       </c>
@@ -23128,14 +23954,16 @@
       <c r="BP204" s="9"/>
       <c r="BQ204" s="9"/>
     </row>
-    <row r="205" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="205" spans="1:69" ht="16.5" thickBot="1">
       <c r="A205" s="3" t="s">
         <v>416</v>
       </c>
       <c r="B205" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C205" s="4"/>
+      <c r="C205" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D205" s="4" t="s">
         <v>395</v>
       </c>
@@ -23204,14 +24032,16 @@
       <c r="BP205" s="9"/>
       <c r="BQ205" s="9"/>
     </row>
-    <row r="206" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="206" spans="1:69" ht="16.5" thickBot="1">
       <c r="A206" s="3" t="s">
         <v>418</v>
       </c>
       <c r="B206" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="C206" s="4"/>
+      <c r="C206" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D206" s="4" t="s">
         <v>395</v>
       </c>
@@ -23280,14 +24110,16 @@
       <c r="BP206" s="9"/>
       <c r="BQ206" s="9"/>
     </row>
-    <row r="207" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="207" spans="1:69" ht="16.5" thickBot="1">
       <c r="A207" s="3" t="s">
         <v>420</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="C207" s="4"/>
+      <c r="C207" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D207" s="4" t="s">
         <v>395</v>
       </c>
@@ -23356,14 +24188,16 @@
       <c r="BP207" s="9"/>
       <c r="BQ207" s="9"/>
     </row>
-    <row r="208" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="208" spans="1:69" ht="16.5" thickBot="1">
       <c r="A208" s="3" t="s">
         <v>422</v>
       </c>
       <c r="B208" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="C208" s="4"/>
+      <c r="C208" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D208" s="4" t="s">
         <v>395</v>
       </c>
@@ -23432,14 +24266,16 @@
       <c r="BP208" s="9"/>
       <c r="BQ208" s="9"/>
     </row>
-    <row r="209" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="209" spans="1:69" ht="16.5" thickBot="1">
       <c r="A209" s="3" t="s">
         <v>424</v>
       </c>
       <c r="B209" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="C209" s="4"/>
+      <c r="C209" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D209" s="4" t="s">
         <v>395</v>
       </c>
@@ -23508,14 +24344,16 @@
       <c r="BP209" s="9"/>
       <c r="BQ209" s="9"/>
     </row>
-    <row r="210" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="210" spans="1:69" ht="16.5" thickBot="1">
       <c r="A210" s="3" t="s">
         <v>426</v>
       </c>
       <c r="B210" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="C210" s="4"/>
+      <c r="C210" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D210" s="4" t="s">
         <v>395</v>
       </c>
@@ -23584,14 +24422,16 @@
       <c r="BP210" s="9"/>
       <c r="BQ210" s="9"/>
     </row>
-    <row r="211" spans="1:69" ht="32.25" hidden="1" thickBot="1">
+    <row r="211" spans="1:69" ht="32.25" thickBot="1">
       <c r="A211" s="3" t="s">
         <v>428</v>
       </c>
       <c r="B211" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="C211" s="4"/>
+      <c r="C211" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D211" s="4" t="s">
         <v>395</v>
       </c>
@@ -23660,14 +24500,16 @@
       <c r="BP211" s="9"/>
       <c r="BQ211" s="9"/>
     </row>
-    <row r="212" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="212" spans="1:69" ht="16.5" thickBot="1">
       <c r="A212" s="3" t="s">
         <v>430</v>
       </c>
       <c r="B212" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="C212" s="4"/>
+      <c r="C212" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D212" s="4" t="s">
         <v>395</v>
       </c>
@@ -23736,14 +24578,16 @@
       <c r="BP212" s="9"/>
       <c r="BQ212" s="9"/>
     </row>
-    <row r="213" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="213" spans="1:69" ht="16.5" thickBot="1">
       <c r="A213" s="3" t="s">
         <v>432</v>
       </c>
       <c r="B213" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="C213" s="4"/>
+      <c r="C213" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D213" s="4" t="s">
         <v>395</v>
       </c>
@@ -23812,14 +24656,16 @@
       <c r="BP213" s="9"/>
       <c r="BQ213" s="9"/>
     </row>
-    <row r="214" spans="1:69" ht="16.5" hidden="1" thickBot="1">
+    <row r="214" spans="1:69" ht="16.5" thickBot="1">
       <c r="A214" s="3" t="s">
         <v>434</v>
       </c>
       <c r="B214" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="C214" s="4"/>
+      <c r="C214" s="4" t="s">
+        <v>561</v>
+      </c>
       <c r="D214" s="4" t="s">
         <v>395</v>
       </c>
@@ -23888,7 +24734,8 @@
       <c r="BP214" s="9"/>
       <c r="BQ214" s="9"/>
     </row>
-    <row r="215" spans="1:69" ht="202.5">
+    <row r="215" spans="1:69" ht="200.25">
+      <c r="D215" s="27"/>
       <c r="I215" s="6" t="s">
         <v>483</v>
       </c>
@@ -24053,27 +24900,27 @@
       </c>
       <c r="I216">
         <f>SUM(I3:I214)</f>
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J216">
         <f t="shared" ref="J216:BQ216" si="0">SUM(J3:J214)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K216">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L216">
         <f>SUM(L3:L214)</f>
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="N216">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="O216">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="P216">
         <f t="shared" si="0"/>
@@ -24089,59 +24936,59 @@
       </c>
       <c r="S216">
         <f>SUM(S3:S214)</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="U216">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="V216">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="W216">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="X216">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="Z216">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="AA216">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="AB216">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AC216">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AD216">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="AE216">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AG216">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AH216">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="AJ216">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="AK216">
         <f t="shared" si="0"/>
@@ -24149,15 +24996,15 @@
       </c>
       <c r="AL216">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AM216">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AO216">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="AP216">
         <f t="shared" si="0"/>
@@ -24165,7 +25012,7 @@
       </c>
       <c r="AQ216">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AR216" s="12">
         <f t="shared" si="0"/>
@@ -24173,7 +25020,7 @@
       </c>
       <c r="AS216">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AT216">
         <f t="shared" si="0"/>
@@ -24181,7 +25028,7 @@
       </c>
       <c r="AU216">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AV216">
         <f t="shared" si="0"/>
@@ -24189,19 +25036,23 @@
       </c>
       <c r="AW216">
         <f>SUM(AW3:AW214)</f>
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="AY216">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AZ216">
         <f>SUM(AZ3:AZ214)</f>
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="BB216">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>51</v>
+      </c>
+      <c r="BC216">
+        <f t="shared" si="0"/>
+        <v>82</v>
       </c>
       <c r="BD216" s="12">
         <f t="shared" si="0"/>
@@ -24209,26 +25060,26 @@
       </c>
       <c r="BE216">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="BF216">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="BG216" s="12" t="s">
         <v>480</v>
       </c>
       <c r="BH216">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="BI216">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="BK216">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="BL216">
         <f t="shared" si="0"/>
@@ -24236,7 +25087,7 @@
       </c>
       <c r="BN216">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BO216">
         <f t="shared" si="0"/>

</xml_diff>